<commit_message>
fixed date mismatch for plot, verified test 3
</commit_message>
<xml_diff>
--- a/Data/fake_nocalib.xlsx
+++ b/Data/fake_nocalib.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:SF4"/>
+  <dimension ref="A1:SG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1933,6 +1933,9 @@
       <c r="SF1" s="2" t="n">
         <v>2521</v>
       </c>
+      <c r="SG1" s="2" t="n">
+        <v>2522</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -1941,67 +1944,67 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.34</v>
+        <v>0.3400000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4191338609297701</v>
+        <v>0.4204531193381447</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5583096414636474</v>
+        <v>0.5629962637107235</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6075738260184688</v>
+        <v>0.7181255052401537</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5690193021793856</v>
+        <v>0.7353792558244767</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6067106011253892</v>
+        <v>0.6634561158807928</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2165607880480358</v>
+        <v>0.6785936953210321</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4167827895044908</v>
+        <v>0.244192668384428</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7277496845214747</v>
+        <v>0.454617067444382</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9460959484845357</v>
+        <v>0.720027980070397</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9999280391624003</v>
+        <v>0.9721146405848189</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9999955885782713</v>
+        <v>0.9984818907044347</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9999978859458895</v>
+        <v>0.9997485057136849</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9999999989567695</v>
+        <v>0.9999407806356677</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9999999999750734</v>
+        <v>0.9999992180687854</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.999999999998692</v>
+        <v>0.9999999354073765</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9999999999997918</v>
+        <v>0.9999999952658166</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9999999999999933</v>
+        <v>0.9999999995918449</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999921714</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>0.9999999999999588</v>
       </c>
       <c r="V2" t="n">
-        <v>1</v>
+        <v>0.9999999999999978</v>
       </c>
       <c r="W2" t="n">
         <v>1</v>
@@ -3435,6 +3438,9 @@
         <v>1</v>
       </c>
       <c r="SF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="SG2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3448,406 +3454,406 @@
         <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3234857030618779</v>
+        <v>0.3231932765123403</v>
       </c>
       <c r="D3" t="n">
-        <v>0.288299579686091</v>
+        <v>0.2862255244832053</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2803722436314497</v>
+        <v>0.2151322014019616</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3485631116229937</v>
+        <v>0.2303956107036899</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3646793575703084</v>
+        <v>0.314840728894836</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7329340126820582</v>
+        <v>0.3138150297263795</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5804020504524197</v>
+        <v>0.7417530179368523</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2721616033383013</v>
+        <v>0.5445840352473456</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05390112320007086</v>
+        <v>0.2799000403588172</v>
       </c>
       <c r="L3" t="n">
-        <v>7.196078596052048e-05</v>
+        <v>0.0278852300564981</v>
       </c>
       <c r="M3" t="n">
-        <v>4.411420983598544e-06</v>
+        <v>0.00151810744441949</v>
       </c>
       <c r="N3" t="n">
-        <v>2.114054005972167e-06</v>
+        <v>0.0002514941984627928</v>
       </c>
       <c r="O3" t="n">
-        <v>1.04323049911104e-09</v>
+        <v>5.921936358610329e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>2.492668347337439e-11</v>
+        <v>7.819312119487251e-07</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.308062193634111e-12</v>
+        <v>6.459262348630573e-08</v>
       </c>
       <c r="R3" t="n">
-        <v>2.082702511900697e-13</v>
+        <v>4.734183328161191e-09</v>
       </c>
       <c r="S3" t="n">
-        <v>6.651342602489323e-15</v>
+        <v>4.081550887759506e-10</v>
       </c>
       <c r="T3" t="n">
-        <v>9.114575554034432e-17</v>
+        <v>7.82862613173115e-12</v>
       </c>
       <c r="U3" t="n">
-        <v>1.481340228913605e-18</v>
+        <v>4.123440139089813e-14</v>
       </c>
       <c r="V3" t="n">
-        <v>4.069254003906313e-20</v>
+        <v>2.208922167862435e-15</v>
       </c>
       <c r="W3" t="n">
-        <v>4.572467076391615e-23</v>
+        <v>1.282976316709989e-17</v>
       </c>
       <c r="X3" t="n">
-        <v>3.040302373072632e-24</v>
+        <v>1.368673611229222e-19</v>
       </c>
       <c r="Y3" t="n">
-        <v>5.784687452324598e-27</v>
+        <v>2.537509886178239e-21</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.264047686737349e-28</v>
+        <v>8.209096527001162e-23</v>
       </c>
       <c r="AA3" t="n">
-        <v>5.751171783533423e-31</v>
+        <v>8.645180296812349e-25</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.773105531217298e-32</v>
+        <v>3.735173437339378e-26</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.919004159020582e-33</v>
+        <v>2.733229669308026e-28</v>
       </c>
       <c r="AD3" t="n">
-        <v>8.575658962042758e-38</v>
+        <v>3.293333334420333e-30</v>
       </c>
       <c r="AE3" t="n">
-        <v>3.282294285377687e-40</v>
+        <v>8.172600918564627e-33</v>
       </c>
       <c r="AF3" t="n">
-        <v>5.199586038388624e-42</v>
+        <v>1.78361040953903e-34</v>
       </c>
       <c r="AG3" t="n">
-        <v>4.781532972286441e-44</v>
+        <v>8.806497684535654e-37</v>
       </c>
       <c r="AH3" t="n">
-        <v>5.506672334959914e-47</v>
+        <v>3.528733669652618e-39</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.106822682033676e-48</v>
+        <v>3.551414897126198e-41</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.114448871497159e-51</v>
+        <v>1.845539572553126e-43</v>
       </c>
       <c r="AK3" t="n">
-        <v>8.996237137759929e-53</v>
+        <v>2.650369239295483e-45</v>
       </c>
       <c r="AL3" t="n">
-        <v>2.038338781323308e-54</v>
+        <v>1.568473467610158e-46</v>
       </c>
       <c r="AM3" t="n">
-        <v>6.538081574269666e-57</v>
+        <v>4.322348666271413e-48</v>
       </c>
       <c r="AN3" t="n">
-        <v>4.102538179529724e-59</v>
+        <v>1.998146904888979e-50</v>
       </c>
       <c r="AO3" t="n">
-        <v>8.526564246499187e-62</v>
+        <v>1.001084982287456e-52</v>
       </c>
       <c r="AP3" t="n">
-        <v>1.088944771442766e-63</v>
+        <v>8.967916306300224e-55</v>
       </c>
       <c r="AQ3" t="n">
-        <v>2.421709779127509e-67</v>
+        <v>8.35991108793775e-58</v>
       </c>
       <c r="AR3" t="n">
-        <v>3.99749755211013e-70</v>
+        <v>1.323688413880276e-60</v>
       </c>
       <c r="AS3" t="n">
-        <v>4.035023766253999e-72</v>
+        <v>6.94524699348581e-63</v>
       </c>
       <c r="AT3" t="n">
-        <v>3.289620342221218e-73</v>
+        <v>6.485154789932017e-65</v>
       </c>
       <c r="AU3" t="n">
-        <v>4.240685460583728e-76</v>
+        <v>1.132523146676326e-66</v>
       </c>
       <c r="AV3" t="n">
-        <v>6.656228495286984e-79</v>
+        <v>4.135364124334432e-69</v>
       </c>
       <c r="AW3" t="n">
-        <v>3.060224854363575e-79</v>
+        <v>1.888953572971093e-71</v>
       </c>
       <c r="AX3" t="n">
-        <v>9.623894251470976e-83</v>
+        <v>3.155002739253613e-72</v>
       </c>
       <c r="AY3" t="n">
-        <v>1.764535093347632e-84</v>
+        <v>2.15594899571307e-74</v>
       </c>
       <c r="AZ3" t="n">
-        <v>6.926835365805598e-88</v>
+        <v>7.200430506691081e-77</v>
       </c>
       <c r="BA3" t="n">
-        <v>6.449401993761933e-90</v>
+        <v>4.355544394930296e-79</v>
       </c>
       <c r="BB3" t="n">
-        <v>3.445482512948137e-92</v>
+        <v>1.231977946848314e-81</v>
       </c>
       <c r="BC3" t="n">
-        <v>2.270697869347225e-95</v>
+        <v>5.733656429185987e-84</v>
       </c>
       <c r="BD3" t="n">
-        <v>1.725949465794997e-97</v>
+        <v>2.300102378911595e-86</v>
       </c>
       <c r="BE3" t="n">
-        <v>1.689023167538591e-100</v>
+        <v>7.285723422891193e-89</v>
       </c>
       <c r="BF3" t="n">
-        <v>1.228980764607718e-102</v>
+        <v>6.941279378485098e-92</v>
       </c>
       <c r="BG3" t="n">
-        <v>1.771997520949944e-104</v>
+        <v>1.083419960604083e-93</v>
       </c>
       <c r="BH3" t="n">
-        <v>2.051379880551536e-107</v>
+        <v>1.436142765577422e-95</v>
       </c>
       <c r="BI3" t="n">
-        <v>6.892031351389175e-110</v>
+        <v>3.486778000871525e-98</v>
       </c>
       <c r="BJ3" t="n">
-        <v>3.848033896510568e-112</v>
+        <v>1.429008791055144e-100</v>
       </c>
       <c r="BK3" t="n">
-        <v>9.959347035988782e-116</v>
+        <v>2.360220845450451e-103</v>
       </c>
       <c r="BL3" t="n">
-        <v>3.820778863252351e-118</v>
+        <v>9.929566525307267e-106</v>
       </c>
       <c r="BM3" t="n">
-        <v>3.527909187648578e-120</v>
+        <v>2.065100316914139e-108</v>
       </c>
       <c r="BN3" t="n">
-        <v>1.896463127363947e-122</v>
+        <v>2.164521746161432e-110</v>
       </c>
       <c r="BO3" t="n">
-        <v>4.328144627282255e-125</v>
+        <v>3.754279788713721e-113</v>
       </c>
       <c r="BP3" t="n">
-        <v>1.015393990986166e-128</v>
+        <v>2.062936492925158e-116</v>
       </c>
       <c r="BQ3" t="n">
-        <v>2.950568166403277e-131</v>
+        <v>5.701455711544083e-119</v>
       </c>
       <c r="BR3" t="n">
-        <v>2.049203460066984e-133</v>
+        <v>2.966293183778675e-121</v>
       </c>
       <c r="BS3" t="n">
-        <v>4.302941553204693e-136</v>
+        <v>9.545462129556182e-124</v>
       </c>
       <c r="BT3" t="n">
-        <v>2.313167626414338e-138</v>
+        <v>3.460507018349236e-126</v>
       </c>
       <c r="BU3" t="n">
-        <v>6.909476480860414e-141</v>
+        <v>1.633430866533558e-128</v>
       </c>
       <c r="BV3" t="n">
-        <v>1.516475489364675e-143</v>
+        <v>3.648468406062058e-131</v>
       </c>
       <c r="BW3" t="n">
-        <v>9.409170228132339e-146</v>
+        <v>9.736710488133254e-134</v>
       </c>
       <c r="BX3" t="n">
-        <v>6.423843551427064e-149</v>
+        <v>1.697406253819052e-136</v>
       </c>
       <c r="BY3" t="n">
-        <v>8.782315625315234e-152</v>
+        <v>2.017868414854885e-139</v>
       </c>
       <c r="BZ3" t="n">
-        <v>3.149715168426196e-154</v>
+        <v>1.109838387622664e-141</v>
       </c>
       <c r="CA3" t="n">
-        <v>8.429613061641768e-157</v>
+        <v>9.83941222376737e-145</v>
       </c>
       <c r="CB3" t="n">
-        <v>7.896810222126366e-160</v>
+        <v>2.545052624705583e-147</v>
       </c>
       <c r="CC3" t="n">
-        <v>1.46679257177332e-162</v>
+        <v>3.789465879669885e-150</v>
       </c>
       <c r="CD3" t="n">
-        <v>9.958186530563662e-166</v>
+        <v>5.400217330243092e-153</v>
       </c>
       <c r="CE3" t="n">
-        <v>1.291414272148889e-168</v>
+        <v>1.020728191081044e-155</v>
       </c>
       <c r="CF3" t="n">
-        <v>6.925479061486237e-172</v>
+        <v>6.119703929619499e-159</v>
       </c>
       <c r="CG3" t="n">
-        <v>9.984643484709576e-175</v>
+        <v>9.290061487525068e-162</v>
       </c>
       <c r="CH3" t="n">
-        <v>3.407479320888232e-177</v>
+        <v>1.389278573541469e-164</v>
       </c>
       <c r="CI3" t="n">
-        <v>4.001678153682664e-180</v>
+        <v>3.018426688383909e-167</v>
       </c>
       <c r="CJ3" t="n">
-        <v>2.167387946851962e-182</v>
+        <v>1.544902461056762e-169</v>
       </c>
       <c r="CK3" t="n">
-        <v>2.426137163341782e-185</v>
+        <v>1.649573484296101e-172</v>
       </c>
       <c r="CL3" t="n">
-        <v>3.446113708678388e-188</v>
+        <v>1.239428902511692e-175</v>
       </c>
       <c r="CM3" t="n">
-        <v>1.203868782925009e-190</v>
+        <v>7.282688237073656e-178</v>
       </c>
       <c r="CN3" t="n">
-        <v>6.013532507205709e-193</v>
+        <v>1.233216867888955e-180</v>
       </c>
       <c r="CO3" t="n">
-        <v>4.81066479505085e-196</v>
+        <v>4.226822397837822e-183</v>
       </c>
       <c r="CP3" t="n">
-        <v>4.955113583294613e-198</v>
+        <v>1.158467395524725e-185</v>
       </c>
       <c r="CQ3" t="n">
-        <v>3.888582385705325e-201</v>
+        <v>8.111634033141904e-188</v>
       </c>
       <c r="CR3" t="n">
-        <v>1.056708804837002e-203</v>
+        <v>1.082752384146899e-190</v>
       </c>
       <c r="CS3" t="n">
-        <v>2.925188306728098e-206</v>
+        <v>3.04002607063479e-193</v>
       </c>
       <c r="CT3" t="n">
-        <v>2.264652184476244e-209</v>
+        <v>3.35179886341235e-196</v>
       </c>
       <c r="CU3" t="n">
-        <v>1.947253762467009e-212</v>
+        <v>2.861814717674259e-199</v>
       </c>
       <c r="CV3" t="n">
-        <v>8.79078154799603e-216</v>
+        <v>2.618498316119997e-202</v>
       </c>
       <c r="CW3" t="n">
-        <v>1.93297402524706e-218</v>
+        <v>5.756701258431772e-205</v>
       </c>
       <c r="CX3" t="n">
-        <v>8.37560088110331e-221</v>
+        <v>8.161322331772085e-208</v>
       </c>
       <c r="CY3" t="n">
-        <v>1.563889412666692e-223</v>
+        <v>2.69994902355047e-210</v>
       </c>
       <c r="CZ3" t="n">
-        <v>1.843074198370208e-226</v>
+        <v>3.977747956546883e-213</v>
       </c>
       <c r="DA3" t="n">
-        <v>1.20883684771995e-229</v>
+        <v>2.646361419343663e-216</v>
       </c>
       <c r="DB3" t="n">
-        <v>1.080605946471258e-232</v>
+        <v>2.154474899975639e-219</v>
       </c>
       <c r="DC3" t="n">
-        <v>4.335203640161579e-235</v>
+        <v>2.426296952624667e-222</v>
       </c>
       <c r="DD3" t="n">
-        <v>1.807272497214012e-236</v>
+        <v>8.671071930744764e-225</v>
       </c>
       <c r="DE3" t="n">
-        <v>1.510512892024061e-239</v>
+        <v>4.721761411161403e-226</v>
       </c>
       <c r="DF3" t="n">
-        <v>1.220750433426468e-242</v>
+        <v>6.234361033281678e-229</v>
       </c>
       <c r="DG3" t="n">
-        <v>1.184334668916831e-245</v>
+        <v>3.850082666254173e-232</v>
       </c>
       <c r="DH3" t="n">
-        <v>2.774742215357097e-248</v>
+        <v>6.085885084523206e-235</v>
       </c>
       <c r="DI3" t="n">
-        <v>2.629586098178897e-251</v>
+        <v>9.688910059125909e-238</v>
       </c>
       <c r="DJ3" t="n">
-        <v>2.907834819977946e-254</v>
+        <v>2.121238798306453e-240</v>
       </c>
       <c r="DK3" t="n">
-        <v>1.455259476826532e-257</v>
+        <v>1.223172945752218e-243</v>
       </c>
       <c r="DL3" t="n">
-        <v>4.889114804855755e-260</v>
+        <v>3.186345018273024e-246</v>
       </c>
       <c r="DM3" t="n">
-        <v>6.045134277724531e-263</v>
+        <v>2.986411475610899e-249</v>
       </c>
       <c r="DN3" t="n">
-        <v>2.981391265807844e-266</v>
+        <v>6.397579923031843e-252</v>
       </c>
       <c r="DO3" t="n">
-        <v>2.357874101890774e-269</v>
+        <v>4.594486726873716e-255</v>
       </c>
       <c r="DP3" t="n">
-        <v>1.296580024409511e-272</v>
+        <v>3.08900599329973e-258</v>
       </c>
       <c r="DQ3" t="n">
-        <v>1.890306226988819e-275</v>
+        <v>2.182917711259896e-261</v>
       </c>
       <c r="DR3" t="n">
-        <v>3.249783805796397e-278</v>
+        <v>3.4977614158307e-264</v>
       </c>
       <c r="DS3" t="n">
-        <v>5.312629226643776e-281</v>
+        <v>9.472673393156493e-267</v>
       </c>
       <c r="DT3" t="n">
-        <v>3.822648077554142e-284</v>
+        <v>8.369157153832356e-270</v>
       </c>
       <c r="DU3" t="n">
-        <v>1.948770548110138e-287</v>
+        <v>5.419134085796373e-273</v>
       </c>
       <c r="DV3" t="n">
-        <v>2.289688688565028e-290</v>
+        <v>5.723154436853306e-276</v>
       </c>
       <c r="DW3" t="n">
-        <v>6.265432392356884e-293</v>
+        <v>1.218052859427839e-278</v>
       </c>
       <c r="DX3" t="n">
-        <v>1.184402853694744e-295</v>
+        <v>9.984567541440087e-282</v>
       </c>
       <c r="DY3" t="n">
-        <v>3.047732755217711e-299</v>
+        <v>9.773571585562611e-285</v>
       </c>
       <c r="DZ3" t="n">
-        <v>2.886823452113357e-302</v>
+        <v>7.007896300844706e-288</v>
       </c>
       <c r="EA3" t="n">
-        <v>5.962705892664113e-305</v>
+        <v>4.89641512129886e-291</v>
       </c>
       <c r="EB3" t="n">
-        <v>0</v>
+        <v>1.927869326669561e-293</v>
       </c>
       <c r="EC3" t="n">
-        <v>0</v>
+        <v>2.119235103382775e-296</v>
       </c>
       <c r="ED3" t="n">
-        <v>0</v>
+        <v>8.310466174206517e-299</v>
       </c>
       <c r="EE3" t="n">
-        <v>0</v>
+        <v>7.283824512438452e-302</v>
       </c>
       <c r="EF3" t="n">
-        <v>0</v>
+        <v>4.137317069518141e-305</v>
       </c>
       <c r="EG3" t="n">
         <v>0</v>
@@ -4939,6 +4945,9 @@
         <v>0</v>
       </c>
       <c r="SF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="SG3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4952,355 +4961,355 @@
         <v>0.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.257380436008352</v>
+        <v>0.256353604149515</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1533907788502616</v>
+        <v>0.1507782118060711</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1120539303500815</v>
+        <v>0.06674229335788452</v>
       </c>
       <c r="F4" t="n">
-        <v>0.08241758619762067</v>
+        <v>0.03422513347183336</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0286100413043022</v>
+        <v>0.02170315522437116</v>
       </c>
       <c r="H4" t="n">
-        <v>0.05050519926990599</v>
+        <v>0.007591274952588354</v>
       </c>
       <c r="I4" t="n">
-        <v>0.002815160043089418</v>
+        <v>0.01405431367871977</v>
       </c>
       <c r="J4" t="n">
-        <v>8.871214022408411e-05</v>
+        <v>0.0007988973082724498</v>
       </c>
       <c r="K4" t="n">
-        <v>2.928315393474193e-06</v>
+        <v>7.197957078569808e-05</v>
       </c>
       <c r="L4" t="n">
-        <v>5.163920156145053e-11</v>
+        <v>1.293586830273262e-07</v>
       </c>
       <c r="M4" t="n">
-        <v>7.450184611619742e-13</v>
+        <v>1.851145820024733e-09</v>
       </c>
       <c r="N4" t="n">
-        <v>1.045844258248846e-13</v>
+        <v>8.785225634490864e-11</v>
       </c>
       <c r="O4" t="n">
-        <v>5.780087600346684e-18</v>
+        <v>7.462552365327504e-13</v>
       </c>
       <c r="P4" t="n">
-        <v>2.587922458215427e-20</v>
+        <v>2.552966996833278e-15</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.886103721138013e-22</v>
+        <v>4.53565169696821e-17</v>
       </c>
       <c r="R4" t="n">
-        <v>1.336089337701366e-23</v>
+        <v>8.991790933644894e-19</v>
       </c>
       <c r="S4" t="n">
-        <v>9.110605811051798e-26</v>
+        <v>1.267831093961639e-20</v>
       </c>
       <c r="T4" t="n">
-        <v>3.085612646268759e-28</v>
+        <v>5.074810462491077e-23</v>
       </c>
       <c r="U4" t="n">
-        <v>8.733501072733999e-31</v>
+        <v>7.465837289856729e-26</v>
       </c>
       <c r="V4" t="n">
-        <v>4.943442603094118e-33</v>
+        <v>6.842204988639893e-28</v>
       </c>
       <c r="W4" t="n">
-        <v>3.664269943407732e-36</v>
+        <v>1.003861747773716e-30</v>
       </c>
       <c r="X4" t="n">
-        <v>3.842218911395243e-38</v>
+        <v>3.274118933796584e-33</v>
       </c>
       <c r="Y4" t="n">
-        <v>2.903684069933693e-41</v>
+        <v>9.958024035456358e-36</v>
       </c>
       <c r="Z4" t="n">
-        <v>1.443947326348998e-43</v>
+        <v>6.384661027688728e-38</v>
       </c>
       <c r="AA4" t="n">
-        <v>3.247516777751882e-46</v>
+        <v>1.68222640900028e-40</v>
       </c>
       <c r="AB4" t="n">
-        <v>3.713583442990786e-48</v>
+        <v>1.861505245999103e-42</v>
       </c>
       <c r="AC4" t="n">
-        <v>4.076403799956477e-50</v>
+        <v>4.223535094532186e-45</v>
       </c>
       <c r="AD4" t="n">
-        <v>8.174458301167994e-54</v>
+        <v>1.162172777263558e-47</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.178863022117241e-56</v>
+        <v>1.581619011069234e-50</v>
       </c>
       <c r="AF4" t="n">
-        <v>6.737370529717939e-59</v>
+        <v>7.940247489624705e-53</v>
       </c>
       <c r="AG4" t="n">
-        <v>1.641190914867157e-61</v>
+        <v>2.045492919934869e-55</v>
       </c>
       <c r="AH4" t="n">
-        <v>1.676185603223421e-64</v>
+        <v>2.848384345847496e-58</v>
       </c>
       <c r="AI4" t="n">
-        <v>7.336435419556468e-67</v>
+        <v>9.417155315531184e-61</v>
       </c>
       <c r="AJ4" t="n">
-        <v>1.371274493221073e-69</v>
+        <v>1.55026341011521e-63</v>
       </c>
       <c r="AK4" t="n">
-        <v>1.925469773047183e-71</v>
+        <v>9.087953013607001e-66</v>
       </c>
       <c r="AL4" t="n">
-        <v>9.105540324607929e-74</v>
+        <v>9.593843638430837e-68</v>
       </c>
       <c r="AM4" t="n">
-        <v>1.183913682815772e-76</v>
+        <v>5.40276613173805e-70</v>
       </c>
       <c r="AN4" t="n">
-        <v>2.178566128404293e-79</v>
+        <v>8.457403605425062e-73</v>
       </c>
       <c r="AO4" t="n">
-        <v>2.488307346212303e-82</v>
+        <v>1.342498596565131e-75</v>
       </c>
       <c r="AP4" t="n">
-        <v>7.772603067444147e-85</v>
+        <v>3.584252498921526e-78</v>
       </c>
       <c r="AQ4" t="n">
-        <v>3.37806781793934e-88</v>
+        <v>2.436286471404693e-81</v>
       </c>
       <c r="AR4" t="n">
-        <v>3.20967296110021e-91</v>
+        <v>2.361220514559712e-84</v>
       </c>
       <c r="AS4" t="n">
-        <v>8.138420504487484e-94</v>
+        <v>4.165235010048621e-87</v>
       </c>
       <c r="AT4" t="n">
-        <v>1.217252972741222e-95</v>
+        <v>1.002221547314689e-89</v>
       </c>
       <c r="AU4" t="n">
-        <v>1.046601108860346e-98</v>
+        <v>5.32568790451684e-92</v>
       </c>
       <c r="AV4" t="n">
-        <v>8.843052887219143e-102</v>
+        <v>7.816831861167795e-95</v>
       </c>
       <c r="AW4" t="n">
-        <v>6.819686804061328e-103</v>
+        <v>1.169698260549334e-97</v>
       </c>
       <c r="AX4" t="n">
-        <v>3.053042442922998e-106</v>
+        <v>3.996138233777963e-99</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.233173745737082e-108</v>
+        <v>8.35106108202985e-102</v>
       </c>
       <c r="AZ4" t="n">
-        <v>6.390880675791291e-112</v>
+        <v>1.211285242342639e-104</v>
       </c>
       <c r="BA4" t="n">
-        <v>1.528607768399657e-114</v>
+        <v>2.417356518814763e-107</v>
       </c>
       <c r="BB4" t="n">
-        <v>2.674699033269893e-117</v>
+        <v>2.657657370461082e-110</v>
       </c>
       <c r="BC4" t="n">
-        <v>2.027772663856374e-120</v>
+        <v>4.585232555345257e-113</v>
       </c>
       <c r="BD4" t="n">
-        <v>4.132582093854624e-123</v>
+        <v>7.752857121028684e-116</v>
       </c>
       <c r="BE4" t="n">
-        <v>3.10771222041119e-126</v>
+        <v>9.46706459057224e-119</v>
       </c>
       <c r="BF4" t="n">
-        <v>7.300144744514906e-129</v>
+        <v>6.487153800606464e-122</v>
       </c>
       <c r="BG4" t="n">
-        <v>2.762748771546907e-131</v>
+        <v>2.627835884149546e-124</v>
       </c>
       <c r="BH4" t="n">
-        <v>3.304897192870537e-134</v>
+        <v>1.021936556736778e-126</v>
       </c>
       <c r="BI4" t="n">
-        <v>3.817889033892446e-137</v>
+        <v>1.528360940476105e-129</v>
       </c>
       <c r="BJ4" t="n">
-        <v>6.436531499554002e-140</v>
+        <v>2.028640123671117e-132</v>
       </c>
       <c r="BK4" t="n">
-        <v>3.513033781057269e-143</v>
+        <v>1.944508376844312e-135</v>
       </c>
       <c r="BL4" t="n">
-        <v>5.418267242384247e-146</v>
+        <v>3.54621353024024e-138</v>
       </c>
       <c r="BM4" t="n">
-        <v>4.263389992166138e-148</v>
+        <v>3.577737192292854e-141</v>
       </c>
       <c r="BN4" t="n">
-        <v>7.451817285206974e-151</v>
+        <v>1.785768207231026e-143</v>
       </c>
       <c r="BO4" t="n">
-        <v>6.58051246655233e-154</v>
+        <v>1.451834427262673e-146</v>
       </c>
       <c r="BP4" t="n">
-        <v>2.575763465030965e-157</v>
+        <v>7.179239155717839e-150</v>
       </c>
       <c r="BQ4" t="n">
-        <v>3.271300590867878e-160</v>
+        <v>8.040239235048001e-153</v>
       </c>
       <c r="BR4" t="n">
-        <v>6.182802363628907e-163</v>
+        <v>1.394180549853944e-155</v>
       </c>
       <c r="BS4" t="n">
-        <v>6.082052047012701e-166</v>
+        <v>1.51295539451959e-158</v>
       </c>
       <c r="BT4" t="n">
-        <v>9.385542632306946e-169</v>
+        <v>1.965612126583086e-161</v>
       </c>
       <c r="BU4" t="n">
-        <v>1.251104767658341e-171</v>
+        <v>2.773733604064349e-164</v>
       </c>
       <c r="BV4" t="n">
-        <v>1.265197141396324e-174</v>
+        <v>2.901199788305986e-167</v>
       </c>
       <c r="BW4" t="n">
-        <v>2.219641175303755e-177</v>
+        <v>3.092418832732052e-170</v>
       </c>
       <c r="BX4" t="n">
-        <v>1.093280741301559e-180</v>
+        <v>2.873291305673903e-173</v>
       </c>
       <c r="BY4" t="n">
-        <v>1.847304186478146e-183</v>
+        <v>1.789000208805206e-176</v>
       </c>
       <c r="BZ4" t="n">
-        <v>2.483829719992466e-186</v>
+        <v>4.50914064468463e-179</v>
       </c>
       <c r="CA4" t="n">
-        <v>2.664531863918213e-189</v>
+        <v>2.626422091865968e-182</v>
       </c>
       <c r="CB4" t="n">
-        <v>1.432952370970346e-192</v>
+        <v>2.981559357222825e-185</v>
       </c>
       <c r="CC4" t="n">
-        <v>1.138044521555616e-195</v>
+        <v>2.011964206699953e-188</v>
       </c>
       <c r="CD4" t="n">
-        <v>9.571594187885709e-199</v>
+        <v>1.506892153943804e-191</v>
       </c>
       <c r="CE4" t="n">
-        <v>5.812302961455871e-202</v>
+        <v>1.862690257122632e-194</v>
       </c>
       <c r="CF4" t="n">
-        <v>2.437987204254546e-205</v>
+        <v>8.084639132649444e-198</v>
       </c>
       <c r="CG4" t="n">
-        <v>1.562842481624089e-208</v>
+        <v>5.239379982384315e-201</v>
       </c>
       <c r="CH4" t="n">
-        <v>3.603072278917492e-211</v>
+        <v>3.348892900955869e-204</v>
       </c>
       <c r="CI4" t="n">
-        <v>2.462781008750336e-214</v>
+        <v>5.292158879840529e-207</v>
       </c>
       <c r="CJ4" t="n">
-        <v>3.945277233624979e-217</v>
+        <v>8.54736883973549e-210</v>
       </c>
       <c r="CK4" t="n">
-        <v>2.120360188324329e-220</v>
+        <v>4.50531694617805e-213</v>
       </c>
       <c r="CL4" t="n">
-        <v>3.946061870691089e-223</v>
+        <v>2.076990875527825e-216</v>
       </c>
       <c r="CM4" t="n">
-        <v>4.749623136614965e-226</v>
+        <v>5.390700144018678e-219</v>
       </c>
       <c r="CN4" t="n">
-        <v>7.325506983791312e-229</v>
+        <v>3.842966667280099e-222</v>
       </c>
       <c r="CO4" t="n">
-        <v>3.332740677462081e-232</v>
+        <v>5.203757634805211e-225</v>
       </c>
       <c r="CP4" t="n">
-        <v>9.084221959426779e-235</v>
+        <v>4.824135981945217e-228</v>
       </c>
       <c r="CQ4" t="n">
-        <v>4.519774275980414e-238</v>
+        <v>1.212371419303675e-230</v>
       </c>
       <c r="CR4" t="n">
-        <v>7.361190262887773e-241</v>
+        <v>7.439436366918048e-234</v>
       </c>
       <c r="CS4" t="n">
-        <v>6.816784418715309e-244</v>
+        <v>1.03260464226071e-236</v>
       </c>
       <c r="CT4" t="n">
-        <v>3.115162607352926e-247</v>
+        <v>6.073038811201116e-240</v>
       </c>
       <c r="CU4" t="n">
-        <v>1.548532795543576e-250</v>
+        <v>3.003909717191947e-243</v>
       </c>
       <c r="CV4" t="n">
-        <v>6.078110356544677e-254</v>
+        <v>1.620913967207032e-246</v>
       </c>
       <c r="CW4" t="n">
-        <v>5.040049160054227e-257</v>
+        <v>1.348511731663008e-249</v>
       </c>
       <c r="CX4" t="n">
-        <v>1.312769605165485e-259</v>
+        <v>8.096856571938103e-253</v>
       </c>
       <c r="CY4" t="n">
-        <v>1.284078441206241e-262</v>
+        <v>1.57728688685453e-255</v>
       </c>
       <c r="CZ4" t="n">
-        <v>7.041343643232261e-266</v>
+        <v>1.234361760273162e-258</v>
       </c>
       <c r="DA4" t="n">
-        <v>3.001418150215576e-269</v>
+        <v>4.938588001378184e-262</v>
       </c>
       <c r="DB4" t="n">
-        <v>1.331100682122903e-272</v>
+        <v>2.191939935138384e-265</v>
       </c>
       <c r="DC4" t="n">
-        <v>1.9103275502714e-275</v>
+        <v>1.0959416957832e-268</v>
       </c>
       <c r="DD4" t="n">
-        <v>2.636056270627561e-277</v>
+        <v>1.614891576763922e-271</v>
       </c>
       <c r="DE4" t="n">
-        <v>1.202103301116029e-280</v>
+        <v>2.929986815596866e-273</v>
       </c>
       <c r="DF4" t="n">
-        <v>5.015925273512777e-284</v>
+        <v>1.704535370373279e-276</v>
       </c>
       <c r="DG4" t="n">
-        <v>4.541296840907018e-287</v>
+        <v>6.416723795986421e-280</v>
       </c>
       <c r="DH4" t="n">
-        <v>4.161559111554993e-290</v>
+        <v>6.650762384716971e-283</v>
       </c>
       <c r="DI4" t="n">
-        <v>2.218894670929109e-293</v>
+        <v>5.398769000528248e-286</v>
       </c>
       <c r="DJ4" t="n">
-        <v>1.079398431187477e-296</v>
+        <v>4.585208900849863e-289</v>
       </c>
       <c r="DK4" t="n">
-        <v>3.96672595745341e-300</v>
+        <v>1.844707500609777e-292</v>
       </c>
       <c r="DL4" t="n">
-        <v>4.17982350927754e-303</v>
+        <v>1.584245601333634e-295</v>
       </c>
       <c r="DM4" t="n">
-        <v>2.940158594367175e-306</v>
+        <v>8.93579638656233e-299</v>
       </c>
       <c r="DN4" t="n">
-        <v>0</v>
+        <v>9.030744194026781e-302</v>
       </c>
       <c r="DO4" t="n">
-        <v>0</v>
+        <v>3.512685138125671e-305</v>
       </c>
       <c r="DP4" t="n">
         <v>0</v>
@@ -6443,6 +6452,9 @@
         <v>0</v>
       </c>
       <c r="SF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="SG4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6457,7 +6469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:SF4"/>
+  <dimension ref="A1:SG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7963,6 +7975,9 @@
       <c r="SF1" s="2" t="n">
         <v>2521</v>
       </c>
+      <c r="SG1" s="2" t="n">
+        <v>2522</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -7971,418 +7986,418 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3400000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3737990010649987</v>
+        <v>0.3886646214012456</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4967069968957108</v>
+        <v>0.4463821290676815</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4003900367609493</v>
+        <v>0.6041578606263894</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6248943208091761</v>
+        <v>0.4570422934613618</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5416850500010489</v>
+        <v>0.6339304040938666</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5051374094731473</v>
+        <v>0.4642045728974047</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4485402500012159</v>
+        <v>0.396543269094435</v>
       </c>
       <c r="J2" t="n">
-        <v>0.05235529559516616</v>
+        <v>0.3263497035003734</v>
       </c>
       <c r="K2" t="n">
-        <v>0.02340093209856329</v>
+        <v>0.05891997771326453</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0273650432317778</v>
+        <v>0.02312882481876145</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0008831283251668485</v>
+        <v>0.0257677007766999</v>
       </c>
       <c r="N2" t="n">
-        <v>7.838304533879286e-05</v>
+        <v>0.002532480842624122</v>
       </c>
       <c r="O2" t="n">
-        <v>1.520263762580036e-05</v>
+        <v>0.0001972777381398554</v>
       </c>
       <c r="P2" t="n">
-        <v>1.119728918709498e-06</v>
+        <v>4.418538298721034e-05</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.826789801905538e-07</v>
+        <v>7.354355272591708e-07</v>
       </c>
       <c r="R2" t="n">
-        <v>1.169573124112852e-09</v>
+        <v>1.118240601225256e-07</v>
       </c>
       <c r="S2" t="n">
-        <v>1.686931778649659e-10</v>
+        <v>1.169104925246798e-08</v>
       </c>
       <c r="T2" t="n">
-        <v>6.394419611710038e-12</v>
+        <v>4.253747061385827e-10</v>
       </c>
       <c r="U2" t="n">
-        <v>1.516715113292629e-13</v>
+        <v>1.150307625037306e-11</v>
       </c>
       <c r="V2" t="n">
-        <v>1.020805052911603e-14</v>
+        <v>5.725574102911696e-13</v>
       </c>
       <c r="W2" t="n">
-        <v>2.418013164679917e-16</v>
+        <v>2.0232678523802e-14</v>
       </c>
       <c r="X2" t="n">
-        <v>1.293735701960954e-17</v>
+        <v>7.401100408715972e-16</v>
       </c>
       <c r="Y2" t="n">
-        <v>3.646108179712359e-20</v>
+        <v>3.78233310612607e-18</v>
       </c>
       <c r="Z2" t="n">
-        <v>9.083792223258793e-21</v>
+        <v>4.463684189815293e-20</v>
       </c>
       <c r="AA2" t="n">
-        <v>7.07780413621599e-23</v>
+        <v>2.241583043091277e-21</v>
       </c>
       <c r="AB2" t="n">
-        <v>5.16140401255943e-25</v>
+        <v>8.898517004461279e-23</v>
       </c>
       <c r="AC2" t="n">
-        <v>3.547283207544002e-27</v>
+        <v>1.338953186537166e-24</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.886730792672441e-28</v>
+        <v>1.317267140845874e-26</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.809573476807328e-30</v>
+        <v>4.700629922576633e-28</v>
       </c>
       <c r="AF2" t="n">
-        <v>4.266534068393013e-33</v>
+        <v>1.012193283041124e-30</v>
       </c>
       <c r="AG2" t="n">
-        <v>1.631725847752653e-35</v>
+        <v>8.130292969530914e-33</v>
       </c>
       <c r="AH2" t="n">
-        <v>1.700927815063104e-37</v>
+        <v>8.557245077338672e-35</v>
       </c>
       <c r="AI2" t="n">
-        <v>2.935025702710306e-39</v>
+        <v>1.577752925341245e-36</v>
       </c>
       <c r="AJ2" t="n">
-        <v>2.37063142158157e-41</v>
+        <v>1.330698542813266e-38</v>
       </c>
       <c r="AK2" t="n">
-        <v>4.644896744531083e-43</v>
+        <v>7.057451313511805e-41</v>
       </c>
       <c r="AL2" t="n">
-        <v>5.05787387703171e-46</v>
+        <v>4.617888590820748e-43</v>
       </c>
       <c r="AM2" t="n">
-        <v>2.726740615305811e-48</v>
+        <v>2.662311553348682e-45</v>
       </c>
       <c r="AN2" t="n">
-        <v>3.55525903755116e-48</v>
+        <v>9.223305036749229e-48</v>
       </c>
       <c r="AO2" t="n">
-        <v>6.370154473905442e-53</v>
+        <v>8.689408662193109e-49</v>
       </c>
       <c r="AP2" t="n">
-        <v>1.916953109102302e-53</v>
+        <v>3.82211594450631e-51</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.682377690668892e-56</v>
+        <v>7.984703984320029e-53</v>
       </c>
       <c r="AR2" t="n">
-        <v>9.560072258567347e-60</v>
+        <v>2.894139938511865e-55</v>
       </c>
       <c r="AS2" t="n">
-        <v>5.262860844737634e-62</v>
+        <v>1.827351416115799e-57</v>
       </c>
       <c r="AT2" t="n">
-        <v>5.599989160100215e-64</v>
+        <v>8.86189353464205e-60</v>
       </c>
       <c r="AU2" t="n">
-        <v>5.765235600469575e-65</v>
+        <v>1.673850209763674e-61</v>
       </c>
       <c r="AV2" t="n">
-        <v>4.472814114687165e-68</v>
+        <v>5.770052124380065e-63</v>
       </c>
       <c r="AW2" t="n">
-        <v>1.434150560030124e-69</v>
+        <v>3.05043931162489e-65</v>
       </c>
       <c r="AX2" t="n">
-        <v>8.695173080212812e-72</v>
+        <v>5.0226502392779e-67</v>
       </c>
       <c r="AY2" t="n">
-        <v>1.319690966633378e-74</v>
+        <v>3.181484793274098e-69</v>
       </c>
       <c r="AZ2" t="n">
-        <v>4.904843581416169e-77</v>
+        <v>1.18187676823107e-71</v>
       </c>
       <c r="BA2" t="n">
-        <v>9.661822289337311e-80</v>
+        <v>2.18267862766315e-74</v>
       </c>
       <c r="BB2" t="n">
-        <v>6.575603578804386e-81</v>
+        <v>8.70791576645501e-77</v>
       </c>
       <c r="BC2" t="n">
-        <v>7.593294516426209e-85</v>
+        <v>3.646242958938329e-79</v>
       </c>
       <c r="BD2" t="n">
-        <v>5.649863695002554e-87</v>
+        <v>5.138424868303154e-82</v>
       </c>
       <c r="BE2" t="n">
-        <v>9.323396025462571e-89</v>
+        <v>5.133640666892574e-84</v>
       </c>
       <c r="BF2" t="n">
-        <v>5.669227962683873e-92</v>
+        <v>4.068581180467672e-86</v>
       </c>
       <c r="BG2" t="n">
-        <v>4.841622911259237e-94</v>
+        <v>3.625050985563531e-88</v>
       </c>
       <c r="BH2" t="n">
-        <v>4.024028036421313e-95</v>
+        <v>1.431798539310462e-90</v>
       </c>
       <c r="BI2" t="n">
-        <v>1.637834746150178e-96</v>
+        <v>4.671506228279481e-92</v>
       </c>
       <c r="BJ2" t="n">
-        <v>1.15653713951882e-99</v>
+        <v>3.982240935939469e-94</v>
       </c>
       <c r="BK2" t="n">
-        <v>3.975011823781732e-102</v>
+        <v>1.38370831921821e-96</v>
       </c>
       <c r="BL2" t="n">
-        <v>1.334765651855974e-104</v>
+        <v>3.874100067537786e-99</v>
       </c>
       <c r="BM2" t="n">
-        <v>2.044952074188779e-107</v>
+        <v>5.896517906161021e-102</v>
       </c>
       <c r="BN2" t="n">
-        <v>5.681929217017981e-110</v>
+        <v>1.388871502930474e-104</v>
       </c>
       <c r="BO2" t="n">
-        <v>1.195450630640361e-112</v>
+        <v>2.671046045508126e-107</v>
       </c>
       <c r="BP2" t="n">
-        <v>2.809376641416066e-115</v>
+        <v>1.073490623118688e-109</v>
       </c>
       <c r="BQ2" t="n">
-        <v>3.120726719805123e-117</v>
+        <v>2.493504105341266e-112</v>
       </c>
       <c r="BR2" t="n">
-        <v>3.397168248219558e-120</v>
+        <v>1.265641775460008e-114</v>
       </c>
       <c r="BS2" t="n">
-        <v>9.721223479289832e-123</v>
+        <v>3.107059462100585e-117</v>
       </c>
       <c r="BT2" t="n">
-        <v>1.838175754117392e-125</v>
+        <v>9.313438118223531e-120</v>
       </c>
       <c r="BU2" t="n">
-        <v>6.155565877695931e-128</v>
+        <v>3.129368130872864e-122</v>
       </c>
       <c r="BV2" t="n">
-        <v>1.777618759435743e-130</v>
+        <v>5.608913225348151e-125</v>
       </c>
       <c r="BW2" t="n">
-        <v>8.386227445319385e-133</v>
+        <v>8.222020503797854e-128</v>
       </c>
       <c r="BX2" t="n">
-        <v>6.853479877040797e-136</v>
+        <v>4.242759001344459e-130</v>
       </c>
       <c r="BY2" t="n">
-        <v>8.638342247259386e-138</v>
+        <v>1.346207467252771e-132</v>
       </c>
       <c r="BZ2" t="n">
-        <v>6.728103924580017e-141</v>
+        <v>5.169059552169898e-135</v>
       </c>
       <c r="CA2" t="n">
-        <v>4.531120419247886e-143</v>
+        <v>9.211912249444266e-138</v>
       </c>
       <c r="CB2" t="n">
-        <v>3.564208470765192e-146</v>
+        <v>2.80731636776549e-140</v>
       </c>
       <c r="CC2" t="n">
-        <v>1.048948899728364e-148</v>
+        <v>4.632776154742529e-143</v>
       </c>
       <c r="CD2" t="n">
-        <v>2.109267877752464e-151</v>
+        <v>1.665510477249076e-145</v>
       </c>
       <c r="CE2" t="n">
-        <v>2.514386498978565e-154</v>
+        <v>1.883726142519307e-148</v>
       </c>
       <c r="CF2" t="n">
-        <v>3.32318179952351e-157</v>
+        <v>3.114484504064593e-151</v>
       </c>
       <c r="CG2" t="n">
-        <v>5.152431627998352e-160</v>
+        <v>5.470873812152878e-154</v>
       </c>
       <c r="CH2" t="n">
-        <v>1.045371278268696e-162</v>
+        <v>9.304637150116469e-157</v>
       </c>
       <c r="CI2" t="n">
-        <v>5.126610397212649e-165</v>
+        <v>1.832240526422285e-159</v>
       </c>
       <c r="CJ2" t="n">
-        <v>2.594183426041524e-167</v>
+        <v>1.160716938697965e-161</v>
       </c>
       <c r="CK2" t="n">
-        <v>2.852533120889667e-170</v>
+        <v>1.568176344308986e-164</v>
       </c>
       <c r="CL2" t="n">
-        <v>1.285391738267445e-172</v>
+        <v>1.696741474581261e-167</v>
       </c>
       <c r="CM2" t="n">
-        <v>2.223963043624645e-175</v>
+        <v>4.300651463939555e-170</v>
       </c>
       <c r="CN2" t="n">
-        <v>1.685649526911871e-178</v>
+        <v>1.047508751676931e-172</v>
       </c>
       <c r="CO2" t="n">
-        <v>2.670086915342163e-181</v>
+        <v>1.732939138909158e-175</v>
       </c>
       <c r="CP2" t="n">
-        <v>2.330661698602036e-184</v>
+        <v>1.523598167725165e-178</v>
       </c>
       <c r="CQ2" t="n">
-        <v>4.900750135356906e-187</v>
+        <v>3.151197171340903e-181</v>
       </c>
       <c r="CR2" t="n">
-        <v>5.046544752156317e-190</v>
+        <v>3.302267406095422e-184</v>
       </c>
       <c r="CS2" t="n">
-        <v>9.249710140435574e-193</v>
+        <v>5.134916248086702e-187</v>
       </c>
       <c r="CT2" t="n">
-        <v>1.751824138533092e-195</v>
+        <v>1.005814877920144e-189</v>
       </c>
       <c r="CU2" t="n">
-        <v>2.634234804591644e-198</v>
+        <v>1.192711241181832e-192</v>
       </c>
       <c r="CV2" t="n">
-        <v>5.160943191261716e-201</v>
+        <v>2.85328819644691e-195</v>
       </c>
       <c r="CW2" t="n">
-        <v>1.526587657135688e-203</v>
+        <v>4.316903310314282e-198</v>
       </c>
       <c r="CX2" t="n">
-        <v>2.552104786716484e-206</v>
+        <v>9.566071053159932e-201</v>
       </c>
       <c r="CY2" t="n">
-        <v>5.40436278756897e-209</v>
+        <v>2.438278671094978e-203</v>
       </c>
       <c r="CZ2" t="n">
-        <v>1.349116172050441e-211</v>
+        <v>4.348715588948986e-206</v>
       </c>
       <c r="DA2" t="n">
-        <v>1.105545631806793e-214</v>
+        <v>6.61655663132059e-209</v>
       </c>
       <c r="DB2" t="n">
-        <v>1.342261136627342e-217</v>
+        <v>8.032726191815989e-212</v>
       </c>
       <c r="DC2" t="n">
-        <v>9.544316092727889e-220</v>
+        <v>8.480139282890336e-215</v>
       </c>
       <c r="DD2" t="n">
-        <v>3.567005714088845e-222</v>
+        <v>5.43651098465913e-217</v>
       </c>
       <c r="DE2" t="n">
-        <v>2.397942911524217e-225</v>
+        <v>4.31755823222587e-220</v>
       </c>
       <c r="DF2" t="n">
-        <v>2.586948296380725e-228</v>
+        <v>4.558141521482147e-223</v>
       </c>
       <c r="DG2" t="n">
-        <v>9.06188210253464e-231</v>
+        <v>3.700890856332966e-226</v>
       </c>
       <c r="DH2" t="n">
-        <v>3.886614858212058e-233</v>
+        <v>1.785066964076756e-228</v>
       </c>
       <c r="DI2" t="n">
-        <v>8.791275100119018e-236</v>
+        <v>7.562644955200168e-231</v>
       </c>
       <c r="DJ2" t="n">
-        <v>1.414562812630237e-238</v>
+        <v>1.208275760238667e-233</v>
       </c>
       <c r="DK2" t="n">
-        <v>2.387324601335643e-241</v>
+        <v>1.390003135345403e-236</v>
       </c>
       <c r="DL2" t="n">
-        <v>2.897498312560437e-244</v>
+        <v>2.150474439561489e-239</v>
       </c>
       <c r="DM2" t="n">
-        <v>5.108776753395392e-247</v>
+        <v>1.369477406242299e-242</v>
       </c>
       <c r="DN2" t="n">
-        <v>3.511160701587145e-249</v>
+        <v>4.382132788123227e-245</v>
       </c>
       <c r="DO2" t="n">
-        <v>2.871754232587332e-252</v>
+        <v>1.157487734453493e-247</v>
       </c>
       <c r="DP2" t="n">
-        <v>2.800672027790661e-255</v>
+        <v>2.150736566185093e-250</v>
       </c>
       <c r="DQ2" t="n">
-        <v>9.143291690508602e-258</v>
+        <v>2.582027569033155e-253</v>
       </c>
       <c r="DR2" t="n">
-        <v>7.117681272461723e-261</v>
+        <v>4.112244888211057e-256</v>
       </c>
       <c r="DS2" t="n">
-        <v>4.572417750726473e-264</v>
+        <v>4.171585755963235e-259</v>
       </c>
       <c r="DT2" t="n">
-        <v>4.466262677812194e-266</v>
+        <v>3.506042592803475e-262</v>
       </c>
       <c r="DU2" t="n">
-        <v>6.021315133415379e-269</v>
+        <v>1.76432180434712e-264</v>
       </c>
       <c r="DV2" t="n">
-        <v>1.340466769810262e-271</v>
+        <v>7.376672162470656e-267</v>
       </c>
       <c r="DW2" t="n">
-        <v>1.202469662596311e-274</v>
+        <v>5.658245753395952e-270</v>
       </c>
       <c r="DX2" t="n">
-        <v>8.785781265792055e-278</v>
+        <v>4.761898940410685e-273</v>
       </c>
       <c r="DY2" t="n">
-        <v>2.352839701462913e-280</v>
+        <v>4.223394674280097e-276</v>
       </c>
       <c r="DZ2" t="n">
-        <v>3.775816374673988e-283</v>
+        <v>1.315724126168327e-278</v>
       </c>
       <c r="EA2" t="n">
-        <v>3.130521832559127e-286</v>
+        <v>1.08717160814707e-281</v>
       </c>
       <c r="EB2" t="n">
-        <v>7.081626247678845e-289</v>
+        <v>1.052360080531971e-284</v>
       </c>
       <c r="EC2" t="n">
-        <v>8.087904774296174e-292</v>
+        <v>1.729816217465152e-287</v>
       </c>
       <c r="ED2" t="n">
-        <v>1.157207881367494e-294</v>
+        <v>1.533692706770631e-290</v>
       </c>
       <c r="EE2" t="n">
-        <v>7.58025253922219e-298</v>
+        <v>2.624222753665482e-293</v>
       </c>
       <c r="EF2" t="n">
-        <v>1.36358826846082e-300</v>
+        <v>5.132561599015998e-296</v>
       </c>
       <c r="EG2" t="n">
-        <v>1.806331120430708e-303</v>
+        <v>3.057723759624186e-299</v>
       </c>
       <c r="EH2" t="n">
-        <v>2.506772969496655e-306</v>
+        <v>7.405948786680854e-302</v>
       </c>
       <c r="EI2" t="n">
-        <v>0</v>
+        <v>5.491002418069827e-305</v>
       </c>
       <c r="EJ2" t="n">
         <v>0</v>
@@ -9465,6 +9480,9 @@
         <v>0</v>
       </c>
       <c r="SF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="SG2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9478,70 +9496,70 @@
         <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3327291070190232</v>
+        <v>0.3308648686140421</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3286702834046455</v>
+        <v>0.3427263105743406</v>
       </c>
       <c r="E3" t="n">
-        <v>0.400695257314418</v>
+        <v>0.3043853518361088</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3248977292540809</v>
+        <v>0.4355761493624736</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4156430742620588</v>
+        <v>0.3316908442446918</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4849786520966848</v>
+        <v>0.5126667448772062</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5502521606608423</v>
+        <v>0.6002088913501653</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9457124655483301</v>
+        <v>0.6731938052299796</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9764598068335671</v>
+        <v>0.9406048925350664</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9726335092367744</v>
+        <v>0.9768490249286601</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9991164317218874</v>
+        <v>0.9742303852881182</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9999215600965287</v>
+        <v>0.9974673014546422</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9999847961935276</v>
+        <v>0.9998027030722875</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9999988801002351</v>
+        <v>0.999955814504737</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9999998173178443</v>
+        <v>0.9999992645431238</v>
       </c>
       <c r="R3" t="n">
-        <v>0.999999998822563</v>
+        <v>0.999999888175658</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9999999998312392</v>
+        <v>0.9999999883087933</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9999999999936036</v>
+        <v>0.9999999995746203</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9999999999998483</v>
+        <v>0.9999999999884968</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9999999999999899</v>
+        <v>0.9999999999994273</v>
       </c>
       <c r="W3" t="n">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999798</v>
       </c>
       <c r="X3" t="n">
-        <v>1</v>
+        <v>0.9999999999999992</v>
       </c>
       <c r="Y3" t="n">
         <v>1</v>
@@ -10969,6 +10987,9 @@
         <v>1</v>
       </c>
       <c r="SF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="SG3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10982,403 +11003,403 @@
         <v>0.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2934718919159781</v>
+        <v>0.2804705099847123</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1746227196996436</v>
+        <v>0.2108915603579781</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1989147059246327</v>
+        <v>0.09145678753750179</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05020794993674293</v>
+        <v>0.1073815571761648</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04267187573689227</v>
+        <v>0.0343787516614418</v>
       </c>
       <c r="H4" t="n">
-        <v>0.009883938430167825</v>
+        <v>0.02312868222538915</v>
       </c>
       <c r="I4" t="n">
-        <v>0.001207589337941767</v>
+        <v>0.003247839555399664</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001932238856503659</v>
+        <v>0.0004564912696471053</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0001392610678694548</v>
+        <v>0.0004751297516691026</v>
       </c>
       <c r="L4" t="n">
-        <v>1.447531447874394e-06</v>
+        <v>2.215025257828964e-05</v>
       </c>
       <c r="M4" t="n">
-        <v>4.399529457649207e-07</v>
+        <v>1.913935181909412e-06</v>
       </c>
       <c r="N4" t="n">
-        <v>5.68581325138369e-08</v>
+        <v>2.177027335639375e-07</v>
       </c>
       <c r="O4" t="n">
-        <v>1.168846649693126e-09</v>
+        <v>1.918957272267653e-08</v>
       </c>
       <c r="P4" t="n">
-        <v>1.708460860463424e-10</v>
+        <v>1.122757762579345e-10</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.175444751622856e-12</v>
+        <v>2.13489996108615e-11</v>
       </c>
       <c r="R4" t="n">
-        <v>7.86388704955431e-12</v>
+        <v>2.820072538580712e-13</v>
       </c>
       <c r="S4" t="n">
-        <v>6.761626764408629e-14</v>
+        <v>1.572564502127937e-13</v>
       </c>
       <c r="T4" t="n">
-        <v>1.894693582123516e-15</v>
+        <v>4.967770626225244e-15</v>
       </c>
       <c r="U4" t="n">
-        <v>7.116882472480206e-17</v>
+        <v>1.344256626456365e-16</v>
       </c>
       <c r="V4" t="n">
-        <v>1.901975470578566e-19</v>
+        <v>1.17908679450393e-18</v>
       </c>
       <c r="W4" t="n">
-        <v>3.46359222055276e-21</v>
+        <v>8.521934193971309e-21</v>
       </c>
       <c r="X4" t="n">
-        <v>6.45963370310888e-24</v>
+        <v>5.300380818009627e-23</v>
       </c>
       <c r="Y4" t="n">
-        <v>2.672361831083019e-25</v>
+        <v>1.545096108638721e-24</v>
       </c>
       <c r="Z4" t="n">
-        <v>6.599429044236994e-28</v>
+        <v>2.095183162808199e-26</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.812413197120713e-29</v>
+        <v>5.245177423654955e-28</v>
       </c>
       <c r="AB4" t="n">
-        <v>2.433487253497114e-31</v>
+        <v>3.009125137503684e-30</v>
       </c>
       <c r="AC4" t="n">
-        <v>1.287534276494063e-32</v>
+        <v>1.518273689922616e-32</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.162112438690706e-35</v>
+        <v>4.573357970683252e-34</v>
       </c>
       <c r="AE4" t="n">
-        <v>7.043746047473071e-38</v>
+        <v>1.122649276578699e-36</v>
       </c>
       <c r="AF4" t="n">
-        <v>1.147228571501236e-39</v>
+        <v>1.920699415382076e-38</v>
       </c>
       <c r="AG4" t="n">
-        <v>1.983572724601819e-41</v>
+        <v>1.041732248319391e-40</v>
       </c>
       <c r="AH4" t="n">
-        <v>1.099214109290753e-43</v>
+        <v>5.49698325190916e-43</v>
       </c>
       <c r="AI4" t="n">
-        <v>2.753577324747715e-46</v>
+        <v>8.312324298133966e-46</v>
       </c>
       <c r="AJ4" t="n">
-        <v>4.128410444001617e-48</v>
+        <v>5.565941485502695e-48</v>
       </c>
       <c r="AK4" t="n">
-        <v>5.408322062599134e-51</v>
+        <v>1.028687214679252e-49</v>
       </c>
       <c r="AL4" t="n">
-        <v>1.128194102924419e-52</v>
+        <v>6.069636463826136e-52</v>
       </c>
       <c r="AM4" t="n">
-        <v>1.176073079430912e-54</v>
+        <v>3.469635383737044e-54</v>
       </c>
       <c r="AN4" t="n">
-        <v>3.59473117229043e-57</v>
+        <v>4.440066211019457e-56</v>
       </c>
       <c r="AO4" t="n">
-        <v>3.955841454995551e-58</v>
+        <v>1.155871542276966e-57</v>
       </c>
       <c r="AP4" t="n">
-        <v>5.588501152717967e-61</v>
+        <v>3.746892751824252e-59</v>
       </c>
       <c r="AQ4" t="n">
-        <v>8.374322135468768e-63</v>
+        <v>7.05083931988653e-61</v>
       </c>
       <c r="AR4" t="n">
-        <v>1.170954020367575e-64</v>
+        <v>5.073104861072121e-63</v>
       </c>
       <c r="AS4" t="n">
-        <v>4.165203301552408e-67</v>
+        <v>9.68298386986609e-66</v>
       </c>
       <c r="AT4" t="n">
-        <v>6.840071322667045e-68</v>
+        <v>3.443647332802493e-68</v>
       </c>
       <c r="AU4" t="n">
-        <v>7.509938836129474e-73</v>
+        <v>4.829372658707518e-70</v>
       </c>
       <c r="AV4" t="n">
-        <v>1.794431073572376e-74</v>
+        <v>2.679761582948738e-72</v>
       </c>
       <c r="AW4" t="n">
-        <v>7.934446767047143e-78</v>
+        <v>1.463061886216209e-74</v>
       </c>
       <c r="AX4" t="n">
-        <v>1.890286845989091e-80</v>
+        <v>3.747759133527122e-77</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.922388487024399e-82</v>
+        <v>8.49739521846003e-80</v>
       </c>
       <c r="AZ4" t="n">
-        <v>6.759695188862616e-85</v>
+        <v>3.626162198437479e-82</v>
       </c>
       <c r="BA4" t="n">
-        <v>1.022115541205165e-86</v>
+        <v>2.115813135098485e-84</v>
       </c>
       <c r="BB4" t="n">
-        <v>8.15597464979384e-90</v>
+        <v>1.476333154864625e-86</v>
       </c>
       <c r="BC4" t="n">
-        <v>1.306667323894053e-91</v>
+        <v>1.775895683773194e-88</v>
       </c>
       <c r="BD4" t="n">
-        <v>3.323888211622727e-94</v>
+        <v>7.024100725948044e-91</v>
       </c>
       <c r="BE4" t="n">
-        <v>6.789449334868529e-97</v>
+        <v>1.281193379185666e-93</v>
       </c>
       <c r="BF4" t="n">
-        <v>3.304345423416374e-98</v>
+        <v>5.887829819755327e-96</v>
       </c>
       <c r="BG4" t="n">
-        <v>1.047162245219669e-100</v>
+        <v>2.313051079923991e-98</v>
       </c>
       <c r="BH4" t="n">
-        <v>4.200837885334507e-100</v>
+        <v>2.6444413032289e-100</v>
       </c>
       <c r="BI4" t="n">
-        <v>8.0238037069988e-105</v>
+        <v>1.508473948521804e-101</v>
       </c>
       <c r="BJ4" t="n">
-        <v>8.021244705274809e-107</v>
+        <v>5.636156785015245e-104</v>
       </c>
       <c r="BK4" t="n">
-        <v>1.284578624691279e-109</v>
+        <v>1.474006247766875e-106</v>
       </c>
       <c r="BL4" t="n">
-        <v>1.362619168872853e-112</v>
+        <v>2.675973246790757e-109</v>
       </c>
       <c r="BM4" t="n">
-        <v>3.10840489727995e-115</v>
+        <v>6.138801967059162e-112</v>
       </c>
       <c r="BN4" t="n">
-        <v>3.94015670739698e-118</v>
+        <v>8.700240860880718e-115</v>
       </c>
       <c r="BO4" t="n">
-        <v>7.174904233602555e-121</v>
+        <v>1.624100989624688e-117</v>
       </c>
       <c r="BP4" t="n">
-        <v>1.65394283701487e-123</v>
+        <v>1.372197799115501e-120</v>
       </c>
       <c r="BQ4" t="n">
-        <v>1.393700613642396e-126</v>
+        <v>2.890118629077044e-123</v>
       </c>
       <c r="BR4" t="n">
-        <v>3.681224700517526e-129</v>
+        <v>8.09601869632772e-126</v>
       </c>
       <c r="BS4" t="n">
-        <v>3.780670197610212e-132</v>
+        <v>9.035943404443166e-129</v>
       </c>
       <c r="BT4" t="n">
-        <v>7.824634245398888e-135</v>
+        <v>8.713774063127265e-132</v>
       </c>
       <c r="BU4" t="n">
-        <v>8.856594167187765e-138</v>
+        <v>9.162408161459281e-135</v>
       </c>
       <c r="BV4" t="n">
-        <v>8.447204974820219e-141</v>
+        <v>1.799044342400478e-137</v>
       </c>
       <c r="BW4" t="n">
-        <v>2.106507408812045e-143</v>
+        <v>3.668145500492888e-140</v>
       </c>
       <c r="BX4" t="n">
-        <v>7.125622997247849e-146</v>
+        <v>9.010816298859896e-143</v>
       </c>
       <c r="BY4" t="n">
-        <v>3.005642044490487e-149</v>
+        <v>8.117782583500878e-146</v>
       </c>
       <c r="BZ4" t="n">
-        <v>8.281568711863723e-152</v>
+        <v>2.499657077931179e-148</v>
       </c>
       <c r="CA4" t="n">
-        <v>1.014054656588591e-154</v>
+        <v>2.884221014221378e-151</v>
       </c>
       <c r="CB4" t="n">
-        <v>2.707846781535603e-157</v>
+        <v>8.60690322354738e-154</v>
       </c>
       <c r="CC4" t="n">
-        <v>5.825999961756438e-159</v>
+        <v>1.038438255362965e-156</v>
       </c>
       <c r="CD4" t="n">
-        <v>5.450129234568065e-162</v>
+        <v>1.504311424436323e-158</v>
       </c>
       <c r="CE4" t="n">
-        <v>8.946829952066779e-165</v>
+        <v>2.519228714702654e-161</v>
       </c>
       <c r="CF4" t="n">
-        <v>1.182410964260344e-167</v>
+        <v>2.885996848234689e-164</v>
       </c>
       <c r="CG4" t="n">
-        <v>1.745824681547715e-170</v>
+        <v>2.803683361045745e-167</v>
       </c>
       <c r="CH4" t="n">
-        <v>5.262749043452874e-173</v>
+        <v>3.545635528037962e-170</v>
       </c>
       <c r="CI4" t="n">
-        <v>9.510175286545521e-175</v>
+        <v>9.742193991732929e-173</v>
       </c>
       <c r="CJ4" t="n">
-        <v>2.771205793643455e-178</v>
+        <v>3.482301309141829e-175</v>
       </c>
       <c r="CK4" t="n">
-        <v>4.110327655304359e-181</v>
+        <v>3.995402744496315e-178</v>
       </c>
       <c r="CL4" t="n">
-        <v>5.748867512423151e-184</v>
+        <v>5.722302575352594e-181</v>
       </c>
       <c r="CM4" t="n">
-        <v>1.286747940702386e-186</v>
+        <v>1.453530653136138e-183</v>
       </c>
       <c r="CN4" t="n">
-        <v>4.367074232609134e-189</v>
+        <v>2.502590547253381e-186</v>
       </c>
       <c r="CO4" t="n">
-        <v>4.68406775929644e-192</v>
+        <v>4.026978713256243e-189</v>
       </c>
       <c r="CP4" t="n">
-        <v>9.058775753730011e-195</v>
+        <v>6.894046423849462e-192</v>
       </c>
       <c r="CQ4" t="n">
-        <v>9.965445684509347e-198</v>
+        <v>5.842862561212546e-195</v>
       </c>
       <c r="CR4" t="n">
-        <v>1.690799731206525e-200</v>
+        <v>1.11531263409016e-197</v>
       </c>
       <c r="CS4" t="n">
-        <v>3.642096643563485e-203</v>
+        <v>1.230319541205045e-200</v>
       </c>
       <c r="CT4" t="n">
-        <v>5.856246746296492e-206</v>
+        <v>2.195983355506923e-203</v>
       </c>
       <c r="CU4" t="n">
-        <v>2.371559931838471e-208</v>
+        <v>5.020242574785584e-206</v>
       </c>
       <c r="CV4" t="n">
-        <v>1.654795909867353e-211</v>
+        <v>1.015337445206485e-208</v>
       </c>
       <c r="CW4" t="n">
-        <v>1.050879710266396e-214</v>
+        <v>8.353281793542779e-212</v>
       </c>
       <c r="CX4" t="n">
-        <v>5.729761813267457e-217</v>
+        <v>8.0054177265819e-215</v>
       </c>
       <c r="CY4" t="n">
-        <v>9.680732203962379e-220</v>
+        <v>2.110188573207284e-217</v>
       </c>
       <c r="CZ4" t="n">
-        <v>5.662604877710034e-223</v>
+        <v>3.912896999764731e-220</v>
       </c>
       <c r="DA4" t="n">
-        <v>8.549577750446851e-226</v>
+        <v>4.132203247108951e-223</v>
       </c>
       <c r="DB4" t="n">
-        <v>8.689352992265192e-229</v>
+        <v>4.150404092212378e-226</v>
       </c>
       <c r="DC4" t="n">
-        <v>3.383306040085875e-230</v>
+        <v>4.483929669178973e-229</v>
       </c>
       <c r="DD4" t="n">
-        <v>1.012716696497363e-233</v>
+        <v>1.974294023945881e-231</v>
       </c>
       <c r="DE4" t="n">
-        <v>1.480207697629124e-236</v>
+        <v>2.462321759305391e-234</v>
       </c>
       <c r="DF4" t="n">
-        <v>2.106788064684261e-239</v>
+        <v>2.196938746310341e-237</v>
       </c>
       <c r="DG4" t="n">
-        <v>5.121871843313264e-241</v>
+        <v>3.712595345497315e-240</v>
       </c>
       <c r="DH4" t="n">
-        <v>3.212664794471243e-243</v>
+        <v>2.830577356969342e-242</v>
       </c>
       <c r="DI4" t="n">
-        <v>2.429718214040557e-246</v>
+        <v>1.050059296160012e-244</v>
       </c>
       <c r="DJ4" t="n">
-        <v>2.423632800281966e-249</v>
+        <v>1.017274284398029e-247</v>
       </c>
       <c r="DK4" t="n">
-        <v>7.17523289911708e-252</v>
+        <v>1.260121462500148e-250</v>
       </c>
       <c r="DL4" t="n">
-        <v>4.967049568737269e-255</v>
+        <v>3.598764063593689e-253</v>
       </c>
       <c r="DM4" t="n">
-        <v>9.431066031375601e-258</v>
+        <v>5.3004377428502e-256</v>
       </c>
       <c r="DN4" t="n">
-        <v>1.813645329375176e-260</v>
+        <v>6.491124034247331e-259</v>
       </c>
       <c r="DO4" t="n">
-        <v>3.555549705778225e-263</v>
+        <v>2.050590720231929e-261</v>
       </c>
       <c r="DP4" t="n">
-        <v>2.729454316992975e-266</v>
+        <v>1.706167261888081e-264</v>
       </c>
       <c r="DQ4" t="n">
-        <v>2.201666110653078e-269</v>
+        <v>1.084229350154708e-267</v>
       </c>
       <c r="DR4" t="n">
-        <v>3.173827055327821e-272</v>
+        <v>1.998349583763482e-270</v>
       </c>
       <c r="DS4" t="n">
-        <v>3.57958060557292e-275</v>
+        <v>2.134066413449949e-273</v>
       </c>
       <c r="DT4" t="n">
-        <v>8.515301252240871e-278</v>
+        <v>1.738829847011345e-276</v>
       </c>
       <c r="DU4" t="n">
-        <v>1.482201934909117e-279</v>
+        <v>5.939312054580107e-279</v>
       </c>
       <c r="DV4" t="n">
-        <v>6.282589688810167e-283</v>
+        <v>1.829645733516766e-281</v>
       </c>
       <c r="DW4" t="n">
-        <v>4.786108627990092e-286</v>
+        <v>1.599977037332655e-284</v>
       </c>
       <c r="DX4" t="n">
-        <v>4.191674514531038e-289</v>
+        <v>1.314771344402366e-287</v>
       </c>
       <c r="DY4" t="n">
-        <v>3.414217685590051e-291</v>
+        <v>9.344301162476996e-291</v>
       </c>
       <c r="DZ4" t="n">
-        <v>2.169606142166873e-294</v>
+        <v>2.80016225685532e-293</v>
       </c>
       <c r="EA4" t="n">
-        <v>1.623096623675233e-297</v>
+        <v>2.748448905437284e-296</v>
       </c>
       <c r="EB4" t="n">
-        <v>1.143468684840539e-300</v>
+        <v>1.771867372577223e-299</v>
       </c>
       <c r="EC4" t="n">
-        <v>1.085615662410139e-303</v>
+        <v>1.984807778282893e-302</v>
       </c>
       <c r="ED4" t="n">
-        <v>1.789013449720053e-306</v>
+        <v>2.680723363966801e-305</v>
       </c>
       <c r="EE4" t="n">
-        <v>0</v>
+        <v>3.947878587960706e-308</v>
       </c>
       <c r="EF4" t="n">
         <v>0</v>
@@ -12473,6 +12494,9 @@
         <v>0</v>
       </c>
       <c r="SF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="SG4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12487,7 +12511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:SF4"/>
+  <dimension ref="A1:SG4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13993,6 +14017,9 @@
       <c r="SF1" s="2" t="n">
         <v>2521</v>
       </c>
+      <c r="SG1" s="2" t="n">
+        <v>2522</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -14004,361 +14031,361 @@
         <v>0.34</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3676571349839057</v>
+        <v>0.2732288957993735</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4006098519506244</v>
+        <v>0.3570473787970924</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2423473608918792</v>
+        <v>0.3819773497471248</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02268495308171238</v>
+        <v>0.1954519946601752</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01268835610165971</v>
+        <v>0.08112531388741084</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03099267116505003</v>
+        <v>0.02617090090064152</v>
       </c>
       <c r="I2" t="n">
-        <v>0.009948915538846595</v>
+        <v>0.03700636277628283</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001427445120400899</v>
+        <v>0.009683288906800267</v>
       </c>
       <c r="K2" t="n">
-        <v>8.350859409576117e-05</v>
+        <v>0.001169065762425234</v>
       </c>
       <c r="L2" t="n">
-        <v>1.793813948076547e-07</v>
+        <v>0.0002342132859040842</v>
       </c>
       <c r="M2" t="n">
-        <v>1.17454591044856e-09</v>
+        <v>2.216386837100766e-05</v>
       </c>
       <c r="N2" t="n">
-        <v>1.297830605076371e-10</v>
+        <v>2.405287787064458e-06</v>
       </c>
       <c r="O2" t="n">
-        <v>2.898115082402115e-13</v>
+        <v>3.365686794930939e-08</v>
       </c>
       <c r="P2" t="n">
-        <v>7.952612939999262e-15</v>
+        <v>2.60528209927367e-10</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.68501052430758e-17</v>
+        <v>8.496950824326657e-12</v>
       </c>
       <c r="R2" t="n">
-        <v>4.739925619732459e-19</v>
+        <v>1.551792213526147e-13</v>
       </c>
       <c r="S2" t="n">
-        <v>6.828860165763027e-20</v>
+        <v>5.174627368328493e-16</v>
       </c>
       <c r="T2" t="n">
-        <v>5.53491882716184e-24</v>
+        <v>2.099109652167115e-17</v>
       </c>
       <c r="U2" t="n">
-        <v>1.724064382523975e-25</v>
+        <v>4.048487123401357e-19</v>
       </c>
       <c r="V2" t="n">
-        <v>6.10514466965823e-29</v>
+        <v>1.263839571931414e-21</v>
       </c>
       <c r="W2" t="n">
-        <v>6.915364553185056e-31</v>
+        <v>8.145144915245995e-24</v>
       </c>
       <c r="X2" t="n">
-        <v>5.218535497882964e-31</v>
+        <v>3.71903412569322e-26</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.007992384536384e-35</v>
+        <v>1.269210746385768e-27</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.948264647643314e-38</v>
+        <v>2.972646586770325e-30</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.536305262914061e-41</v>
+        <v>3.237813237451207e-33</v>
       </c>
       <c r="AB2" t="n">
-        <v>8.237644436436907e-44</v>
+        <v>1.074233702000034e-35</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.026601603424991e-46</v>
+        <v>2.266732347037029e-38</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.112923196315193e-49</v>
+        <v>3.404238050425361e-41</v>
       </c>
       <c r="AE2" t="n">
-        <v>4.016849996807437e-52</v>
+        <v>7.271862523439922e-44</v>
       </c>
       <c r="AF2" t="n">
-        <v>1.196757741862006e-54</v>
+        <v>2.213964664094924e-46</v>
       </c>
       <c r="AG2" t="n">
-        <v>3.262048556706351e-57</v>
+        <v>2.346951180372658e-49</v>
       </c>
       <c r="AH2" t="n">
-        <v>2.727778647377673e-59</v>
+        <v>2.152150751744109e-51</v>
       </c>
       <c r="AI2" t="n">
-        <v>2.459594798044638e-61</v>
+        <v>4.279160877267557e-54</v>
       </c>
       <c r="AJ2" t="n">
-        <v>3.28646640851716e-64</v>
+        <v>2.201770168264382e-56</v>
       </c>
       <c r="AK2" t="n">
-        <v>1.268192410089393e-66</v>
+        <v>5.359671331779412e-58</v>
       </c>
       <c r="AL2" t="n">
-        <v>2.62208814437253e-68</v>
+        <v>2.094613640534627e-60</v>
       </c>
       <c r="AM2" t="n">
-        <v>7.915067813405226e-70</v>
+        <v>4.039006964824344e-62</v>
       </c>
       <c r="AN2" t="n">
-        <v>2.107747891773615e-73</v>
+        <v>3.949618669524015e-64</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.529583940486025e-76</v>
+        <v>2.750235900583203e-67</v>
       </c>
       <c r="AP2" t="n">
-        <v>2.348285114831478e-79</v>
+        <v>4.691283516931374e-70</v>
       </c>
       <c r="AQ2" t="n">
-        <v>6.067186801614679e-82</v>
+        <v>7.812689930107244e-73</v>
       </c>
       <c r="AR2" t="n">
-        <v>1.247108575219159e-84</v>
+        <v>1.015621491055453e-75</v>
       </c>
       <c r="AS2" t="n">
-        <v>1.039834771654614e-87</v>
+        <v>3.808739550477936e-78</v>
       </c>
       <c r="AT2" t="n">
-        <v>1.398003788550672e-90</v>
+        <v>5.705054364428818e-81</v>
       </c>
       <c r="AU2" t="n">
-        <v>7.759914847322812e-93</v>
+        <v>1.003446395548553e-83</v>
       </c>
       <c r="AV2" t="n">
-        <v>5.209797048475954e-95</v>
+        <v>5.194430533063578e-86</v>
       </c>
       <c r="AW2" t="n">
-        <v>1.547695938174801e-97</v>
+        <v>9.550924596299756e-89</v>
       </c>
       <c r="AX2" t="n">
-        <v>1.504278310471618e-100</v>
+        <v>5.909392806096315e-91</v>
       </c>
       <c r="AY2" t="n">
-        <v>4.341745189813476e-103</v>
+        <v>1.669203493140827e-93</v>
       </c>
       <c r="AZ2" t="n">
-        <v>4.612284612856334e-106</v>
+        <v>2.55160843587683e-96</v>
       </c>
       <c r="BA2" t="n">
-        <v>6.040364678984049e-109</v>
+        <v>3.529773445046923e-99</v>
       </c>
       <c r="BB2" t="n">
-        <v>1.101883142179365e-111</v>
+        <v>5.454402774068141e-102</v>
       </c>
       <c r="BC2" t="n">
-        <v>3.912839250382702e-114</v>
+        <v>8.251720193568128e-105</v>
       </c>
       <c r="BD2" t="n">
-        <v>7.555141229015933e-117</v>
+        <v>1.543250361797498e-107</v>
       </c>
       <c r="BE2" t="n">
-        <v>4.48363813382798e-120</v>
+        <v>6.474361442546307e-110</v>
       </c>
       <c r="BF2" t="n">
-        <v>1.987980286339206e-122</v>
+        <v>6.137635617908293e-113</v>
       </c>
       <c r="BG2" t="n">
-        <v>8.302644353621824e-126</v>
+        <v>1.675942097761349e-115</v>
       </c>
       <c r="BH2" t="n">
-        <v>9.849897356687213e-129</v>
+        <v>1.059022021050042e-118</v>
       </c>
       <c r="BI2" t="n">
-        <v>6.443259843621389e-132</v>
+        <v>1.459466549834281e-121</v>
       </c>
       <c r="BJ2" t="n">
-        <v>4.840809859530923e-135</v>
+        <v>1.701288733578674e-124</v>
       </c>
       <c r="BK2" t="n">
-        <v>4.445662207489315e-138</v>
+        <v>1.083007227530421e-127</v>
       </c>
       <c r="BL2" t="n">
-        <v>1.968334626414918e-141</v>
+        <v>8.863121695831475e-131</v>
       </c>
       <c r="BM2" t="n">
-        <v>1.782988283666289e-144</v>
+        <v>7.374772712806372e-134</v>
       </c>
       <c r="BN2" t="n">
-        <v>1.517177203066844e-147</v>
+        <v>6.399129938889886e-137</v>
       </c>
       <c r="BO2" t="n">
-        <v>2.415114079337641e-150</v>
+        <v>3.09382681855717e-140</v>
       </c>
       <c r="BP2" t="n">
-        <v>2.985237358945942e-153</v>
+        <v>9.216975308199311e-143</v>
       </c>
       <c r="BQ2" t="n">
-        <v>1.64759079023519e-156</v>
+        <v>8.44727770657713e-146</v>
       </c>
       <c r="BR2" t="n">
-        <v>1.057060650820365e-159</v>
+        <v>6.529388648923937e-149</v>
       </c>
       <c r="BS2" t="n">
-        <v>8.177208810045492e-162</v>
+        <v>3.669421667083298e-152</v>
       </c>
       <c r="BT2" t="n">
-        <v>1.563622085342296e-164</v>
+        <v>1.998794669728862e-154</v>
       </c>
       <c r="BU2" t="n">
-        <v>9.895031976334979e-168</v>
+        <v>1.580077935610468e-157</v>
       </c>
       <c r="BV2" t="n">
-        <v>1.064897740169398e-170</v>
+        <v>1.093076295887019e-160</v>
       </c>
       <c r="BW2" t="n">
-        <v>1.068554129763722e-173</v>
+        <v>8.458646569849782e-164</v>
       </c>
       <c r="BX2" t="n">
-        <v>2.397476935727727e-176</v>
+        <v>1.081346629729683e-166</v>
       </c>
       <c r="BY2" t="n">
-        <v>1.140530286446095e-179</v>
+        <v>5.338058331901286e-169</v>
       </c>
       <c r="BZ2" t="n">
-        <v>1.358536379958916e-182</v>
+        <v>3.836103278033798e-172</v>
       </c>
       <c r="CA2" t="n">
-        <v>9.425366739227779e-186</v>
+        <v>3.257102598085161e-175</v>
       </c>
       <c r="CB2" t="n">
-        <v>6.934391126967191e-189</v>
+        <v>3.226390391699587e-178</v>
       </c>
       <c r="CC2" t="n">
-        <v>4.352566155857013e-192</v>
+        <v>1.707408672471369e-181</v>
       </c>
       <c r="CD2" t="n">
-        <v>4.501671335829414e-195</v>
+        <v>1.815419688673355e-184</v>
       </c>
       <c r="CE2" t="n">
-        <v>7.754654973424365e-198</v>
+        <v>1.01908897445214e-187</v>
       </c>
       <c r="CF2" t="n">
-        <v>3.526402444046896e-200</v>
+        <v>1.863620545547416e-190</v>
       </c>
       <c r="CG2" t="n">
-        <v>1.237659036374753e-203</v>
+        <v>2.813623098474391e-193</v>
       </c>
       <c r="CH2" t="n">
-        <v>7.067872064274835e-206</v>
+        <v>2.116979634197807e-196</v>
       </c>
       <c r="CI2" t="n">
-        <v>7.135507513572114e-209</v>
+        <v>7.053179952833195e-199</v>
       </c>
       <c r="CJ2" t="n">
-        <v>4.383979160069207e-212</v>
+        <v>3.929498916229202e-202</v>
       </c>
       <c r="CK2" t="n">
-        <v>2.279220168062485e-215</v>
+        <v>2.603176647103759e-205</v>
       </c>
       <c r="CL2" t="n">
-        <v>1.244034213323286e-218</v>
+        <v>1.301990339927298e-208</v>
       </c>
       <c r="CM2" t="n">
-        <v>1.2368448475627e-221</v>
+        <v>1.658665367937752e-211</v>
       </c>
       <c r="CN2" t="n">
-        <v>2.197601222411756e-224</v>
+        <v>8.140519286288745e-215</v>
       </c>
       <c r="CO2" t="n">
-        <v>1.27597666434243e-227</v>
+        <v>9.785552576279905e-218</v>
       </c>
       <c r="CP2" t="n">
-        <v>1.714124831361727e-230</v>
+        <v>5.919914396442165e-221</v>
       </c>
       <c r="CQ2" t="n">
-        <v>4.770512014101915e-233</v>
+        <v>6.846945039402231e-224</v>
       </c>
       <c r="CR2" t="n">
-        <v>9.165226396796583e-236</v>
+        <v>2.186941480778297e-226</v>
       </c>
       <c r="CS2" t="n">
-        <v>4.019966079031388e-239</v>
+        <v>3.840710551036565e-229</v>
       </c>
       <c r="CT2" t="n">
-        <v>2.311015185638442e-242</v>
+        <v>3.130977508039419e-232</v>
       </c>
       <c r="CU2" t="n">
-        <v>2.049122955059732e-245</v>
+        <v>2.482224887845293e-235</v>
       </c>
       <c r="CV2" t="n">
-        <v>9.041173188338012e-249</v>
+        <v>1.637702569899997e-238</v>
       </c>
       <c r="CW2" t="n">
-        <v>3.970902485286937e-252</v>
+        <v>7.871536317585233e-242</v>
       </c>
       <c r="CX2" t="n">
-        <v>2.397363876397826e-255</v>
+        <v>2.790542267515406e-245</v>
       </c>
       <c r="CY2" t="n">
-        <v>1.585232506407631e-258</v>
+        <v>2.65793700460113e-248</v>
       </c>
       <c r="CZ2" t="n">
-        <v>1.745335732389643e-261</v>
+        <v>3.640543035864978e-251</v>
       </c>
       <c r="DA2" t="n">
-        <v>1.340262943456179e-264</v>
+        <v>1.554454044193339e-254</v>
       </c>
       <c r="DB2" t="n">
-        <v>1.177804910383589e-267</v>
+        <v>1.540910946095008e-257</v>
       </c>
       <c r="DC2" t="n">
-        <v>5.460831399992054e-271</v>
+        <v>8.810107713942819e-261</v>
       </c>
       <c r="DD2" t="n">
-        <v>1.514182062815329e-273</v>
+        <v>3.165857263099195e-264</v>
       </c>
       <c r="DE2" t="n">
-        <v>1.073637170977804e-276</v>
+        <v>1.565753511107612e-266</v>
       </c>
       <c r="DF2" t="n">
-        <v>4.82390238027996e-280</v>
+        <v>8.163079918199396e-270</v>
       </c>
       <c r="DG2" t="n">
-        <v>3.466355703170838e-283</v>
+        <v>6.096789591502077e-273</v>
       </c>
       <c r="DH2" t="n">
-        <v>1.264809174994922e-286</v>
+        <v>2.242494647074508e-276</v>
       </c>
       <c r="DI2" t="n">
-        <v>1.581240424070338e-289</v>
+        <v>8.677582329531957e-280</v>
       </c>
       <c r="DJ2" t="n">
-        <v>1.352506447793223e-292</v>
+        <v>1.116021504607511e-282</v>
       </c>
       <c r="DK2" t="n">
-        <v>1.020117908225242e-295</v>
+        <v>5.620643995871633e-286</v>
       </c>
       <c r="DL2" t="n">
-        <v>3.353913096963402e-299</v>
+        <v>3.592899091022959e-289</v>
       </c>
       <c r="DM2" t="n">
-        <v>1.9079021611638e-302</v>
+        <v>1.643502448194804e-292</v>
       </c>
       <c r="DN2" t="n">
-        <v>0</v>
+        <v>6.820462331047236e-296</v>
       </c>
       <c r="DO2" t="n">
-        <v>0</v>
+        <v>4.170584735531864e-299</v>
       </c>
       <c r="DP2" t="n">
-        <v>0</v>
+        <v>2.365164541023265e-302</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0</v>
+        <v>1.90366187513251e-305</v>
       </c>
       <c r="DR2" t="n">
         <v>0</v>
@@ -15495,6 +15522,9 @@
         <v>0</v>
       </c>
       <c r="SF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="SG2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15508,412 +15538,412 @@
         <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3347730999449947</v>
+        <v>0.327885617810503</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3487807978433128</v>
+        <v>0.3458002504664768</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4023101361888788</v>
+        <v>0.3943551133879112</v>
       </c>
       <c r="F3" t="n">
-        <v>0.220295815350855</v>
+        <v>0.4879872348472923</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1971271018241854</v>
+        <v>0.4054012763950544</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5480534220147836</v>
+        <v>0.4788562394286533</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7285741153879662</v>
+        <v>0.7759229425904722</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3307490819469984</v>
+        <v>0.9224705375289627</v>
       </c>
       <c r="K3" t="n">
-        <v>0.6689353817365178</v>
+        <v>0.7651473950505274</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0381232465029433</v>
+        <v>0.9512635316275361</v>
       </c>
       <c r="M3" t="n">
-        <v>0.001237477563099213</v>
+        <v>0.5764633518958928</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0004549266056320915</v>
+        <v>0.2107593778305738</v>
       </c>
       <c r="O3" t="n">
-        <v>9.213498969754e-06</v>
+        <v>0.03647887357944728</v>
       </c>
       <c r="P3" t="n">
-        <v>2.070795852525252e-06</v>
+        <v>0.001932275650069587</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.901166491706687e-09</v>
+        <v>0.0005768907031645145</v>
       </c>
       <c r="R3" t="n">
-        <v>1.17814802297722e-09</v>
+        <v>3.714842216578469e-05</v>
       </c>
       <c r="S3" t="n">
-        <v>2.104689444942856e-09</v>
+        <v>9.471834488651051e-07</v>
       </c>
       <c r="T3" t="n">
-        <v>6.510958229812842e-13</v>
+        <v>1.273634333432807e-06</v>
       </c>
       <c r="U3" t="n">
-        <v>1.017394509658375e-13</v>
+        <v>1.149633499378786e-07</v>
       </c>
       <c r="V3" t="n">
-        <v>4.876522144306531e-17</v>
+        <v>2.820399734832495e-09</v>
       </c>
       <c r="W3" t="n">
-        <v>3.056179354321348e-18</v>
+        <v>7.642131975303347e-11</v>
       </c>
       <c r="X3" t="n">
-        <v>2.449944824191969e-17</v>
+        <v>2.104358706579529e-12</v>
       </c>
       <c r="Y3" t="n">
-        <v>1.012529258573575e-22</v>
+        <v>2.727292673673261e-12</v>
       </c>
       <c r="Z3" t="n">
-        <v>4.485143062788259e-25</v>
+        <v>2.408484368714808e-14</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.5998052991869e-27</v>
+        <v>5.093587894881834e-17</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.06038153882154e-29</v>
+        <v>7.241056667325636e-19</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.009284942321279e-31</v>
+        <v>3.050211930372963e-21</v>
       </c>
       <c r="AD3" t="n">
-        <v>6.507602429905332e-35</v>
+        <v>1.455047688322969e-23</v>
       </c>
       <c r="AE3" t="n">
-        <v>2.326704366374474e-37</v>
+        <v>5.04629933536169e-26</v>
       </c>
       <c r="AF3" t="n">
-        <v>2.30061713597767e-39</v>
+        <v>4.62587951838205e-28</v>
       </c>
       <c r="AG3" t="n">
-        <v>2.770998215891516e-42</v>
+        <v>1.022223026860448e-30</v>
       </c>
       <c r="AH3" t="n">
-        <v>1.110036773130879e-43</v>
+        <v>2.642552184227002e-32</v>
       </c>
       <c r="AI3" t="n">
-        <v>5.648477170160874e-45</v>
+        <v>1.874202076120459e-34</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.108119528625119e-49</v>
+        <v>4.155732664602428e-36</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.655425796207647e-51</v>
+        <v>1.561658766739161e-37</v>
       </c>
       <c r="AL3" t="n">
-        <v>2.048672099248567e-52</v>
+        <v>2.512874271080311e-39</v>
       </c>
       <c r="AM3" t="n">
-        <v>3.924654318026694e-53</v>
+        <v>2.896731972549231e-40</v>
       </c>
       <c r="AN3" t="n">
-        <v>3.084431386307886e-57</v>
+        <v>1.262347485932166e-41</v>
       </c>
       <c r="AO3" t="n">
-        <v>3.450874144757713e-60</v>
+        <v>1.250024146394366e-44</v>
       </c>
       <c r="AP3" t="n">
-        <v>1.227762365216286e-62</v>
+        <v>6.967764782884355e-47</v>
       </c>
       <c r="AQ3" t="n">
-        <v>1.270896691364435e-64</v>
+        <v>3.260522242269303e-49</v>
       </c>
       <c r="AR3" t="n">
-        <v>7.507359493956838e-67</v>
+        <v>9.968335997779824e-52</v>
       </c>
       <c r="AS3" t="n">
-        <v>5.126244351732382e-70</v>
+        <v>1.386354779577383e-53</v>
       </c>
       <c r="AT3" t="n">
-        <v>1.562462995013018e-72</v>
+        <v>4.166500261990701e-56</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.412018724221601e-74</v>
+        <v>2.213530396767181e-58</v>
       </c>
       <c r="AV3" t="n">
-        <v>4.703243554101796e-76</v>
+        <v>3.164455967328136e-60</v>
       </c>
       <c r="AW3" t="n">
-        <v>4.203330387067694e-78</v>
+        <v>1.492192806128458e-62</v>
       </c>
       <c r="AX3" t="n">
-        <v>2.931244049561936e-81</v>
+        <v>3.589068792283606e-64</v>
       </c>
       <c r="AY3" t="n">
-        <v>3.45116123427265e-83</v>
+        <v>2.838745642468455e-66</v>
       </c>
       <c r="AZ3" t="n">
-        <v>9.396214345634918e-86</v>
+        <v>1.381983135000831e-68</v>
       </c>
       <c r="BA3" t="n">
-        <v>3.693505056132215e-88</v>
+        <v>5.947784668326823e-71</v>
       </c>
       <c r="BB3" t="n">
-        <v>1.25671688343816e-90</v>
+        <v>3.040158183515843e-73</v>
       </c>
       <c r="BC3" t="n">
-        <v>1.856345267080499e-92</v>
+        <v>9.714526167067421e-76</v>
       </c>
       <c r="BD3" t="n">
-        <v>8.180388543635468e-95</v>
+        <v>4.101422939817453e-78</v>
       </c>
       <c r="BE3" t="n">
-        <v>7.161277453306006e-98</v>
+        <v>5.589751911951992e-80</v>
       </c>
       <c r="BF3" t="n">
-        <v>1.226404165943722e-99</v>
+        <v>1.330972212830238e-82</v>
       </c>
       <c r="BG3" t="n">
-        <v>4.171540832075322e-103</v>
+        <v>8.739540937513761e-85</v>
       </c>
       <c r="BH3" t="n">
-        <v>1.187335029613284e-105</v>
+        <v>9.340904953684714e-88</v>
       </c>
       <c r="BI3" t="n">
-        <v>1.258872798816957e-108</v>
+        <v>2.926115986622179e-90</v>
       </c>
       <c r="BJ3" t="n">
-        <v>1.884014780341103e-111</v>
+        <v>9.453733803957785e-93</v>
       </c>
       <c r="BK3" t="n">
-        <v>3.972892370953544e-114</v>
+        <v>1.079752372214212e-95</v>
       </c>
       <c r="BL3" t="n">
-        <v>1.172670380737244e-117</v>
+        <v>1.436458932574614e-98</v>
       </c>
       <c r="BM3" t="n">
-        <v>1.922156065710426e-120</v>
+        <v>2.312324450868011e-101</v>
       </c>
       <c r="BN3" t="n">
-        <v>3.554223779618809e-123</v>
+        <v>4.244842804453696e-104</v>
       </c>
       <c r="BO3" t="n">
-        <v>2.75922997183012e-126</v>
+        <v>2.552804257962827e-107</v>
       </c>
       <c r="BP3" t="n">
-        <v>1.047894414473256e-128</v>
+        <v>1.126847367787014e-109</v>
       </c>
       <c r="BQ3" t="n">
-        <v>9.13538214259533e-132</v>
+        <v>2.135170669153582e-112</v>
       </c>
       <c r="BR3" t="n">
-        <v>9.625659031523266e-135</v>
+        <v>3.767122073078351e-115</v>
       </c>
       <c r="BS3" t="n">
-        <v>4.787192870315953e-137</v>
+        <v>3.462138330252244e-118</v>
       </c>
       <c r="BT3" t="n">
-        <v>2.458707307973499e-139</v>
+        <v>3.848376429545151e-120</v>
       </c>
       <c r="BU3" t="n">
-        <v>3.000009492495257e-142</v>
+        <v>4.79765545849335e-123</v>
       </c>
       <c r="BV3" t="n">
-        <v>8.987245328080363e-145</v>
+        <v>7.478996672163857e-126</v>
       </c>
       <c r="BW3" t="n">
-        <v>1.552868181427783e-147</v>
+        <v>9.029779768103169e-129</v>
       </c>
       <c r="BX3" t="n">
-        <v>7.257184498759724e-150</v>
+        <v>2.056374240318799e-131</v>
       </c>
       <c r="BY3" t="n">
-        <v>3.010316266799833e-153</v>
+        <v>2.777995902053298e-133</v>
       </c>
       <c r="BZ3" t="n">
-        <v>5.597187180572344e-156</v>
+        <v>3.786273938096904e-136</v>
       </c>
       <c r="CA3" t="n">
-        <v>9.07210537110057e-159</v>
+        <v>5.051707657754018e-139</v>
       </c>
       <c r="CB3" t="n">
-        <v>1.531536272587352e-161</v>
+        <v>1.441029475969088e-141</v>
       </c>
       <c r="CC3" t="n">
-        <v>1.402557645979277e-164</v>
+        <v>1.4038614206813e-144</v>
       </c>
       <c r="CD3" t="n">
-        <v>4.003581108480205e-167</v>
+        <v>3.984738495679102e-147</v>
       </c>
       <c r="CE3" t="n">
-        <v>8.729202242148831e-170</v>
+        <v>4.468732740168959e-150</v>
       </c>
       <c r="CF3" t="n">
-        <v>1.702048659183331e-171</v>
+        <v>1.99774951906154e-152</v>
       </c>
       <c r="CG3" t="n">
-        <v>4.303417683263536e-175</v>
+        <v>4.653758665410819e-155</v>
       </c>
       <c r="CH3" t="n">
-        <v>3.117498095149417e-177</v>
+        <v>9.039787283555511e-158</v>
       </c>
       <c r="CI3" t="n">
-        <v>7.247882484143966e-180</v>
+        <v>5.333598879923594e-160</v>
       </c>
       <c r="CJ3" t="n">
-        <v>9.814151092246302e-183</v>
+        <v>4.939022697982675e-163</v>
       </c>
       <c r="CK3" t="n">
-        <v>9.576224936051629e-186</v>
+        <v>6.778214529155929e-166</v>
       </c>
       <c r="CL3" t="n">
-        <v>3.571075201568951e-189</v>
+        <v>4.774917216055685e-169</v>
       </c>
       <c r="CM3" t="n">
-        <v>9.245673010361075e-192</v>
+        <v>1.43413373585458e-171</v>
       </c>
       <c r="CN3" t="n">
-        <v>1.930174644172185e-194</v>
+        <v>1.225914648365171e-174</v>
       </c>
       <c r="CO3" t="n">
-        <v>1.760776745214765e-197</v>
+        <v>1.890145219269872e-177</v>
       </c>
       <c r="CP3" t="n">
-        <v>3.811040223491353e-200</v>
+        <v>2.31182098991998e-180</v>
       </c>
       <c r="CQ3" t="n">
-        <v>3.806442558771288e-202</v>
+        <v>5.646705671398009e-183</v>
       </c>
       <c r="CR3" t="n">
-        <v>1.942630942500464e-204</v>
+        <v>5.101670836482347e-185</v>
       </c>
       <c r="CS3" t="n">
-        <v>1.202185066994546e-207</v>
+        <v>1.884876221552207e-187</v>
       </c>
       <c r="CT3" t="n">
-        <v>1.6261018860204e-210</v>
+        <v>4.180278647039086e-190</v>
       </c>
       <c r="CU3" t="n">
-        <v>4.281263523401624e-213</v>
+        <v>9.424519057921695e-193</v>
       </c>
       <c r="CV3" t="n">
-        <v>3.533145932586071e-216</v>
+        <v>1.383322170467666e-195</v>
       </c>
       <c r="CW3" t="n">
-        <v>2.918866158830655e-219</v>
+        <v>1.345119668521655e-198</v>
       </c>
       <c r="CX3" t="n">
-        <v>7.230482462799681e-223</v>
+        <v>4.521368669206971e-202</v>
       </c>
       <c r="CY3" t="n">
-        <v>4.36999608226864e-226</v>
+        <v>3.5531800540029e-205</v>
       </c>
       <c r="CZ3" t="n">
-        <v>1.457087915818367e-228</v>
+        <v>1.289594554821995e-207</v>
       </c>
       <c r="DA3" t="n">
-        <v>1.612419727765966e-231</v>
+        <v>1.039900790106077e-210</v>
       </c>
       <c r="DB3" t="n">
-        <v>4.259472553416369e-234</v>
+        <v>2.530147001790062e-213</v>
       </c>
       <c r="DC3" t="n">
-        <v>3.937122798202396e-237</v>
+        <v>3.408384417468145e-216</v>
       </c>
       <c r="DD3" t="n">
-        <v>7.39415102430017e-240</v>
+        <v>1.701200497943949e-219</v>
       </c>
       <c r="DE3" t="n">
-        <v>1.032410688590381e-242</v>
+        <v>1.24932966666873e-221</v>
       </c>
       <c r="DF3" t="n">
-        <v>9.638493746439871e-246</v>
+        <v>1.207556542009989e-224</v>
       </c>
       <c r="DG3" t="n">
-        <v>1.887189242930257e-248</v>
+        <v>2.559955232229153e-227</v>
       </c>
       <c r="DH3" t="n">
-        <v>8.765119224288667e-252</v>
+        <v>1.426099634350969e-230</v>
       </c>
       <c r="DI3" t="n">
-        <v>1.356748628415236e-254</v>
+        <v>9.477010047172382e-234</v>
       </c>
       <c r="DJ3" t="n">
-        <v>3.492812514639693e-257</v>
+        <v>2.83412232296621e-236</v>
       </c>
       <c r="DK3" t="n">
-        <v>6.467066755424593e-260</v>
+        <v>3.210673891341249e-239</v>
       </c>
       <c r="DL3" t="n">
-        <v>2.092694605455837e-263</v>
+        <v>3.256037517581492e-242</v>
       </c>
       <c r="DM3" t="n">
-        <v>2.2672616475387e-266</v>
+        <v>3.107744568394687e-245</v>
       </c>
       <c r="DN3" t="n">
-        <v>3.643675229688036e-269</v>
+        <v>2.195850694465593e-248</v>
       </c>
       <c r="DO3" t="n">
-        <v>1.088577268008502e-272</v>
+        <v>2.035930002781598e-251</v>
       </c>
       <c r="DP3" t="n">
-        <v>2.499088651634405e-275</v>
+        <v>2.352172562223392e-254</v>
       </c>
       <c r="DQ3" t="n">
-        <v>3.551512197302196e-278</v>
+        <v>2.910767654682732e-257</v>
       </c>
       <c r="DR3" t="n">
-        <v>4.038728466683379e-281</v>
+        <v>7.954766567232817e-260</v>
       </c>
       <c r="DS3" t="n">
-        <v>7.946875614892771e-284</v>
+        <v>6.957780778526225e-263</v>
       </c>
       <c r="DT3" t="n">
-        <v>1.028817493514364e-286</v>
+        <v>2.782687740704523e-265</v>
       </c>
       <c r="DU3" t="n">
-        <v>4.499972024345346e-290</v>
+        <v>1.51622362223081e-268</v>
       </c>
       <c r="DV3" t="n">
-        <v>6.468876953657543e-293</v>
+        <v>1.807987634949266e-271</v>
       </c>
       <c r="DW3" t="n">
-        <v>7.317506821287701e-296</v>
+        <v>2.802134179017095e-274</v>
       </c>
       <c r="DX3" t="n">
-        <v>9.007409755117837e-299</v>
+        <v>2.443605361180025e-277</v>
       </c>
       <c r="DY3" t="n">
-        <v>3.495576878940115e-302</v>
+        <v>9.089088334425414e-281</v>
       </c>
       <c r="DZ3" t="n">
-        <v>1.372745663843555e-305</v>
+        <v>9.334295612432178e-284</v>
       </c>
       <c r="EA3" t="n">
-        <v>0</v>
+        <v>9.826180336094973e-287</v>
       </c>
       <c r="EB3" t="n">
-        <v>0</v>
+        <v>6.000493094402965e-290</v>
       </c>
       <c r="EC3" t="n">
-        <v>0</v>
+        <v>7.07106316874169e-293</v>
       </c>
       <c r="ED3" t="n">
-        <v>0</v>
+        <v>6.778437218129133e-296</v>
       </c>
       <c r="EE3" t="n">
-        <v>0</v>
+        <v>4.865557400667559e-298</v>
       </c>
       <c r="EF3" t="n">
-        <v>0</v>
+        <v>1.346603084280594e-300</v>
       </c>
       <c r="EG3" t="n">
-        <v>0</v>
+        <v>2.004704832119067e-303</v>
       </c>
       <c r="EH3" t="n">
-        <v>0</v>
+        <v>6.519348256947147e-307</v>
       </c>
       <c r="EI3" t="n">
         <v>0</v>
@@ -16999,6 +17029,9 @@
         <v>0</v>
       </c>
       <c r="SF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="SG3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17012,76 +17045,76 @@
         <v>0.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2975697650710996</v>
+        <v>0.3988854863901236</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2506093502060628</v>
+        <v>0.2971523707364307</v>
       </c>
       <c r="E4" t="n">
-        <v>0.355342502919242</v>
+        <v>0.223667536864964</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7570192315674326</v>
+        <v>0.3165607704925325</v>
       </c>
       <c r="G4" t="n">
-        <v>0.790184542074155</v>
+        <v>0.5134734097175349</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4209539068201664</v>
+        <v>0.4949728596707051</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2614769690731871</v>
+        <v>0.1870706946332449</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6691081735409615</v>
+        <v>0.06784617356423693</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3309811096693864</v>
+        <v>0.2336835391870474</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9618765741156619</v>
+        <v>0.04850225508655991</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9987625212623549</v>
+        <v>0.4235144842357362</v>
       </c>
       <c r="N4" t="n">
-        <v>0.9995450732645849</v>
+        <v>0.7892382168816392</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9999907865007404</v>
+        <v>0.9635210927636848</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9999979292041394</v>
+        <v>0.9980677240894021</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9999999910988335</v>
+        <v>0.9994231092883384</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9999999988218519</v>
+        <v>0.9999628515776791</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9999999978953106</v>
+        <v>0.9999990528165505</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9999999999993489</v>
+        <v>0.9999987263656666</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9999999999998983</v>
+        <v>0.99999988503665</v>
       </c>
       <c r="V4" t="n">
-        <v>1</v>
+        <v>0.9999999971796002</v>
       </c>
       <c r="W4" t="n">
-        <v>1</v>
+        <v>0.9999999999235786</v>
       </c>
       <c r="X4" t="n">
-        <v>1</v>
+        <v>0.9999999999978956</v>
       </c>
       <c r="Y4" t="n">
-        <v>1</v>
+        <v>0.9999999999972726</v>
       </c>
       <c r="Z4" t="n">
-        <v>1</v>
+        <v>0.9999999999999758</v>
       </c>
       <c r="AA4" t="n">
         <v>1</v>
@@ -18503,6 +18536,9 @@
         <v>1</v>
       </c>
       <c r="SF4" t="n">
+        <v>1</v>
+      </c>
+      <c r="SG4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new fake mus to match new rates and 10 simulations matching sectors for test 3
</commit_message>
<xml_diff>
--- a/Data/fake_nocalib.xlsx
+++ b/Data/fake_nocalib.xlsx
@@ -1944,73 +1944,73 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3400000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4204531193381447</v>
+        <v>0.3793476846011162</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5629962637107235</v>
+        <v>0.2443382457136077</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7181255052401537</v>
+        <v>0.4095524216894881</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7353792558244767</v>
+        <v>0.6635434669992045</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6634561158807928</v>
+        <v>0.8677242659820423</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6785936953210321</v>
+        <v>0.9571203441474139</v>
       </c>
       <c r="I2" t="n">
-        <v>0.244192668384428</v>
+        <v>0.9762388172196976</v>
       </c>
       <c r="J2" t="n">
-        <v>0.454617067444382</v>
+        <v>0.9807121798149688</v>
       </c>
       <c r="K2" t="n">
-        <v>0.720027980070397</v>
+        <v>0.9818872557099124</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9721146405848189</v>
+        <v>0.996658946601905</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9984818907044347</v>
+        <v>0.9988826873923726</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9997485057136849</v>
+        <v>0.9999836269568585</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9999407806356677</v>
+        <v>0.9999975313527698</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9999992180687854</v>
+        <v>0.9999996380446543</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9999999354073765</v>
+        <v>0.9999999888121439</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9999999952658166</v>
+        <v>0.9999999997141267</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9999999995918449</v>
+        <v>0.9999999999693473</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9999999999921714</v>
+        <v>0.9999999999897953</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9999999999999588</v>
+        <v>0.999999999999273</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9999999999999978</v>
+        <v>0.9999999999999754</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>0.9999999999999989</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="Y2" t="n">
         <v>1</v>
@@ -3454,412 +3454,412 @@
         <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3231932765123403</v>
+        <v>0.3296342073030863</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2862255244832053</v>
+        <v>0.3214936029049453</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2151322014019616</v>
+        <v>0.3280990912466611</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2303956107036899</v>
+        <v>0.2401513653268916</v>
       </c>
       <c r="G3" t="n">
-        <v>0.314840728894836</v>
+        <v>0.1220483975709383</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3138150297263795</v>
+        <v>0.04169547107543006</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7417530179368523</v>
+        <v>0.0235910464715743</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5445840352473456</v>
+        <v>0.0192529375272495</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2799000403588172</v>
+        <v>0.0181081705752914</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0278852300564981</v>
+        <v>0.003340920995463079</v>
       </c>
       <c r="M3" t="n">
-        <v>0.00151810744441949</v>
+        <v>0.001117300590388375</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0002514941984627928</v>
+        <v>1.637302197906345e-05</v>
       </c>
       <c r="O3" t="n">
-        <v>5.921936358610329e-05</v>
+        <v>2.468646314439176e-06</v>
       </c>
       <c r="P3" t="n">
-        <v>7.819312119487251e-07</v>
+        <v>3.619553220963576e-07</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.459262348630573e-08</v>
+        <v>1.118785610012044e-08</v>
       </c>
       <c r="R3" t="n">
-        <v>4.734183328161191e-09</v>
+        <v>2.858733826074507e-10</v>
       </c>
       <c r="S3" t="n">
-        <v>4.081550887759506e-10</v>
+        <v>3.065273871913303e-11</v>
       </c>
       <c r="T3" t="n">
-        <v>7.82862613173115e-12</v>
+        <v>1.020475990134383e-11</v>
       </c>
       <c r="U3" t="n">
-        <v>4.123440139089813e-14</v>
+        <v>7.269509111457317e-13</v>
       </c>
       <c r="V3" t="n">
-        <v>2.208922167862435e-15</v>
+        <v>2.465675334814873e-14</v>
       </c>
       <c r="W3" t="n">
-        <v>1.282976316709989e-17</v>
+        <v>1.062939060395602e-15</v>
       </c>
       <c r="X3" t="n">
-        <v>1.368673611229222e-19</v>
+        <v>6.644673182821444e-17</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.537509886178239e-21</v>
+        <v>2.520931580206053e-18</v>
       </c>
       <c r="Z3" t="n">
-        <v>8.209096527001162e-23</v>
+        <v>1.297266635876832e-20</v>
       </c>
       <c r="AA3" t="n">
-        <v>8.645180296812349e-25</v>
+        <v>4.396779080261565e-22</v>
       </c>
       <c r="AB3" t="n">
-        <v>3.735173437339378e-26</v>
+        <v>6.124532202742192e-24</v>
       </c>
       <c r="AC3" t="n">
-        <v>2.733229669308026e-28</v>
+        <v>3.151967707531632e-25</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.293333334420333e-30</v>
+        <v>9.263358699584408e-27</v>
       </c>
       <c r="AE3" t="n">
-        <v>8.172600918564627e-33</v>
+        <v>2.068301886086068e-29</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.78361040953903e-34</v>
+        <v>6.486970928810728e-31</v>
       </c>
       <c r="AG3" t="n">
-        <v>8.806497684535654e-37</v>
+        <v>3.933648137379379e-33</v>
       </c>
       <c r="AH3" t="n">
-        <v>3.528733669652618e-39</v>
+        <v>3.031273873584111e-35</v>
       </c>
       <c r="AI3" t="n">
-        <v>3.551414897126198e-41</v>
+        <v>5.507542086270659e-37</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.845539572553126e-43</v>
+        <v>2.274624694623524e-39</v>
       </c>
       <c r="AK3" t="n">
-        <v>2.650369239295483e-45</v>
+        <v>6.154109012305736e-41</v>
       </c>
       <c r="AL3" t="n">
-        <v>1.568473467610158e-46</v>
+        <v>1.003727369831053e-42</v>
       </c>
       <c r="AM3" t="n">
-        <v>4.322348666271413e-48</v>
+        <v>2.718431951714819e-44</v>
       </c>
       <c r="AN3" t="n">
-        <v>1.998146904888979e-50</v>
+        <v>4.813886081518068e-46</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.001084982287456e-52</v>
+        <v>9.178677434698341e-49</v>
       </c>
       <c r="AP3" t="n">
-        <v>8.967916306300224e-55</v>
+        <v>5.449626853517709e-51</v>
       </c>
       <c r="AQ3" t="n">
-        <v>8.35991108793775e-58</v>
+        <v>8.20595186809358e-53</v>
       </c>
       <c r="AR3" t="n">
-        <v>1.323688413880276e-60</v>
+        <v>3.835679834072938e-55</v>
       </c>
       <c r="AS3" t="n">
-        <v>6.94524699348581e-63</v>
+        <v>3.234895888913618e-57</v>
       </c>
       <c r="AT3" t="n">
-        <v>6.485154789932017e-65</v>
+        <v>1.187025698392477e-60</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.132523146676326e-66</v>
+        <v>2.615360518692618e-63</v>
       </c>
       <c r="AV3" t="n">
-        <v>4.135364124334432e-69</v>
+        <v>2.076181926814557e-65</v>
       </c>
       <c r="AW3" t="n">
-        <v>1.888953572971093e-71</v>
+        <v>1.035154921040368e-67</v>
       </c>
       <c r="AX3" t="n">
-        <v>3.155002739253613e-72</v>
+        <v>1.212833259527395e-69</v>
       </c>
       <c r="AY3" t="n">
-        <v>2.15594899571307e-74</v>
+        <v>2.629894751960169e-71</v>
       </c>
       <c r="AZ3" t="n">
-        <v>7.200430506691081e-77</v>
+        <v>9.03232060590459e-74</v>
       </c>
       <c r="BA3" t="n">
-        <v>4.355544394930296e-79</v>
+        <v>6.127576116742845e-76</v>
       </c>
       <c r="BB3" t="n">
-        <v>1.231977946848314e-81</v>
+        <v>2.59490365776871e-78</v>
       </c>
       <c r="BC3" t="n">
-        <v>5.733656429185987e-84</v>
+        <v>1.264538222878302e-80</v>
       </c>
       <c r="BD3" t="n">
-        <v>2.300102378911595e-86</v>
+        <v>7.71869210033123e-83</v>
       </c>
       <c r="BE3" t="n">
-        <v>7.285723422891193e-89</v>
+        <v>7.956241909484133e-85</v>
       </c>
       <c r="BF3" t="n">
-        <v>6.941279378485098e-92</v>
+        <v>1.063136796035789e-87</v>
       </c>
       <c r="BG3" t="n">
-        <v>1.083419960604083e-93</v>
+        <v>3.583682309043511e-90</v>
       </c>
       <c r="BH3" t="n">
-        <v>1.436142765577422e-95</v>
+        <v>2.908896322153387e-93</v>
       </c>
       <c r="BI3" t="n">
-        <v>3.486778000871525e-98</v>
+        <v>2.645129056339503e-96</v>
       </c>
       <c r="BJ3" t="n">
-        <v>1.429008791055144e-100</v>
+        <v>5.38581463183456e-99</v>
       </c>
       <c r="BK3" t="n">
-        <v>2.360220845450451e-103</v>
+        <v>1.179563186519831e-101</v>
       </c>
       <c r="BL3" t="n">
-        <v>9.929566525307267e-106</v>
+        <v>1.453516746796217e-103</v>
       </c>
       <c r="BM3" t="n">
-        <v>2.065100316914139e-108</v>
+        <v>2.355633655299669e-105</v>
       </c>
       <c r="BN3" t="n">
-        <v>2.164521746161432e-110</v>
+        <v>4.551495678445881e-108</v>
       </c>
       <c r="BO3" t="n">
-        <v>3.754279788713721e-113</v>
+        <v>8.566009224309254e-111</v>
       </c>
       <c r="BP3" t="n">
-        <v>2.062936492925158e-116</v>
+        <v>3.316515953792697e-113</v>
       </c>
       <c r="BQ3" t="n">
-        <v>5.701455711544083e-119</v>
+        <v>1.569670905295456e-115</v>
       </c>
       <c r="BR3" t="n">
-        <v>2.966293183778675e-121</v>
+        <v>8.426312649475215e-118</v>
       </c>
       <c r="BS3" t="n">
-        <v>9.545462129556182e-124</v>
+        <v>3.167625832011999e-120</v>
       </c>
       <c r="BT3" t="n">
-        <v>3.460507018349236e-126</v>
+        <v>2.580271855207091e-123</v>
       </c>
       <c r="BU3" t="n">
-        <v>1.633430866533558e-128</v>
+        <v>3.66723778858186e-125</v>
       </c>
       <c r="BV3" t="n">
-        <v>3.648468406062058e-131</v>
+        <v>6.3111680146318e-127</v>
       </c>
       <c r="BW3" t="n">
-        <v>9.736710488133254e-134</v>
+        <v>1.03789910889218e-129</v>
       </c>
       <c r="BX3" t="n">
-        <v>1.697406253819052e-136</v>
+        <v>2.006964115787512e-132</v>
       </c>
       <c r="BY3" t="n">
-        <v>2.017868414854885e-139</v>
+        <v>1.162337655114935e-134</v>
       </c>
       <c r="BZ3" t="n">
-        <v>1.109838387622664e-141</v>
+        <v>2.921839297535298e-137</v>
       </c>
       <c r="CA3" t="n">
-        <v>9.83941222376737e-145</v>
+        <v>1.050788414802883e-139</v>
       </c>
       <c r="CB3" t="n">
-        <v>2.545052624705583e-147</v>
+        <v>3.475277884235044e-142</v>
       </c>
       <c r="CC3" t="n">
-        <v>3.789465879669885e-150</v>
+        <v>1.955756862480445e-144</v>
       </c>
       <c r="CD3" t="n">
-        <v>5.400217330243092e-153</v>
+        <v>1.145645820147438e-146</v>
       </c>
       <c r="CE3" t="n">
-        <v>1.020728191081044e-155</v>
+        <v>9.468539978473212e-149</v>
       </c>
       <c r="CF3" t="n">
-        <v>6.119703929619499e-159</v>
+        <v>1.37613766624853e-151</v>
       </c>
       <c r="CG3" t="n">
-        <v>9.290061487525068e-162</v>
+        <v>2.059994325789272e-154</v>
       </c>
       <c r="CH3" t="n">
-        <v>1.389278573541469e-164</v>
+        <v>3.080055979023925e-157</v>
       </c>
       <c r="CI3" t="n">
-        <v>3.018426688383909e-167</v>
+        <v>1.074209948838355e-159</v>
       </c>
       <c r="CJ3" t="n">
-        <v>1.544902461056762e-169</v>
+        <v>3.737270064115036e-162</v>
       </c>
       <c r="CK3" t="n">
-        <v>1.649573484296101e-172</v>
+        <v>2.356765990164629e-164</v>
       </c>
       <c r="CL3" t="n">
-        <v>1.239428902511692e-175</v>
+        <v>5.601475385343265e-167</v>
       </c>
       <c r="CM3" t="n">
-        <v>7.282688237073656e-178</v>
+        <v>2.476541497654852e-169</v>
       </c>
       <c r="CN3" t="n">
-        <v>1.233216867888955e-180</v>
+        <v>3.708856347554187e-172</v>
       </c>
       <c r="CO3" t="n">
-        <v>4.226822397837822e-183</v>
+        <v>4.874052877048397e-175</v>
       </c>
       <c r="CP3" t="n">
-        <v>1.158467395524725e-185</v>
+        <v>4.420360412564045e-178</v>
       </c>
       <c r="CQ3" t="n">
-        <v>8.111634033141904e-188</v>
+        <v>1.015398811900328e-180</v>
       </c>
       <c r="CR3" t="n">
-        <v>1.082752384146899e-190</v>
+        <v>1.967651738616531e-183</v>
       </c>
       <c r="CS3" t="n">
-        <v>3.04002607063479e-193</v>
+        <v>4.199827959280762e-186</v>
       </c>
       <c r="CT3" t="n">
-        <v>3.35179886341235e-196</v>
+        <v>5.902052327130323e-189</v>
       </c>
       <c r="CU3" t="n">
-        <v>2.861814717674259e-199</v>
+        <v>2.234507089248548e-191</v>
       </c>
       <c r="CV3" t="n">
-        <v>2.618498316119997e-202</v>
+        <v>3.697412300075998e-194</v>
       </c>
       <c r="CW3" t="n">
-        <v>5.756701258431772e-205</v>
+        <v>7.039511272337362e-197</v>
       </c>
       <c r="CX3" t="n">
-        <v>8.161322331772085e-208</v>
+        <v>7.726470825086164e-200</v>
       </c>
       <c r="CY3" t="n">
-        <v>2.69994902355047e-210</v>
+        <v>2.151620053319313e-202</v>
       </c>
       <c r="CZ3" t="n">
-        <v>3.977747956546883e-213</v>
+        <v>1.654916868437297e-205</v>
       </c>
       <c r="DA3" t="n">
-        <v>2.646361419343663e-216</v>
+        <v>1.527338356625677e-208</v>
       </c>
       <c r="DB3" t="n">
-        <v>2.154474899975639e-219</v>
+        <v>1.731412047493001e-211</v>
       </c>
       <c r="DC3" t="n">
-        <v>2.426296952624667e-222</v>
+        <v>1.966266242998464e-214</v>
       </c>
       <c r="DD3" t="n">
-        <v>8.671071930744764e-225</v>
+        <v>2.668812108121044e-217</v>
       </c>
       <c r="DE3" t="n">
-        <v>4.721761411161403e-226</v>
+        <v>4.496418066993332e-220</v>
       </c>
       <c r="DF3" t="n">
-        <v>6.234361033281678e-229</v>
+        <v>1.880938801269126e-223</v>
       </c>
       <c r="DG3" t="n">
-        <v>3.850082666254173e-232</v>
+        <v>6.957876432928298e-226</v>
       </c>
       <c r="DH3" t="n">
-        <v>6.085885084523206e-235</v>
+        <v>1.15435353881347e-228</v>
       </c>
       <c r="DI3" t="n">
-        <v>9.688910059125909e-238</v>
+        <v>1.399054055317152e-231</v>
       </c>
       <c r="DJ3" t="n">
-        <v>2.121238798306453e-240</v>
+        <v>1.132308441187853e-234</v>
       </c>
       <c r="DK3" t="n">
-        <v>1.223172945752218e-243</v>
+        <v>1.605326867785111e-237</v>
       </c>
       <c r="DL3" t="n">
-        <v>3.186345018273024e-246</v>
+        <v>5.163779547941914e-240</v>
       </c>
       <c r="DM3" t="n">
-        <v>2.986411475610899e-249</v>
+        <v>5.244825610201538e-243</v>
       </c>
       <c r="DN3" t="n">
-        <v>6.397579923031843e-252</v>
+        <v>1.11341600576241e-245</v>
       </c>
       <c r="DO3" t="n">
-        <v>4.594486726873716e-255</v>
+        <v>4.814933658750475e-248</v>
       </c>
       <c r="DP3" t="n">
-        <v>3.08900599329973e-258</v>
+        <v>8.341310293478246e-251</v>
       </c>
       <c r="DQ3" t="n">
-        <v>2.182917711259896e-261</v>
+        <v>5.672208180152159e-254</v>
       </c>
       <c r="DR3" t="n">
-        <v>3.4977614158307e-264</v>
+        <v>3.382990806315404e-257</v>
       </c>
       <c r="DS3" t="n">
-        <v>9.472673393156493e-267</v>
+        <v>2.247958680111657e-260</v>
       </c>
       <c r="DT3" t="n">
-        <v>8.369157153832356e-270</v>
+        <v>1.597581536725054e-263</v>
       </c>
       <c r="DU3" t="n">
-        <v>5.419134085796373e-273</v>
+        <v>2.832188042282474e-266</v>
       </c>
       <c r="DV3" t="n">
-        <v>5.723154436853306e-276</v>
+        <v>1.285180611913135e-269</v>
       </c>
       <c r="DW3" t="n">
-        <v>1.218052859427839e-278</v>
+        <v>5.834652141737865e-272</v>
       </c>
       <c r="DX3" t="n">
-        <v>9.984567541440087e-282</v>
+        <v>2.429031838470496e-275</v>
       </c>
       <c r="DY3" t="n">
-        <v>9.773571585562611e-285</v>
+        <v>3.47442820843071e-278</v>
       </c>
       <c r="DZ3" t="n">
-        <v>7.007896300844706e-288</v>
+        <v>8.899497899751342e-281</v>
       </c>
       <c r="EA3" t="n">
-        <v>4.89641512129886e-291</v>
+        <v>8.387398452567341e-284</v>
       </c>
       <c r="EB3" t="n">
-        <v>1.927869326669561e-293</v>
+        <v>5.114260369772167e-287</v>
       </c>
       <c r="EC3" t="n">
-        <v>2.119235103382775e-296</v>
+        <v>6.838337296065189e-290</v>
       </c>
       <c r="ED3" t="n">
-        <v>8.310466174206517e-299</v>
+        <v>4.725897561815482e-293</v>
       </c>
       <c r="EE3" t="n">
-        <v>7.283824512438452e-302</v>
+        <v>3.872354068427063e-296</v>
       </c>
       <c r="EF3" t="n">
-        <v>4.137317069518141e-305</v>
+        <v>3.956039584689241e-299</v>
       </c>
       <c r="EG3" t="n">
-        <v>0</v>
+        <v>2.433203239533613e-302</v>
       </c>
       <c r="EH3" t="n">
-        <v>0</v>
+        <v>2.086398602478703e-305</v>
       </c>
       <c r="EI3" t="n">
         <v>0</v>
@@ -4961,358 +4961,358 @@
         <v>0.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.256353604149515</v>
+        <v>0.2910181080957974</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1507782118060711</v>
+        <v>0.4341681513814472</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06674229335788452</v>
+        <v>0.2623484870638508</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03422513347183336</v>
+        <v>0.09630516767390387</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02170315522437116</v>
+        <v>0.01022733644701928</v>
       </c>
       <c r="H4" t="n">
-        <v>0.007591274952588354</v>
+        <v>0.001184184777156025</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01405431367871977</v>
+        <v>0.0001701363087279929</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0007988973082724498</v>
+        <v>3.488265778167575e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>7.197957078569808e-05</v>
+        <v>4.573714796075296e-06</v>
       </c>
       <c r="L4" t="n">
-        <v>1.293586830273262e-07</v>
+        <v>1.324026319897256e-07</v>
       </c>
       <c r="M4" t="n">
-        <v>1.851145820024733e-09</v>
+        <v>1.201723901533555e-08</v>
       </c>
       <c r="N4" t="n">
-        <v>8.785225634490864e-11</v>
+        <v>2.1162533247175e-11</v>
       </c>
       <c r="O4" t="n">
-        <v>7.462552365327504e-13</v>
+        <v>9.158427493097828e-13</v>
       </c>
       <c r="P4" t="n">
-        <v>2.552966996833278e-15</v>
+        <v>2.359140804809958e-14</v>
       </c>
       <c r="Q4" t="n">
-        <v>4.53565169696821e-17</v>
+        <v>1.972630577103956e-17</v>
       </c>
       <c r="R4" t="n">
-        <v>8.991790933644894e-19</v>
+        <v>8.035036170079241e-20</v>
       </c>
       <c r="S4" t="n">
-        <v>1.267831093961639e-20</v>
+        <v>1.68319929423848e-21</v>
       </c>
       <c r="T4" t="n">
-        <v>5.074810462491077e-23</v>
+        <v>5.246018683308309e-23</v>
       </c>
       <c r="U4" t="n">
-        <v>7.465837289856729e-26</v>
+        <v>8.94300705166614e-25</v>
       </c>
       <c r="V4" t="n">
-        <v>6.842204988639893e-28</v>
+        <v>8.166563970103888e-27</v>
       </c>
       <c r="W4" t="n">
-        <v>1.003861747773716e-30</v>
+        <v>6.718720282941334e-29</v>
       </c>
       <c r="X4" t="n">
-        <v>3.274118933796584e-33</v>
+        <v>6.667886547680513e-31</v>
       </c>
       <c r="Y4" t="n">
-        <v>9.958024035456358e-36</v>
+        <v>2.74882434558528e-33</v>
       </c>
       <c r="Z4" t="n">
-        <v>6.384661027688728e-38</v>
+        <v>4.379336774327872e-36</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.68222640900028e-40</v>
+        <v>1.558019271311049e-38</v>
       </c>
       <c r="AB4" t="n">
-        <v>1.861505245999103e-42</v>
+        <v>9.152232055572501e-41</v>
       </c>
       <c r="AC4" t="n">
-        <v>4.223535094532186e-45</v>
+        <v>6.319174066535789e-43</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.162172777263558e-47</v>
+        <v>7.062283647913324e-45</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.581619011069234e-50</v>
+        <v>7.549658774148404e-48</v>
       </c>
       <c r="AF4" t="n">
-        <v>7.940247489624705e-53</v>
+        <v>5.846101968866361e-50</v>
       </c>
       <c r="AG4" t="n">
-        <v>2.045492919934869e-55</v>
+        <v>1.556655103666182e-52</v>
       </c>
       <c r="AH4" t="n">
-        <v>2.848384345847496e-58</v>
+        <v>3.361255176871854e-55</v>
       </c>
       <c r="AI4" t="n">
-        <v>9.417155315531184e-61</v>
+        <v>1.753465999620108e-57</v>
       </c>
       <c r="AJ4" t="n">
-        <v>1.55026341011521e-63</v>
+        <v>2.910862206830405e-60</v>
       </c>
       <c r="AK4" t="n">
-        <v>9.087953013607001e-66</v>
+        <v>1.674440719998849e-62</v>
       </c>
       <c r="AL4" t="n">
-        <v>9.593843638430837e-68</v>
+        <v>6.503503789131282e-65</v>
       </c>
       <c r="AM4" t="n">
-        <v>5.40276613173805e-70</v>
+        <v>4.035877157571222e-67</v>
       </c>
       <c r="AN4" t="n">
-        <v>8.457403605425062e-73</v>
+        <v>1.770431944368552e-69</v>
       </c>
       <c r="AO4" t="n">
-        <v>1.342498596565131e-75</v>
+        <v>1.671863692828231e-72</v>
       </c>
       <c r="AP4" t="n">
-        <v>3.584252498921526e-78</v>
+        <v>2.943874003160284e-75</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.436286471404693e-81</v>
+        <v>1.614987983618917e-77</v>
       </c>
       <c r="AR4" t="n">
-        <v>2.361220514559712e-84</v>
+        <v>2.502968187465843e-80</v>
       </c>
       <c r="AS4" t="n">
-        <v>4.165235010048621e-87</v>
+        <v>6.664666904912363e-83</v>
       </c>
       <c r="AT4" t="n">
-        <v>1.002221547314689e-89</v>
+        <v>3.14987528658118e-86</v>
       </c>
       <c r="AU4" t="n">
-        <v>5.32568790451684e-92</v>
+        <v>3.31871534270077e-89</v>
       </c>
       <c r="AV4" t="n">
-        <v>7.816831861167795e-95</v>
+        <v>7.065934777287236e-92</v>
       </c>
       <c r="AW4" t="n">
-        <v>1.169698260549334e-97</v>
+        <v>1.089961266820835e-94</v>
       </c>
       <c r="AX4" t="n">
-        <v>3.996138233777963e-99</v>
+        <v>3.795728253158791e-97</v>
       </c>
       <c r="AY4" t="n">
-        <v>8.35106108202985e-102</v>
+        <v>1.76363593056806e-99</v>
       </c>
       <c r="AZ4" t="n">
-        <v>1.211285242342639e-104</v>
+        <v>2.841816520387164e-102</v>
       </c>
       <c r="BA4" t="n">
-        <v>2.417356518814763e-107</v>
+        <v>6.678466729927062e-105</v>
       </c>
       <c r="BB4" t="n">
-        <v>2.657657370461082e-110</v>
+        <v>1.007845355031097e-107</v>
       </c>
       <c r="BC4" t="n">
-        <v>4.585232555345257e-113</v>
+        <v>2.025845879238848e-110</v>
       </c>
       <c r="BD4" t="n">
-        <v>7.752857121028684e-116</v>
+        <v>3.522549679423013e-113</v>
       </c>
       <c r="BE4" t="n">
-        <v>9.46706459057224e-119</v>
+        <v>1.123682374063724e-115</v>
       </c>
       <c r="BF4" t="n">
-        <v>6.487153800606464e-122</v>
+        <v>8.412813872536072e-119</v>
       </c>
       <c r="BG4" t="n">
-        <v>2.627835884149546e-124</v>
+        <v>9.811927896197844e-122</v>
       </c>
       <c r="BH4" t="n">
-        <v>1.021936556736778e-126</v>
+        <v>5.612100424223407e-125</v>
       </c>
       <c r="BI4" t="n">
-        <v>1.528360940476105e-129</v>
+        <v>4.570073028816219e-128</v>
       </c>
       <c r="BJ4" t="n">
-        <v>2.028640123671117e-132</v>
+        <v>3.913683570550743e-131</v>
       </c>
       <c r="BK4" t="n">
-        <v>1.944508376844312e-135</v>
+        <v>5.494468049361286e-134</v>
       </c>
       <c r="BL4" t="n">
-        <v>3.54621353024024e-138</v>
+        <v>2.210469460073515e-136</v>
       </c>
       <c r="BM4" t="n">
-        <v>3.577737192292854e-141</v>
+        <v>1.127639088953914e-138</v>
       </c>
       <c r="BN4" t="n">
-        <v>1.785768207231026e-143</v>
+        <v>9.406758146462197e-142</v>
       </c>
       <c r="BO4" t="n">
-        <v>1.451834427262673e-146</v>
+        <v>8.495379419321814e-145</v>
       </c>
       <c r="BP4" t="n">
-        <v>7.179239155717839e-150</v>
+        <v>1.046467574119693e-147</v>
       </c>
       <c r="BQ4" t="n">
-        <v>8.040239235048001e-153</v>
+        <v>2.767898651137675e-150</v>
       </c>
       <c r="BR4" t="n">
-        <v>1.394180549853944e-155</v>
+        <v>4.27965372219424e-153</v>
       </c>
       <c r="BS4" t="n">
-        <v>1.51295539451959e-158</v>
+        <v>5.378867727922191e-156</v>
       </c>
       <c r="BT4" t="n">
-        <v>1.965612126583086e-161</v>
+        <v>2.8592130689566e-159</v>
       </c>
       <c r="BU4" t="n">
-        <v>2.773733604064349e-164</v>
+        <v>9.794650465048489e-162</v>
       </c>
       <c r="BV4" t="n">
-        <v>2.901199788305986e-167</v>
+        <v>3.974024412726013e-164</v>
       </c>
       <c r="BW4" t="n">
-        <v>3.092418832732052e-170</v>
+        <v>2.831765004077773e-167</v>
       </c>
       <c r="BX4" t="n">
-        <v>2.873291305673903e-173</v>
+        <v>2.179791889978291e-170</v>
       </c>
       <c r="BY4" t="n">
-        <v>1.789000208805206e-176</v>
+        <v>3.60354379909673e-173</v>
       </c>
       <c r="BZ4" t="n">
-        <v>4.50914064468463e-179</v>
+        <v>3.419565227069598e-176</v>
       </c>
       <c r="CA4" t="n">
-        <v>2.626422091865968e-182</v>
+        <v>5.754876036105853e-179</v>
       </c>
       <c r="CB4" t="n">
-        <v>2.981559357222825e-185</v>
+        <v>6.297444139975329e-182</v>
       </c>
       <c r="CC4" t="n">
-        <v>2.011964206699953e-188</v>
+        <v>1.303517518877018e-184</v>
       </c>
       <c r="CD4" t="n">
-        <v>1.506892153943804e-191</v>
+        <v>2.123854039453688e-187</v>
       </c>
       <c r="CE4" t="n">
-        <v>1.862690257122632e-194</v>
+        <v>4.615384621893259e-190</v>
       </c>
       <c r="CF4" t="n">
-        <v>8.084639132649444e-198</v>
+        <v>2.989263056337442e-193</v>
       </c>
       <c r="CG4" t="n">
-        <v>5.239379982384315e-201</v>
+        <v>2.018360515793767e-196</v>
       </c>
       <c r="CH4" t="n">
-        <v>3.348892900955869e-204</v>
+        <v>1.288088565106835e-199</v>
       </c>
       <c r="CI4" t="n">
-        <v>5.292158879840529e-207</v>
+        <v>1.428208210687579e-202</v>
       </c>
       <c r="CJ4" t="n">
-        <v>8.54736883973549e-210</v>
+        <v>1.677606321366678e-205</v>
       </c>
       <c r="CK4" t="n">
-        <v>4.50531694617805e-213</v>
+        <v>4.185596368516794e-208</v>
       </c>
       <c r="CL4" t="n">
-        <v>2.076990875527825e-216</v>
+        <v>3.505928005651271e-211</v>
       </c>
       <c r="CM4" t="n">
-        <v>5.390700144018678e-219</v>
+        <v>6.515925194768374e-214</v>
       </c>
       <c r="CN4" t="n">
-        <v>3.842966667280099e-222</v>
+        <v>4.996596719488723e-217</v>
       </c>
       <c r="CO4" t="n">
-        <v>5.203757634805211e-225</v>
+        <v>2.924442573316592e-220</v>
       </c>
       <c r="CP4" t="n">
-        <v>4.824135981945217e-228</v>
+        <v>1.387726974057733e-223</v>
       </c>
       <c r="CQ4" t="n">
-        <v>1.212371419303675e-230</v>
+        <v>1.389459324730104e-226</v>
       </c>
       <c r="CR4" t="n">
-        <v>7.439436366918048e-234</v>
+        <v>1.012638689859469e-229</v>
       </c>
       <c r="CS4" t="n">
-        <v>1.03260464226071e-236</v>
+        <v>1.012901352903687e-232</v>
       </c>
       <c r="CT4" t="n">
-        <v>6.073038811201116e-240</v>
+        <v>7.682682980060789e-236</v>
       </c>
       <c r="CU4" t="n">
-        <v>3.003909717191947e-243</v>
+        <v>1.158886994839584e-238</v>
       </c>
       <c r="CV4" t="n">
-        <v>1.620913967207032e-246</v>
+        <v>8.847872588336288e-242</v>
       </c>
       <c r="CW4" t="n">
-        <v>1.348511731663008e-249</v>
+        <v>6.753118531143666e-245</v>
       </c>
       <c r="CX4" t="n">
-        <v>8.096856571938103e-253</v>
+        <v>3.683030423345442e-248</v>
       </c>
       <c r="CY4" t="n">
-        <v>1.57728688685453e-255</v>
+        <v>4.672224316432154e-251</v>
       </c>
       <c r="CZ4" t="n">
-        <v>1.234361760273162e-258</v>
+        <v>1.994760272877952e-254</v>
       </c>
       <c r="DA4" t="n">
-        <v>4.938588001378184e-262</v>
+        <v>9.265281398669763e-258</v>
       </c>
       <c r="DB4" t="n">
-        <v>2.191939935138384e-265</v>
+        <v>7.670556413778959e-261</v>
       </c>
       <c r="DC4" t="n">
-        <v>1.0959416957832e-268</v>
+        <v>3.946028003768054e-264</v>
       </c>
       <c r="DD4" t="n">
-        <v>1.614891576763922e-271</v>
+        <v>2.928208494721857e-267</v>
       </c>
       <c r="DE4" t="n">
-        <v>2.929986815596866e-273</v>
+        <v>1.871474431611791e-270</v>
       </c>
       <c r="DF4" t="n">
-        <v>1.704535370373279e-276</v>
+        <v>7.978617885234363e-274</v>
       </c>
       <c r="DG4" t="n">
-        <v>6.416723795986421e-280</v>
+        <v>9.053910662227748e-277</v>
       </c>
       <c r="DH4" t="n">
-        <v>6.650762384716971e-283</v>
+        <v>8.289159263251626e-280</v>
       </c>
       <c r="DI4" t="n">
-        <v>5.398769000528248e-286</v>
+        <v>4.269364396683114e-283</v>
       </c>
       <c r="DJ4" t="n">
-        <v>4.585208900849863e-289</v>
+        <v>1.772375824045154e-286</v>
       </c>
       <c r="DK4" t="n">
-        <v>1.844707500609777e-292</v>
+        <v>1.171824515122871e-289</v>
       </c>
       <c r="DL4" t="n">
-        <v>1.584245601333634e-295</v>
+        <v>1.628029297081753e-292</v>
       </c>
       <c r="DM4" t="n">
-        <v>8.93579638656233e-299</v>
+        <v>7.902699225195599e-296</v>
       </c>
       <c r="DN4" t="n">
-        <v>9.030744194026781e-302</v>
+        <v>6.675286003317417e-299</v>
       </c>
       <c r="DO4" t="n">
-        <v>3.512685138125671e-305</v>
+        <v>1.433743958235714e-301</v>
       </c>
       <c r="DP4" t="n">
-        <v>0</v>
+        <v>9.531532521972479e-305</v>
       </c>
       <c r="DQ4" t="n">
         <v>0</v>
@@ -7989,415 +7989,415 @@
         <v>0.34</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3886646214012456</v>
+        <v>0.3925771446703679</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4463821290676815</v>
+        <v>0.2641042929582498</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6041578606263894</v>
+        <v>0.1040129123073458</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4570422934613618</v>
+        <v>0.4759377613820385</v>
       </c>
       <c r="G2" t="n">
-        <v>0.6339304040938666</v>
+        <v>0.2216070367593811</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4642045728974047</v>
+        <v>0.04474710449445327</v>
       </c>
       <c r="I2" t="n">
-        <v>0.396543269094435</v>
+        <v>0.03737477951466373</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3263497035003734</v>
+        <v>0.004579290109903504</v>
       </c>
       <c r="K2" t="n">
-        <v>0.05891997771326453</v>
+        <v>0.0007624948999256349</v>
       </c>
       <c r="L2" t="n">
-        <v>0.02312882481876145</v>
+        <v>0.004050269072348509</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0257677007766999</v>
+        <v>0.001251431187995805</v>
       </c>
       <c r="N2" t="n">
-        <v>0.002532480842624122</v>
+        <v>5.322658619785729e-06</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0001972777381398554</v>
+        <v>1.251971591204427e-07</v>
       </c>
       <c r="P2" t="n">
-        <v>4.418538298721034e-05</v>
+        <v>1.152198619473596e-08</v>
       </c>
       <c r="Q2" t="n">
-        <v>7.354355272591708e-07</v>
+        <v>6.906555496690303e-10</v>
       </c>
       <c r="R2" t="n">
-        <v>1.118240601225256e-07</v>
+        <v>1.741111677951821e-11</v>
       </c>
       <c r="S2" t="n">
-        <v>1.169104925246798e-08</v>
+        <v>3.119125858117397e-12</v>
       </c>
       <c r="T2" t="n">
-        <v>4.253747061385827e-10</v>
+        <v>1.858185732208768e-13</v>
       </c>
       <c r="U2" t="n">
-        <v>1.150307625037306e-11</v>
+        <v>4.053774357307213e-15</v>
       </c>
       <c r="V2" t="n">
-        <v>5.725574102911696e-13</v>
+        <v>7.194728746606701e-17</v>
       </c>
       <c r="W2" t="n">
-        <v>2.0232678523802e-14</v>
+        <v>1.56042817390213e-18</v>
       </c>
       <c r="X2" t="n">
-        <v>7.401100408715972e-16</v>
+        <v>6.750125375479974e-20</v>
       </c>
       <c r="Y2" t="n">
-        <v>3.78233310612607e-18</v>
+        <v>1.035311835910705e-21</v>
       </c>
       <c r="Z2" t="n">
-        <v>4.463684189815293e-20</v>
+        <v>1.610303451663393e-23</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.241583043091277e-21</v>
+        <v>2.329662682751806e-25</v>
       </c>
       <c r="AB2" t="n">
-        <v>8.898517004461279e-23</v>
+        <v>6.267020761052599e-28</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.338953186537166e-24</v>
+        <v>2.780588964484502e-30</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.317267140845874e-26</v>
+        <v>1.262025766930035e-31</v>
       </c>
       <c r="AE2" t="n">
-        <v>4.700629922576633e-28</v>
+        <v>1.308550400514769e-33</v>
       </c>
       <c r="AF2" t="n">
-        <v>1.012193283041124e-30</v>
+        <v>5.327892726900952e-35</v>
       </c>
       <c r="AG2" t="n">
-        <v>8.130292969530914e-33</v>
+        <v>5.436971068593053e-38</v>
       </c>
       <c r="AH2" t="n">
-        <v>8.557245077338672e-35</v>
+        <v>1.437142463192435e-39</v>
       </c>
       <c r="AI2" t="n">
-        <v>1.577752925341245e-36</v>
+        <v>2.032100745479471e-41</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.330698542813266e-38</v>
+        <v>2.721979860261748e-43</v>
       </c>
       <c r="AK2" t="n">
-        <v>7.057451313511805e-41</v>
+        <v>7.943803984692056e-45</v>
       </c>
       <c r="AL2" t="n">
-        <v>4.617888590820748e-43</v>
+        <v>1.571253490989273e-47</v>
       </c>
       <c r="AM2" t="n">
-        <v>2.662311553348682e-45</v>
+        <v>6.157977711370059e-49</v>
       </c>
       <c r="AN2" t="n">
-        <v>9.223305036749229e-48</v>
+        <v>9.211059187836741e-51</v>
       </c>
       <c r="AO2" t="n">
-        <v>8.689408662193109e-49</v>
+        <v>4.87947835108862e-53</v>
       </c>
       <c r="AP2" t="n">
-        <v>3.82211594450631e-51</v>
+        <v>1.075344037152151e-55</v>
       </c>
       <c r="AQ2" t="n">
-        <v>7.984703984320029e-53</v>
+        <v>1.328777227288501e-58</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.894139938511865e-55</v>
+        <v>1.34085632501782e-60</v>
       </c>
       <c r="AS2" t="n">
-        <v>1.827351416115799e-57</v>
+        <v>1.683045517502776e-62</v>
       </c>
       <c r="AT2" t="n">
-        <v>8.86189353464205e-60</v>
+        <v>1.40835876055952e-65</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.673850209763674e-61</v>
+        <v>8.911910956006411e-68</v>
       </c>
       <c r="AV2" t="n">
-        <v>5.770052124380065e-63</v>
+        <v>3.293017548484962e-70</v>
       </c>
       <c r="AW2" t="n">
-        <v>3.05043931162489e-65</v>
+        <v>1.158615884101406e-72</v>
       </c>
       <c r="AX2" t="n">
-        <v>5.0226502392779e-67</v>
+        <v>1.056727553962261e-74</v>
       </c>
       <c r="AY2" t="n">
-        <v>3.181484793274098e-69</v>
+        <v>2.668446568666848e-77</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1.18187676823107e-71</v>
+        <v>2.113867171613934e-79</v>
       </c>
       <c r="BA2" t="n">
-        <v>2.18267862766315e-74</v>
+        <v>6.297059057269665e-82</v>
       </c>
       <c r="BB2" t="n">
-        <v>8.70791576645501e-77</v>
+        <v>5.712629238953375e-84</v>
       </c>
       <c r="BC2" t="n">
-        <v>3.646242958938329e-79</v>
+        <v>2.874559110049833e-87</v>
       </c>
       <c r="BD2" t="n">
-        <v>5.138424868303154e-82</v>
+        <v>1.442110787276206e-89</v>
       </c>
       <c r="BE2" t="n">
-        <v>5.133640666892574e-84</v>
+        <v>6.622776011545789e-92</v>
       </c>
       <c r="BF2" t="n">
-        <v>4.068581180467672e-86</v>
+        <v>6.958637263134361e-95</v>
       </c>
       <c r="BG2" t="n">
-        <v>3.625050985563531e-88</v>
+        <v>9.070403479613576e-98</v>
       </c>
       <c r="BH2" t="n">
-        <v>1.431798539310462e-90</v>
+        <v>9.019828074651109e-100</v>
       </c>
       <c r="BI2" t="n">
-        <v>4.671506228279481e-92</v>
+        <v>2.975640064354632e-102</v>
       </c>
       <c r="BJ2" t="n">
-        <v>3.982240935939469e-94</v>
+        <v>7.210492313824905e-105</v>
       </c>
       <c r="BK2" t="n">
-        <v>1.38370831921821e-96</v>
+        <v>1.364820299626642e-107</v>
       </c>
       <c r="BL2" t="n">
-        <v>3.874100067537786e-99</v>
+        <v>1.650119106846655e-110</v>
       </c>
       <c r="BM2" t="n">
-        <v>5.896517906161021e-102</v>
+        <v>3.137871319526548e-113</v>
       </c>
       <c r="BN2" t="n">
-        <v>1.388871502930474e-104</v>
+        <v>1.092440979330077e-115</v>
       </c>
       <c r="BO2" t="n">
-        <v>2.671046045508126e-107</v>
+        <v>1.248169127550239e-118</v>
       </c>
       <c r="BP2" t="n">
-        <v>1.073490623118688e-109</v>
+        <v>6.531427262427118e-121</v>
       </c>
       <c r="BQ2" t="n">
-        <v>2.493504105341266e-112</v>
+        <v>4.805750183836632e-124</v>
       </c>
       <c r="BR2" t="n">
-        <v>1.265641775460008e-114</v>
+        <v>8.449553233272415e-127</v>
       </c>
       <c r="BS2" t="n">
-        <v>3.107059462100585e-117</v>
+        <v>5.359881467062627e-129</v>
       </c>
       <c r="BT2" t="n">
-        <v>9.313438118223531e-120</v>
+        <v>7.461390772466175e-132</v>
       </c>
       <c r="BU2" t="n">
-        <v>3.129368130872864e-122</v>
+        <v>1.077519123084041e-134</v>
       </c>
       <c r="BV2" t="n">
-        <v>5.608913225348151e-125</v>
+        <v>1.674115273894376e-137</v>
       </c>
       <c r="BW2" t="n">
-        <v>8.222020503797854e-128</v>
+        <v>4.757544270125393e-140</v>
       </c>
       <c r="BX2" t="n">
-        <v>4.242759001344459e-130</v>
+        <v>2.286905001959445e-142</v>
       </c>
       <c r="BY2" t="n">
-        <v>1.346207467252771e-132</v>
+        <v>8.398148000500088e-145</v>
       </c>
       <c r="BZ2" t="n">
-        <v>5.169059552169898e-135</v>
+        <v>4.183921166910779e-147</v>
       </c>
       <c r="CA2" t="n">
-        <v>9.211912249444266e-138</v>
+        <v>1.557382570073384e-149</v>
       </c>
       <c r="CB2" t="n">
-        <v>2.80731636776549e-140</v>
+        <v>2.203521812236706e-152</v>
       </c>
       <c r="CC2" t="n">
-        <v>4.632776154742529e-143</v>
+        <v>4.985321277610684e-155</v>
       </c>
       <c r="CD2" t="n">
-        <v>1.665510477249076e-145</v>
+        <v>1.34470046673957e-157</v>
       </c>
       <c r="CE2" t="n">
-        <v>1.883726142519307e-148</v>
+        <v>8.65609357726795e-161</v>
       </c>
       <c r="CF2" t="n">
-        <v>3.114484504064593e-151</v>
+        <v>1.665548677562721e-163</v>
       </c>
       <c r="CG2" t="n">
-        <v>5.470873812152878e-154</v>
+        <v>1.018295439359033e-165</v>
       </c>
       <c r="CH2" t="n">
-        <v>9.304637150116469e-157</v>
+        <v>7.636026321750887e-169</v>
       </c>
       <c r="CI2" t="n">
-        <v>1.832240526422285e-159</v>
+        <v>1.204273785622652e-171</v>
       </c>
       <c r="CJ2" t="n">
-        <v>1.160716938697965e-161</v>
+        <v>3.1991888623125e-174</v>
       </c>
       <c r="CK2" t="n">
-        <v>1.568176344308986e-164</v>
+        <v>1.184506922305404e-176</v>
       </c>
       <c r="CL2" t="n">
-        <v>1.696741474581261e-167</v>
+        <v>3.034375331456541e-179</v>
       </c>
       <c r="CM2" t="n">
-        <v>4.300651463939555e-170</v>
+        <v>3.613668286557026e-182</v>
       </c>
       <c r="CN2" t="n">
-        <v>1.047508751676931e-172</v>
+        <v>2.829726694217513e-184</v>
       </c>
       <c r="CO2" t="n">
-        <v>1.732939138909158e-175</v>
+        <v>7.096411439555469e-186</v>
       </c>
       <c r="CP2" t="n">
-        <v>1.523598167725165e-178</v>
+        <v>5.252220428485966e-189</v>
       </c>
       <c r="CQ2" t="n">
-        <v>3.151197171340903e-181</v>
+        <v>2.105504655119263e-191</v>
       </c>
       <c r="CR2" t="n">
-        <v>3.302267406095422e-184</v>
+        <v>2.166058585981365e-194</v>
       </c>
       <c r="CS2" t="n">
-        <v>5.134916248086702e-187</v>
+        <v>2.909585147169821e-197</v>
       </c>
       <c r="CT2" t="n">
-        <v>1.005814877920144e-189</v>
+        <v>2.827164891451268e-200</v>
       </c>
       <c r="CU2" t="n">
-        <v>1.192711241181832e-192</v>
+        <v>4.506701023672686e-203</v>
       </c>
       <c r="CV2" t="n">
-        <v>2.85328819644691e-195</v>
+        <v>9.330660139268737e-206</v>
       </c>
       <c r="CW2" t="n">
-        <v>4.316903310314282e-198</v>
+        <v>1.91710277576105e-208</v>
       </c>
       <c r="CX2" t="n">
-        <v>9.566071053159932e-201</v>
+        <v>2.175303121675498e-211</v>
       </c>
       <c r="CY2" t="n">
-        <v>2.438278671094978e-203</v>
+        <v>2.767407942000269e-214</v>
       </c>
       <c r="CZ2" t="n">
-        <v>4.348715588948986e-206</v>
+        <v>7.401868342012091e-217</v>
       </c>
       <c r="DA2" t="n">
-        <v>6.61655663132059e-209</v>
+        <v>8.017764992087336e-220</v>
       </c>
       <c r="DB2" t="n">
-        <v>8.032726191815989e-212</v>
+        <v>1.007705739112626e-222</v>
       </c>
       <c r="DC2" t="n">
-        <v>8.480139282890336e-215</v>
+        <v>2.191175748491649e-225</v>
       </c>
       <c r="DD2" t="n">
-        <v>5.43651098465913e-217</v>
+        <v>2.247233844510049e-228</v>
       </c>
       <c r="DE2" t="n">
-        <v>4.31755823222587e-220</v>
+        <v>6.731323900464772e-231</v>
       </c>
       <c r="DF2" t="n">
-        <v>4.558141521482147e-223</v>
+        <v>9.61617217998588e-234</v>
       </c>
       <c r="DG2" t="n">
-        <v>3.700890856332966e-226</v>
+        <v>2.222998864493182e-236</v>
       </c>
       <c r="DH2" t="n">
-        <v>1.785066964076756e-228</v>
+        <v>4.750936430977525e-239</v>
       </c>
       <c r="DI2" t="n">
-        <v>7.562644955200168e-231</v>
+        <v>4.910703312536163e-242</v>
       </c>
       <c r="DJ2" t="n">
-        <v>1.208275760238667e-233</v>
+        <v>4.16524636655914e-245</v>
       </c>
       <c r="DK2" t="n">
-        <v>1.390003135345403e-236</v>
+        <v>3.589685602008726e-248</v>
       </c>
       <c r="DL2" t="n">
-        <v>2.150474439561489e-239</v>
+        <v>1.78317794447061e-251</v>
       </c>
       <c r="DM2" t="n">
-        <v>1.369477406242299e-242</v>
+        <v>7.071153414971812e-255</v>
       </c>
       <c r="DN2" t="n">
-        <v>4.382132788123227e-245</v>
+        <v>5.018512450061782e-258</v>
       </c>
       <c r="DO2" t="n">
-        <v>1.157487734453493e-247</v>
+        <v>9.544802560113963e-261</v>
       </c>
       <c r="DP2" t="n">
-        <v>2.150736566185093e-250</v>
+        <v>1.840276702798644e-263</v>
       </c>
       <c r="DQ2" t="n">
-        <v>2.582027569033155e-253</v>
+        <v>2.398739417253233e-266</v>
       </c>
       <c r="DR2" t="n">
-        <v>4.112244888211057e-256</v>
+        <v>1.965620448344101e-269</v>
       </c>
       <c r="DS2" t="n">
-        <v>4.171585755963235e-259</v>
+        <v>1.371986973745637e-272</v>
       </c>
       <c r="DT2" t="n">
-        <v>3.506042592803475e-262</v>
+        <v>1.530876665252467e-275</v>
       </c>
       <c r="DU2" t="n">
-        <v>1.76432180434712e-264</v>
+        <v>1.393398593635052e-278</v>
       </c>
       <c r="DV2" t="n">
-        <v>7.376672162470656e-267</v>
+        <v>9.656352654822589e-282</v>
       </c>
       <c r="DW2" t="n">
-        <v>5.658245753395952e-270</v>
+        <v>1.348521274290809e-284</v>
       </c>
       <c r="DX2" t="n">
-        <v>4.761898940410685e-273</v>
+        <v>1.016942927228563e-287</v>
       </c>
       <c r="DY2" t="n">
-        <v>4.223394674280097e-276</v>
+        <v>1.145485396386367e-290</v>
       </c>
       <c r="DZ2" t="n">
-        <v>1.315724126168327e-278</v>
+        <v>1.985651319784211e-293</v>
       </c>
       <c r="EA2" t="n">
-        <v>1.08717160814707e-281</v>
+        <v>2.230011295570651e-296</v>
       </c>
       <c r="EB2" t="n">
-        <v>1.052360080531971e-284</v>
+        <v>2.394368408945091e-299</v>
       </c>
       <c r="EC2" t="n">
-        <v>1.729816217465152e-287</v>
+        <v>1.605868239217025e-302</v>
       </c>
       <c r="ED2" t="n">
-        <v>1.533692706770631e-290</v>
+        <v>1.482228177027413e-305</v>
       </c>
       <c r="EE2" t="n">
-        <v>2.624222753665482e-293</v>
+        <v>0</v>
       </c>
       <c r="EF2" t="n">
-        <v>5.132561599015998e-296</v>
+        <v>0</v>
       </c>
       <c r="EG2" t="n">
-        <v>3.057723759624186e-299</v>
+        <v>0</v>
       </c>
       <c r="EH2" t="n">
-        <v>7.405948786680854e-302</v>
+        <v>0</v>
       </c>
       <c r="EI2" t="n">
-        <v>5.491002418069827e-305</v>
+        <v>0</v>
       </c>
       <c r="EJ2" t="n">
         <v>0</v>
@@ -9496,70 +9496,70 @@
         <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3308648686140421</v>
+        <v>0.3305615703995133</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3427263105743406</v>
+        <v>0.3485987952389695</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3043853518361088</v>
+        <v>0.3010523034014769</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4355761493624736</v>
+        <v>0.3497995859382714</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3316908442446918</v>
+        <v>0.5204021500315056</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5126667448772062</v>
+        <v>0.6023668800705113</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6002088913501653</v>
+        <v>0.8531472104367155</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6731938052299796</v>
+        <v>0.7512883020416568</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9406048925350664</v>
+        <v>0.7427894261640088</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9768490249286601</v>
+        <v>0.9812679276753076</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9742303852881182</v>
+        <v>0.997613113798099</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9974673014546422</v>
+        <v>0.9993346002084348</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9998027030722875</v>
+        <v>0.9998419450315696</v>
       </c>
       <c r="P3" t="n">
-        <v>0.999955814504737</v>
+        <v>0.9999943160066167</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9999992645431238</v>
+        <v>0.9999896785808866</v>
       </c>
       <c r="R3" t="n">
-        <v>0.999999888175658</v>
+        <v>0.9999993298791189</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9999999883087933</v>
+        <v>0.9999999817421024</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9999999995746203</v>
+        <v>0.9999999991867171</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9999999999884968</v>
+        <v>0.9999999999780633</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9999999999994273</v>
+        <v>0.9999999999994413</v>
       </c>
       <c r="W3" t="n">
-        <v>0.9999999999999798</v>
+        <v>0.9999999999999918</v>
       </c>
       <c r="X3" t="n">
-        <v>0.9999999999999992</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="Y3" t="n">
         <v>1</v>
@@ -11003,406 +11003,406 @@
         <v>0.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2804705099847123</v>
+        <v>0.2768612849301187</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2108915603579781</v>
+        <v>0.3872969118027807</v>
       </c>
       <c r="E4" t="n">
-        <v>0.09145678753750179</v>
+        <v>0.5949347842911773</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1073815571761648</v>
+        <v>0.1742626526796901</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0343787516614418</v>
+        <v>0.2579908132091134</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02312868222538915</v>
+        <v>0.3528860154350354</v>
       </c>
       <c r="I4" t="n">
-        <v>0.003247839555399664</v>
+        <v>0.1094780100486208</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0004564912696471053</v>
+        <v>0.2441324078484397</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0004751297516691026</v>
+        <v>0.2564480789360655</v>
       </c>
       <c r="L4" t="n">
-        <v>2.215025257828964e-05</v>
+        <v>0.01468180325234387</v>
       </c>
       <c r="M4" t="n">
-        <v>1.913935181909412e-06</v>
+        <v>0.001135455013905196</v>
       </c>
       <c r="N4" t="n">
-        <v>2.177027335639375e-07</v>
+        <v>0.0006600771329454382</v>
       </c>
       <c r="O4" t="n">
-        <v>1.918957272267653e-08</v>
+        <v>0.0001579297712712685</v>
       </c>
       <c r="P4" t="n">
-        <v>1.122757762579345e-10</v>
+        <v>5.67247139696512e-06</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.13489996108615e-11</v>
+        <v>1.032072845789091e-05</v>
       </c>
       <c r="R4" t="n">
-        <v>2.820072538580712e-13</v>
+        <v>6.701034700979659e-07</v>
       </c>
       <c r="S4" t="n">
-        <v>1.572564502127937e-13</v>
+        <v>1.825477860987426e-08</v>
       </c>
       <c r="T4" t="n">
-        <v>4.967770626225244e-15</v>
+        <v>8.130970392862968e-10</v>
       </c>
       <c r="U4" t="n">
-        <v>1.344256626456365e-16</v>
+        <v>2.193255542420798e-11</v>
       </c>
       <c r="V4" t="n">
-        <v>1.17908679450393e-18</v>
+        <v>5.586486450805573e-13</v>
       </c>
       <c r="W4" t="n">
-        <v>8.521934193971309e-21</v>
+        <v>8.235791871634196e-15</v>
       </c>
       <c r="X4" t="n">
-        <v>5.300380818009627e-23</v>
+        <v>2.630961826999917e-16</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.545096108638721e-24</v>
+        <v>3.302272858013397e-18</v>
       </c>
       <c r="Z4" t="n">
-        <v>2.095183162808199e-26</v>
+        <v>3.23730749098599e-20</v>
       </c>
       <c r="AA4" t="n">
-        <v>5.245177423654955e-28</v>
+        <v>4.402399636649791e-22</v>
       </c>
       <c r="AB4" t="n">
-        <v>3.009125137503684e-30</v>
+        <v>3.931430626426097e-23</v>
       </c>
       <c r="AC4" t="n">
-        <v>1.518273689922616e-32</v>
+        <v>1.592950858951379e-23</v>
       </c>
       <c r="AD4" t="n">
-        <v>4.573357970683252e-34</v>
+        <v>5.114822407152378e-27</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.122649276578699e-36</v>
+        <v>7.506480198132974e-29</v>
       </c>
       <c r="AF4" t="n">
-        <v>1.920699415382076e-38</v>
+        <v>1.459705290995046e-31</v>
       </c>
       <c r="AG4" t="n">
-        <v>1.041732248319391e-40</v>
+        <v>3.304051231929837e-33</v>
       </c>
       <c r="AH4" t="n">
-        <v>5.49698325190916e-43</v>
+        <v>2.051908697931438e-36</v>
       </c>
       <c r="AI4" t="n">
-        <v>8.312324298133966e-46</v>
+        <v>3.61511607076776e-39</v>
       </c>
       <c r="AJ4" t="n">
-        <v>5.565941485502695e-48</v>
+        <v>6.012283383023403e-42</v>
       </c>
       <c r="AK4" t="n">
-        <v>1.028687214679252e-49</v>
+        <v>1.935000950687124e-44</v>
       </c>
       <c r="AL4" t="n">
-        <v>6.069636463826136e-52</v>
+        <v>1.90733557337855e-46</v>
       </c>
       <c r="AM4" t="n">
-        <v>3.469635383737044e-54</v>
+        <v>7.863870476116458e-51</v>
       </c>
       <c r="AN4" t="n">
-        <v>4.440066211019457e-56</v>
+        <v>1.00304261928638e-52</v>
       </c>
       <c r="AO4" t="n">
-        <v>1.155871542276966e-57</v>
+        <v>4.311459007918548e-55</v>
       </c>
       <c r="AP4" t="n">
-        <v>3.746892751824252e-59</v>
+        <v>2.842253668542076e-57</v>
       </c>
       <c r="AQ4" t="n">
-        <v>7.05083931988653e-61</v>
+        <v>2.547416038397266e-59</v>
       </c>
       <c r="AR4" t="n">
-        <v>5.073104861072121e-63</v>
+        <v>1.125528238528579e-61</v>
       </c>
       <c r="AS4" t="n">
-        <v>9.68298386986609e-66</v>
+        <v>5.254707365110555e-63</v>
       </c>
       <c r="AT4" t="n">
-        <v>3.443647332802493e-68</v>
+        <v>6.285409193232922e-65</v>
       </c>
       <c r="AU4" t="n">
-        <v>4.829372658707518e-70</v>
+        <v>1.253988207549946e-67</v>
       </c>
       <c r="AV4" t="n">
-        <v>2.679761582948738e-72</v>
+        <v>3.475594580915174e-70</v>
       </c>
       <c r="AW4" t="n">
-        <v>1.463061886216209e-74</v>
+        <v>1.040447368043583e-72</v>
       </c>
       <c r="AX4" t="n">
-        <v>3.747759133527122e-77</v>
+        <v>1.217945401878728e-75</v>
       </c>
       <c r="AY4" t="n">
-        <v>8.49739521846003e-80</v>
+        <v>3.708393925723882e-78</v>
       </c>
       <c r="AZ4" t="n">
-        <v>3.626162198437479e-82</v>
+        <v>2.987367216820788e-81</v>
       </c>
       <c r="BA4" t="n">
-        <v>2.115813135098485e-84</v>
+        <v>7.174206696069925e-84</v>
       </c>
       <c r="BB4" t="n">
-        <v>1.476333154864625e-86</v>
+        <v>1.038033071487114e-86</v>
       </c>
       <c r="BC4" t="n">
-        <v>1.775895683773194e-88</v>
+        <v>9.104589670795908e-89</v>
       </c>
       <c r="BD4" t="n">
-        <v>7.024100725948044e-91</v>
+        <v>3.377227074333916e-91</v>
       </c>
       <c r="BE4" t="n">
-        <v>1.281193379185666e-93</v>
+        <v>2.526467305923611e-92</v>
       </c>
       <c r="BF4" t="n">
-        <v>5.887829819755327e-96</v>
+        <v>3.813051717885848e-94</v>
       </c>
       <c r="BG4" t="n">
-        <v>2.313051079923991e-98</v>
+        <v>1.389167696942116e-96</v>
       </c>
       <c r="BH4" t="n">
-        <v>2.6444413032289e-100</v>
+        <v>4.783990437221084e-99</v>
       </c>
       <c r="BI4" t="n">
-        <v>1.508473948521804e-101</v>
+        <v>2.395336481677466e-101</v>
       </c>
       <c r="BJ4" t="n">
-        <v>5.636156785015245e-104</v>
+        <v>7.25438392366949e-104</v>
       </c>
       <c r="BK4" t="n">
-        <v>1.474006247766875e-106</v>
+        <v>1.538157712118432e-106</v>
       </c>
       <c r="BL4" t="n">
-        <v>2.675973246790757e-109</v>
+        <v>7.449252252407989e-109</v>
       </c>
       <c r="BM4" t="n">
-        <v>6.138801967059162e-112</v>
+        <v>2.561192041226369e-111</v>
       </c>
       <c r="BN4" t="n">
-        <v>8.700240860880718e-115</v>
+        <v>3.228329764111998e-114</v>
       </c>
       <c r="BO4" t="n">
-        <v>1.624100989624688e-117</v>
+        <v>8.954211213403187e-117</v>
       </c>
       <c r="BP4" t="n">
-        <v>1.372197799115501e-120</v>
+        <v>2.952980936604704e-119</v>
       </c>
       <c r="BQ4" t="n">
-        <v>2.890118629077044e-123</v>
+        <v>1.922743195927384e-121</v>
       </c>
       <c r="BR4" t="n">
-        <v>8.09601869632772e-126</v>
+        <v>5.197484157892574e-124</v>
       </c>
       <c r="BS4" t="n">
-        <v>9.035943404443166e-129</v>
+        <v>1.927059267152449e-126</v>
       </c>
       <c r="BT4" t="n">
-        <v>8.713774063127265e-132</v>
+        <v>6.126441065845733e-129</v>
       </c>
       <c r="BU4" t="n">
-        <v>9.162408161459281e-135</v>
+        <v>1.074403639168505e-131</v>
       </c>
       <c r="BV4" t="n">
-        <v>1.799044342400478e-137</v>
+        <v>1.70555522993795e-134</v>
       </c>
       <c r="BW4" t="n">
-        <v>3.668145500492888e-140</v>
+        <v>1.436368742288604e-137</v>
       </c>
       <c r="BX4" t="n">
-        <v>9.010816298859896e-143</v>
+        <v>2.803373230801011e-139</v>
       </c>
       <c r="BY4" t="n">
-        <v>8.117782583500878e-146</v>
+        <v>2.10207453924444e-142</v>
       </c>
       <c r="BZ4" t="n">
-        <v>2.499657077931179e-148</v>
+        <v>1.384004891775871e-144</v>
       </c>
       <c r="CA4" t="n">
-        <v>2.884221014221378e-151</v>
+        <v>7.566336847053272e-147</v>
       </c>
       <c r="CB4" t="n">
-        <v>8.60690322354738e-154</v>
+        <v>4.069312548826448e-149</v>
       </c>
       <c r="CC4" t="n">
-        <v>1.038438255362965e-156</v>
+        <v>3.698783422012895e-152</v>
       </c>
       <c r="CD4" t="n">
-        <v>1.504311424436323e-158</v>
+        <v>1.562844121207056e-154</v>
       </c>
       <c r="CE4" t="n">
-        <v>2.519228714702654e-161</v>
+        <v>6.105386910723577e-157</v>
       </c>
       <c r="CF4" t="n">
-        <v>2.885996848234689e-164</v>
+        <v>6.096376446367742e-160</v>
       </c>
       <c r="CG4" t="n">
-        <v>2.803683361045745e-167</v>
+        <v>7.63819347680882e-163</v>
       </c>
       <c r="CH4" t="n">
-        <v>3.545635528037962e-170</v>
+        <v>1.754020725432861e-165</v>
       </c>
       <c r="CI4" t="n">
-        <v>9.742193991732929e-173</v>
+        <v>6.441772421876906e-168</v>
       </c>
       <c r="CJ4" t="n">
-        <v>3.482301309141829e-175</v>
+        <v>6.485924476316043e-171</v>
       </c>
       <c r="CK4" t="n">
-        <v>3.995402744496315e-178</v>
+        <v>1.010104800008117e-173</v>
       </c>
       <c r="CL4" t="n">
-        <v>5.722302575352594e-181</v>
+        <v>8.361233845241426e-177</v>
       </c>
       <c r="CM4" t="n">
-        <v>1.453530653136138e-183</v>
+        <v>1.044215886413163e-179</v>
       </c>
       <c r="CN4" t="n">
-        <v>2.502590547253381e-186</v>
+        <v>8.873921708347255e-182</v>
       </c>
       <c r="CO4" t="n">
-        <v>4.026978713256243e-189</v>
+        <v>6.346653645417758e-183</v>
       </c>
       <c r="CP4" t="n">
-        <v>6.894046423849462e-192</v>
+        <v>3.502608785403903e-185</v>
       </c>
       <c r="CQ4" t="n">
-        <v>5.842862561212546e-195</v>
+        <v>6.868448030160575e-188</v>
       </c>
       <c r="CR4" t="n">
-        <v>1.11531263409016e-197</v>
+        <v>1.215188533017188e-190</v>
       </c>
       <c r="CS4" t="n">
-        <v>1.230319541205045e-200</v>
+        <v>1.814548819365799e-193</v>
       </c>
       <c r="CT4" t="n">
-        <v>2.195983355506923e-203</v>
+        <v>2.34046011261414e-196</v>
       </c>
       <c r="CU4" t="n">
-        <v>5.020242574785584e-206</v>
+        <v>2.070632275150373e-199</v>
       </c>
       <c r="CV4" t="n">
-        <v>1.015337445206485e-208</v>
+        <v>1.293276309299701e-202</v>
       </c>
       <c r="CW4" t="n">
-        <v>8.353281793542779e-212</v>
+        <v>9.317028162136367e-206</v>
       </c>
       <c r="CX4" t="n">
-        <v>8.0054177265819e-215</v>
+        <v>1.029371079260296e-208</v>
       </c>
       <c r="CY4" t="n">
-        <v>2.110188573207284e-217</v>
+        <v>1.372493360347672e-211</v>
       </c>
       <c r="CZ4" t="n">
-        <v>3.912896999764731e-220</v>
+        <v>3.152227749446149e-214</v>
       </c>
       <c r="DA4" t="n">
-        <v>4.132203247108951e-223</v>
+        <v>2.942541258590683e-217</v>
       </c>
       <c r="DB4" t="n">
-        <v>4.150404092212378e-226</v>
+        <v>2.442908014267043e-220</v>
       </c>
       <c r="DC4" t="n">
-        <v>4.483929669178973e-229</v>
+        <v>2.154261380852871e-223</v>
       </c>
       <c r="DD4" t="n">
-        <v>1.974294023945881e-231</v>
+        <v>1.013181775401219e-225</v>
       </c>
       <c r="DE4" t="n">
-        <v>2.462321759305391e-234</v>
+        <v>7.664555743920786e-228</v>
       </c>
       <c r="DF4" t="n">
-        <v>2.196938746310341e-237</v>
+        <v>8.405159114886139e-231</v>
       </c>
       <c r="DG4" t="n">
-        <v>3.712595345497315e-240</v>
+        <v>1.06793830689566e-233</v>
       </c>
       <c r="DH4" t="n">
-        <v>2.830577356969342e-242</v>
+        <v>1.153409750566206e-236</v>
       </c>
       <c r="DI4" t="n">
-        <v>1.050059296160012e-244</v>
+        <v>1.308757982013104e-239</v>
       </c>
       <c r="DJ4" t="n">
-        <v>1.017274284398029e-247</v>
+        <v>1.334184742741483e-242</v>
       </c>
       <c r="DK4" t="n">
-        <v>1.260121462500148e-250</v>
+        <v>1.693458077806157e-245</v>
       </c>
       <c r="DL4" t="n">
-        <v>3.598764063593689e-253</v>
+        <v>3.431688796062558e-248</v>
       </c>
       <c r="DM4" t="n">
-        <v>5.3004377428502e-256</v>
+        <v>8.594507585631001e-251</v>
       </c>
       <c r="DN4" t="n">
-        <v>6.491124034247331e-259</v>
+        <v>1.070551499727055e-253</v>
       </c>
       <c r="DO4" t="n">
-        <v>2.050590720231929e-261</v>
+        <v>1.829268712232274e-256</v>
       </c>
       <c r="DP4" t="n">
-        <v>1.706167261888081e-264</v>
+        <v>8.860889239908945e-260</v>
       </c>
       <c r="DQ4" t="n">
-        <v>1.084229350154708e-267</v>
+        <v>5.275608585399463e-263</v>
       </c>
       <c r="DR4" t="n">
-        <v>1.998349583763482e-270</v>
+        <v>4.681320214813319e-266</v>
       </c>
       <c r="DS4" t="n">
-        <v>2.134066413449949e-273</v>
+        <v>6.945845357426457e-269</v>
       </c>
       <c r="DT4" t="n">
-        <v>1.738829847011345e-276</v>
+        <v>5.637112194274442e-272</v>
       </c>
       <c r="DU4" t="n">
-        <v>5.939312054580107e-279</v>
+        <v>4.570451562350641e-275</v>
       </c>
       <c r="DV4" t="n">
-        <v>1.829645733516766e-281</v>
+        <v>5.130246499585773e-278</v>
       </c>
       <c r="DW4" t="n">
-        <v>1.599977037332655e-284</v>
+        <v>6.234329055014477e-281</v>
       </c>
       <c r="DX4" t="n">
-        <v>1.314771344402366e-287</v>
+        <v>5.290789108665233e-284</v>
       </c>
       <c r="DY4" t="n">
-        <v>9.344301162476996e-291</v>
+        <v>3.378995804991621e-287</v>
       </c>
       <c r="DZ4" t="n">
-        <v>2.80016225685532e-293</v>
+        <v>3.785350855176243e-290</v>
       </c>
       <c r="EA4" t="n">
-        <v>2.748448905437284e-296</v>
+        <v>1.407591137801778e-292</v>
       </c>
       <c r="EB4" t="n">
-        <v>1.771867372577223e-299</v>
+        <v>2.104685462034886e-295</v>
       </c>
       <c r="EC4" t="n">
-        <v>1.984807778282893e-302</v>
+        <v>1.856013131545712e-298</v>
       </c>
       <c r="ED4" t="n">
-        <v>2.680723363966801e-305</v>
+        <v>1.247922634318774e-301</v>
       </c>
       <c r="EE4" t="n">
-        <v>3.947878587960706e-308</v>
+        <v>1.104449574301207e-304</v>
       </c>
       <c r="EF4" t="n">
-        <v>0</v>
+        <v>1.078714190986368e-307</v>
       </c>
       <c r="EG4" t="n">
         <v>0</v>
@@ -14031,361 +14031,361 @@
         <v>0.34</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2732288957993735</v>
+        <v>0.3045859194679809</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3570473787970924</v>
+        <v>0.1712255876923016</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3819773497471248</v>
+        <v>0.0318820718510463</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1954519946601752</v>
+        <v>0.006744471856317846</v>
       </c>
       <c r="G2" t="n">
-        <v>0.08112531388741084</v>
+        <v>0.0009139791816944766</v>
       </c>
       <c r="H2" t="n">
-        <v>0.02617090090064152</v>
+        <v>4.080671638372934e-05</v>
       </c>
       <c r="I2" t="n">
-        <v>0.03700636277628283</v>
+        <v>2.699457780828986e-06</v>
       </c>
       <c r="J2" t="n">
-        <v>0.009683288906800267</v>
+        <v>5.372826505084906e-07</v>
       </c>
       <c r="K2" t="n">
-        <v>0.001169065762425234</v>
+        <v>1.159782700103099e-08</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0002342132859040842</v>
+        <v>5.464449599227583e-10</v>
       </c>
       <c r="M2" t="n">
-        <v>2.216386837100766e-05</v>
+        <v>3.413510291353302e-12</v>
       </c>
       <c r="N2" t="n">
-        <v>2.405287787064458e-06</v>
+        <v>2.461848418918224e-13</v>
       </c>
       <c r="O2" t="n">
-        <v>3.365686794930939e-08</v>
+        <v>8.223138082971664e-15</v>
       </c>
       <c r="P2" t="n">
-        <v>2.60528209927367e-10</v>
+        <v>8.811349891937464e-17</v>
       </c>
       <c r="Q2" t="n">
-        <v>8.496950824326657e-12</v>
+        <v>1.112250854754959e-18</v>
       </c>
       <c r="R2" t="n">
-        <v>1.551792213526147e-13</v>
+        <v>9.77856994372596e-21</v>
       </c>
       <c r="S2" t="n">
-        <v>5.174627368328493e-16</v>
+        <v>4.013771526900482e-23</v>
       </c>
       <c r="T2" t="n">
-        <v>2.099109652167115e-17</v>
+        <v>9.541091072217902e-26</v>
       </c>
       <c r="U2" t="n">
-        <v>4.048487123401357e-19</v>
+        <v>1.341871693089978e-27</v>
       </c>
       <c r="V2" t="n">
-        <v>1.263839571931414e-21</v>
+        <v>4.458666112471643e-30</v>
       </c>
       <c r="W2" t="n">
-        <v>8.145144915245995e-24</v>
+        <v>3.40935386072898e-33</v>
       </c>
       <c r="X2" t="n">
-        <v>3.71903412569322e-26</v>
+        <v>3.764621711186246e-35</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.269210746385768e-27</v>
+        <v>1.320364381715856e-36</v>
       </c>
       <c r="Z2" t="n">
-        <v>2.972646586770325e-30</v>
+        <v>2.221784896638098e-38</v>
       </c>
       <c r="AA2" t="n">
-        <v>3.237813237451207e-33</v>
+        <v>1.383448677056633e-41</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.074233702000034e-35</v>
+        <v>2.1556313941178e-44</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.266732347037029e-38</v>
+        <v>5.461313114583715e-47</v>
       </c>
       <c r="AD2" t="n">
-        <v>3.404238050425361e-41</v>
+        <v>7.199893629535289e-50</v>
       </c>
       <c r="AE2" t="n">
-        <v>7.271862523439922e-44</v>
+        <v>4.729845068183446e-52</v>
       </c>
       <c r="AF2" t="n">
-        <v>2.213964664094924e-46</v>
+        <v>1.836240103671468e-54</v>
       </c>
       <c r="AG2" t="n">
-        <v>2.346951180372658e-49</v>
+        <v>2.89161224543344e-57</v>
       </c>
       <c r="AH2" t="n">
-        <v>2.152150751744109e-51</v>
+        <v>3.658008462058647e-60</v>
       </c>
       <c r="AI2" t="n">
-        <v>4.279160877267557e-54</v>
+        <v>2.373008063668738e-63</v>
       </c>
       <c r="AJ2" t="n">
-        <v>2.201770168264382e-56</v>
+        <v>5.826642479851055e-66</v>
       </c>
       <c r="AK2" t="n">
-        <v>5.359671331779412e-58</v>
+        <v>2.829768673573505e-68</v>
       </c>
       <c r="AL2" t="n">
-        <v>2.094613640534627e-60</v>
+        <v>1.956619042385718e-71</v>
       </c>
       <c r="AM2" t="n">
-        <v>4.039006964824344e-62</v>
+        <v>9.144204160073489e-74</v>
       </c>
       <c r="AN2" t="n">
-        <v>3.949618669524015e-64</v>
+        <v>5.736791104223973e-76</v>
       </c>
       <c r="AO2" t="n">
-        <v>2.750235900583203e-67</v>
+        <v>2.959496769878785e-78</v>
       </c>
       <c r="AP2" t="n">
-        <v>4.691283516931374e-70</v>
+        <v>3.640929553796568e-81</v>
       </c>
       <c r="AQ2" t="n">
-        <v>7.812689930107244e-73</v>
+        <v>4.463928389090611e-84</v>
       </c>
       <c r="AR2" t="n">
-        <v>1.015621491055453e-75</v>
+        <v>5.692031321661619e-87</v>
       </c>
       <c r="AS2" t="n">
-        <v>3.808739550477936e-78</v>
+        <v>1.299567645260021e-89</v>
       </c>
       <c r="AT2" t="n">
-        <v>5.705054364428818e-81</v>
+        <v>1.987332620518682e-92</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.003446395548553e-83</v>
+        <v>1.405682029287321e-94</v>
       </c>
       <c r="AV2" t="n">
-        <v>5.194430533063578e-86</v>
+        <v>6.163311259693969e-98</v>
       </c>
       <c r="AW2" t="n">
-        <v>9.550924596299756e-89</v>
+        <v>4.485490014960889e-101</v>
       </c>
       <c r="AX2" t="n">
-        <v>5.909392806096315e-91</v>
+        <v>2.560753875931678e-103</v>
       </c>
       <c r="AY2" t="n">
-        <v>1.669203493140827e-93</v>
+        <v>2.851706648881999e-106</v>
       </c>
       <c r="AZ2" t="n">
-        <v>2.55160843587683e-96</v>
+        <v>2.935830929694612e-109</v>
       </c>
       <c r="BA2" t="n">
-        <v>3.529773445046923e-99</v>
+        <v>4.705064489291355e-112</v>
       </c>
       <c r="BB2" t="n">
-        <v>5.454402774068141e-102</v>
+        <v>3.380142371131849e-114</v>
       </c>
       <c r="BC2" t="n">
-        <v>8.251720193568128e-105</v>
+        <v>7.905520852611883e-117</v>
       </c>
       <c r="BD2" t="n">
-        <v>1.543250361797498e-107</v>
+        <v>8.645608063811563e-120</v>
       </c>
       <c r="BE2" t="n">
-        <v>6.474361442546307e-110</v>
+        <v>4.81043824260678e-123</v>
       </c>
       <c r="BF2" t="n">
-        <v>6.137635617908293e-113</v>
+        <v>3.405177999535924e-126</v>
       </c>
       <c r="BG2" t="n">
-        <v>1.675942097761349e-115</v>
+        <v>1.650898815541479e-129</v>
       </c>
       <c r="BH2" t="n">
-        <v>1.059022021050042e-118</v>
+        <v>1.382001103642538e-132</v>
       </c>
       <c r="BI2" t="n">
-        <v>1.459466549834281e-121</v>
+        <v>1.117653913948613e-135</v>
       </c>
       <c r="BJ2" t="n">
-        <v>1.701288733578674e-124</v>
+        <v>9.874183609826823e-139</v>
       </c>
       <c r="BK2" t="n">
-        <v>1.083007227530421e-127</v>
+        <v>9.87323508709034e-142</v>
       </c>
       <c r="BL2" t="n">
-        <v>8.863121695831475e-131</v>
+        <v>6.052594082980776e-145</v>
       </c>
       <c r="BM2" t="n">
-        <v>7.374772712806372e-134</v>
+        <v>3.203228507356625e-148</v>
       </c>
       <c r="BN2" t="n">
-        <v>6.399129938889886e-137</v>
+        <v>2.153866493705476e-151</v>
       </c>
       <c r="BO2" t="n">
-        <v>3.09382681855717e-140</v>
+        <v>2.016017877836612e-154</v>
       </c>
       <c r="BP2" t="n">
-        <v>9.216975308199311e-143</v>
+        <v>2.613388876620287e-157</v>
       </c>
       <c r="BQ2" t="n">
-        <v>8.44727770657713e-146</v>
+        <v>3.677019910239031e-160</v>
       </c>
       <c r="BR2" t="n">
-        <v>6.529388648923937e-149</v>
+        <v>1.787453486359559e-163</v>
       </c>
       <c r="BS2" t="n">
-        <v>3.669421667083298e-152</v>
+        <v>6.128080680696191e-167</v>
       </c>
       <c r="BT2" t="n">
-        <v>1.998794669728862e-154</v>
+        <v>4.205603270505069e-170</v>
       </c>
       <c r="BU2" t="n">
-        <v>1.580077935610468e-157</v>
+        <v>3.56969555408563e-173</v>
       </c>
       <c r="BV2" t="n">
-        <v>1.093076295887019e-160</v>
+        <v>1.955459807878256e-176</v>
       </c>
       <c r="BW2" t="n">
-        <v>8.458646569849782e-164</v>
+        <v>1.199421549414217e-178</v>
       </c>
       <c r="BX2" t="n">
-        <v>1.081346629729683e-166</v>
+        <v>7.989739228612226e-182</v>
       </c>
       <c r="BY2" t="n">
-        <v>5.338058331901286e-169</v>
+        <v>3.594978533699011e-185</v>
       </c>
       <c r="BZ2" t="n">
-        <v>3.836103278033798e-172</v>
+        <v>1.692413185675818e-188</v>
       </c>
       <c r="CA2" t="n">
-        <v>3.257102598085161e-175</v>
+        <v>5.43685201851316e-192</v>
       </c>
       <c r="CB2" t="n">
-        <v>3.226390391699587e-178</v>
+        <v>3.845942230952949e-195</v>
       </c>
       <c r="CC2" t="n">
-        <v>1.707408672471369e-181</v>
+        <v>3.964076546956254e-198</v>
       </c>
       <c r="CD2" t="n">
-        <v>1.815419688673355e-184</v>
+        <v>3.904721793930747e-201</v>
       </c>
       <c r="CE2" t="n">
-        <v>1.01908897445214e-187</v>
+        <v>2.766966335782504e-204</v>
       </c>
       <c r="CF2" t="n">
-        <v>1.863620545547416e-190</v>
+        <v>9.718321290696634e-208</v>
       </c>
       <c r="CG2" t="n">
-        <v>2.813623098474391e-193</v>
+        <v>6.917844298617122e-211</v>
       </c>
       <c r="CH2" t="n">
-        <v>2.116979634197807e-196</v>
+        <v>1.212888493749262e-213</v>
       </c>
       <c r="CI2" t="n">
-        <v>7.053179952833195e-199</v>
+        <v>1.312047036212104e-216</v>
       </c>
       <c r="CJ2" t="n">
-        <v>3.929498916229202e-202</v>
+        <v>2.90540909733428e-219</v>
       </c>
       <c r="CK2" t="n">
-        <v>2.603176647103759e-205</v>
+        <v>1.968596833920156e-222</v>
       </c>
       <c r="CL2" t="n">
-        <v>1.301990339927298e-208</v>
+        <v>5.366481616340782e-225</v>
       </c>
       <c r="CM2" t="n">
-        <v>1.658665367937752e-211</v>
+        <v>3.210182005639906e-228</v>
       </c>
       <c r="CN2" t="n">
-        <v>8.140519286288745e-215</v>
+        <v>1.746645433885775e-231</v>
       </c>
       <c r="CO2" t="n">
-        <v>9.785552576279905e-218</v>
+        <v>1.467446656793903e-234</v>
       </c>
       <c r="CP2" t="n">
-        <v>5.919914396442165e-221</v>
+        <v>8.415444671432234e-237</v>
       </c>
       <c r="CQ2" t="n">
-        <v>6.846945039402231e-224</v>
+        <v>3.637832805227105e-238</v>
       </c>
       <c r="CR2" t="n">
-        <v>2.186941480778297e-226</v>
+        <v>3.803056450464288e-239</v>
       </c>
       <c r="CS2" t="n">
-        <v>3.840710551036565e-229</v>
+        <v>1.468717755692397e-242</v>
       </c>
       <c r="CT2" t="n">
-        <v>3.130977508039419e-232</v>
+        <v>6.128650371826036e-246</v>
       </c>
       <c r="CU2" t="n">
-        <v>2.482224887845293e-235</v>
+        <v>6.726203095961811e-249</v>
       </c>
       <c r="CV2" t="n">
-        <v>1.637702569899997e-238</v>
+        <v>2.219266172581739e-252</v>
       </c>
       <c r="CW2" t="n">
-        <v>7.871536317585233e-242</v>
+        <v>1.082195923138427e-255</v>
       </c>
       <c r="CX2" t="n">
-        <v>2.790542267515406e-245</v>
+        <v>6.476974777478503e-259</v>
       </c>
       <c r="CY2" t="n">
-        <v>2.65793700460113e-248</v>
+        <v>5.477473564946099e-262</v>
       </c>
       <c r="CZ2" t="n">
-        <v>3.640543035864978e-251</v>
+        <v>3.526680006020289e-265</v>
       </c>
       <c r="DA2" t="n">
-        <v>1.554454044193339e-254</v>
+        <v>1.338321049337788e-268</v>
       </c>
       <c r="DB2" t="n">
-        <v>1.540910946095008e-257</v>
+        <v>9.319933766661828e-272</v>
       </c>
       <c r="DC2" t="n">
-        <v>8.810107713942819e-261</v>
+        <v>1.337685115890873e-274</v>
       </c>
       <c r="DD2" t="n">
-        <v>3.165857263099195e-264</v>
+        <v>1.552788148718383e-277</v>
       </c>
       <c r="DE2" t="n">
-        <v>1.565753511107612e-266</v>
+        <v>2.181374177333988e-280</v>
       </c>
       <c r="DF2" t="n">
-        <v>8.163079918199396e-270</v>
+        <v>4.306268033925935e-283</v>
       </c>
       <c r="DG2" t="n">
-        <v>6.096789591502077e-273</v>
+        <v>2.425315793171477e-286</v>
       </c>
       <c r="DH2" t="n">
-        <v>2.242494647074508e-276</v>
+        <v>1.527441473409627e-289</v>
       </c>
       <c r="DI2" t="n">
-        <v>8.677582329531957e-280</v>
+        <v>5.789652549523663e-293</v>
       </c>
       <c r="DJ2" t="n">
-        <v>1.116021504607511e-282</v>
+        <v>1.907741476306189e-296</v>
       </c>
       <c r="DK2" t="n">
-        <v>5.620643995871633e-286</v>
+        <v>8.828294257763906e-300</v>
       </c>
       <c r="DL2" t="n">
-        <v>3.592899091022959e-289</v>
+        <v>6.43162797794563e-303</v>
       </c>
       <c r="DM2" t="n">
-        <v>1.643502448194804e-292</v>
+        <v>0</v>
       </c>
       <c r="DN2" t="n">
-        <v>6.820462331047236e-296</v>
+        <v>0</v>
       </c>
       <c r="DO2" t="n">
-        <v>4.170584735531864e-299</v>
+        <v>0</v>
       </c>
       <c r="DP2" t="n">
-        <v>2.365164541023265e-302</v>
+        <v>0</v>
       </c>
       <c r="DQ2" t="n">
-        <v>1.90366187513251e-305</v>
+        <v>0</v>
       </c>
       <c r="DR2" t="n">
         <v>0</v>
@@ -15538,412 +15538,412 @@
         <v>0.33</v>
       </c>
       <c r="C3" t="n">
-        <v>0.327885617810503</v>
+        <v>0.3350218769697578</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3458002504664768</v>
+        <v>0.3032870103500024</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3943551133879112</v>
+        <v>0.1911758966261369</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4879872348472923</v>
+        <v>0.1325395965273276</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4054012763950544</v>
+        <v>0.05887004172015317</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4788562394286533</v>
+        <v>0.01436961132929153</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7759229425904722</v>
+        <v>0.003422905849885958</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9224705375289627</v>
+        <v>0.003565308416825071</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7651473950505274</v>
+        <v>0.0006023380346275528</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9512635316275361</v>
+        <v>8.748959792452005e-05</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5764633518958928</v>
+        <v>5.671979416800272e-06</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2107593778305738</v>
+        <v>1.6685548480358e-06</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03647887357944728</v>
+        <v>2.218599794074805e-07</v>
       </c>
       <c r="P3" t="n">
-        <v>0.001932275650069587</v>
+        <v>1.383528722870443e-08</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0005768907031645145</v>
+        <v>1.029273569357486e-09</v>
       </c>
       <c r="R3" t="n">
-        <v>3.714842216578469e-05</v>
+        <v>3.500472413053997e-11</v>
       </c>
       <c r="S3" t="n">
-        <v>9.471834488651051e-07</v>
+        <v>1.735133079045604e-12</v>
       </c>
       <c r="T3" t="n">
-        <v>1.273634333432807e-06</v>
+        <v>1.499730538743105e-14</v>
       </c>
       <c r="U3" t="n">
-        <v>1.149633499378786e-07</v>
+        <v>6.415933359028328e-16</v>
       </c>
       <c r="V3" t="n">
-        <v>2.820399734832495e-09</v>
+        <v>7.802456796170959e-18</v>
       </c>
       <c r="W3" t="n">
-        <v>7.642131975303347e-11</v>
+        <v>3.782420741303013e-20</v>
       </c>
       <c r="X3" t="n">
-        <v>2.104358706579529e-12</v>
+        <v>5.575890538085173e-21</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.727292673673261e-12</v>
+        <v>2.884249862406355e-21</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.408484368714808e-14</v>
+        <v>1.667065014344743e-22</v>
       </c>
       <c r="AA3" t="n">
-        <v>5.093587894881834e-17</v>
+        <v>2.189050709091671e-25</v>
       </c>
       <c r="AB3" t="n">
-        <v>7.241056667325636e-19</v>
+        <v>1.11233652052827e-27</v>
       </c>
       <c r="AC3" t="n">
-        <v>3.050211930372963e-21</v>
+        <v>1.140682754598053e-29</v>
       </c>
       <c r="AD3" t="n">
-        <v>1.455047688322969e-23</v>
+        <v>4.091027726428458e-32</v>
       </c>
       <c r="AE3" t="n">
-        <v>5.04629933536169e-26</v>
+        <v>8.418108140574581e-34</v>
       </c>
       <c r="AF3" t="n">
-        <v>4.62587951838205e-28</v>
+        <v>1.540216734626991e-35</v>
       </c>
       <c r="AG3" t="n">
-        <v>1.022223026860448e-30</v>
+        <v>7.596781964264094e-38</v>
       </c>
       <c r="AH3" t="n">
-        <v>2.642552184227002e-32</v>
+        <v>2.333232009214209e-40</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.874202076120459e-34</v>
+        <v>2.099585043266254e-43</v>
       </c>
       <c r="AJ3" t="n">
-        <v>4.155732664602428e-36</v>
+        <v>5.100900284233442e-46</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.561658766739161e-37</v>
+        <v>8.812180536363671e-48</v>
       </c>
       <c r="AL3" t="n">
-        <v>2.512874271080311e-39</v>
+        <v>8.908960180646753e-51</v>
       </c>
       <c r="AM3" t="n">
-        <v>2.896731972549231e-40</v>
+        <v>1.695306484811273e-52</v>
       </c>
       <c r="AN3" t="n">
-        <v>1.262347485932166e-41</v>
+        <v>3.925042978942907e-54</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.250024146394366e-44</v>
+        <v>8.257382049240504e-56</v>
       </c>
       <c r="AP3" t="n">
-        <v>6.967764782884355e-47</v>
+        <v>2.617019018728566e-58</v>
       </c>
       <c r="AQ3" t="n">
-        <v>3.260522242269303e-49</v>
+        <v>7.477166594974172e-61</v>
       </c>
       <c r="AR3" t="n">
-        <v>9.968335997779824e-52</v>
+        <v>2.62313755857875e-63</v>
       </c>
       <c r="AS3" t="n">
-        <v>1.386354779577383e-53</v>
+        <v>1.913263407744964e-65</v>
       </c>
       <c r="AT3" t="n">
-        <v>4.166500261990701e-56</v>
+        <v>6.111139009441882e-68</v>
       </c>
       <c r="AU3" t="n">
-        <v>2.213530396767181e-58</v>
+        <v>1.476847774579703e-69</v>
       </c>
       <c r="AV3" t="n">
-        <v>3.164455967328136e-60</v>
+        <v>5.04510284041744e-73</v>
       </c>
       <c r="AW3" t="n">
-        <v>1.492192806128458e-62</v>
+        <v>4.432386715180571e-76</v>
       </c>
       <c r="AX3" t="n">
-        <v>3.589068792283606e-64</v>
+        <v>8.017112344037956e-78</v>
       </c>
       <c r="AY3" t="n">
-        <v>2.838745642468455e-66</v>
+        <v>2.204131107276549e-80</v>
       </c>
       <c r="AZ3" t="n">
-        <v>1.381983135000831e-68</v>
+        <v>4.880958812616704e-83</v>
       </c>
       <c r="BA3" t="n">
-        <v>5.947784668326823e-71</v>
+        <v>9.105924576832689e-86</v>
       </c>
       <c r="BB3" t="n">
-        <v>3.040158183515843e-73</v>
+        <v>2.476778621341535e-87</v>
       </c>
       <c r="BC3" t="n">
-        <v>9.714526167067421e-76</v>
+        <v>1.757241168539404e-89</v>
       </c>
       <c r="BD3" t="n">
-        <v>4.101422939817453e-78</v>
+        <v>4.476689721707815e-92</v>
       </c>
       <c r="BE3" t="n">
-        <v>5.589751911951992e-80</v>
+        <v>3.107229803788468e-95</v>
       </c>
       <c r="BF3" t="n">
-        <v>1.330972212830238e-82</v>
+        <v>3.157064471789808e-98</v>
       </c>
       <c r="BG3" t="n">
-        <v>8.739540937513761e-85</v>
+        <v>1.585246946723147e-101</v>
       </c>
       <c r="BH3" t="n">
-        <v>9.340904953684714e-88</v>
+        <v>1.485231532447764e-104</v>
       </c>
       <c r="BI3" t="n">
-        <v>2.926115986622179e-90</v>
+        <v>1.710842935234424e-107</v>
       </c>
       <c r="BJ3" t="n">
-        <v>9.453733803957785e-93</v>
+        <v>2.585255845260844e-110</v>
       </c>
       <c r="BK3" t="n">
-        <v>1.079752372214212e-95</v>
+        <v>5.167109411089019e-113</v>
       </c>
       <c r="BL3" t="n">
-        <v>1.436458932574614e-98</v>
+        <v>5.340723789829516e-116</v>
       </c>
       <c r="BM3" t="n">
-        <v>2.312324450868011e-101</v>
+        <v>3.441744573879464e-119</v>
       </c>
       <c r="BN3" t="n">
-        <v>4.244842804453696e-104</v>
+        <v>4.612584668238229e-122</v>
       </c>
       <c r="BO3" t="n">
-        <v>2.552804257962827e-107</v>
+        <v>9.54371195950204e-125</v>
       </c>
       <c r="BP3" t="n">
-        <v>1.126847367787014e-109</v>
+        <v>3.332729012448659e-127</v>
       </c>
       <c r="BQ3" t="n">
-        <v>2.135170669153582e-112</v>
+        <v>1.230365553688111e-129</v>
       </c>
       <c r="BR3" t="n">
-        <v>3.767122073078351e-115</v>
+        <v>4.175755391391657e-133</v>
       </c>
       <c r="BS3" t="n">
-        <v>3.462138330252244e-118</v>
+        <v>8.784848700860875e-137</v>
       </c>
       <c r="BT3" t="n">
-        <v>3.848376429545151e-120</v>
+        <v>4.764318651113657e-140</v>
       </c>
       <c r="BU3" t="n">
-        <v>4.79765545849335e-123</v>
+        <v>1.029229466341156e-142</v>
       </c>
       <c r="BV3" t="n">
-        <v>7.478996672163857e-126</v>
+        <v>8.062214003992389e-146</v>
       </c>
       <c r="BW3" t="n">
-        <v>9.029779768103169e-129</v>
+        <v>5.382838045803583e-148</v>
       </c>
       <c r="BX3" t="n">
-        <v>2.056374240318799e-131</v>
+        <v>5.842558035898871e-151</v>
       </c>
       <c r="BY3" t="n">
-        <v>2.777995902053298e-133</v>
+        <v>2.513246013589534e-154</v>
       </c>
       <c r="BZ3" t="n">
-        <v>3.786273938096904e-136</v>
+        <v>1.50755698019652e-157</v>
       </c>
       <c r="CA3" t="n">
-        <v>5.051707657754018e-139</v>
+        <v>2.595139209930919e-161</v>
       </c>
       <c r="CB3" t="n">
-        <v>1.441029475969088e-141</v>
+        <v>4.066495330535554e-164</v>
       </c>
       <c r="CC3" t="n">
-        <v>1.4038614206813e-144</v>
+        <v>6.976793940252256e-167</v>
       </c>
       <c r="CD3" t="n">
-        <v>3.984738495679102e-147</v>
+        <v>1.491500329787516e-169</v>
       </c>
       <c r="CE3" t="n">
-        <v>4.468732740168959e-150</v>
+        <v>1.969047971019873e-172</v>
       </c>
       <c r="CF3" t="n">
-        <v>1.99774951906154e-152</v>
+        <v>5.613018774002939e-176</v>
       </c>
       <c r="CG3" t="n">
-        <v>4.653758665410819e-155</v>
+        <v>3.820408173039742e-179</v>
       </c>
       <c r="CH3" t="n">
-        <v>9.039787283555511e-158</v>
+        <v>1.353138410154463e-181</v>
       </c>
       <c r="CI3" t="n">
-        <v>5.333598879923594e-160</v>
+        <v>2.344994285706655e-184</v>
       </c>
       <c r="CJ3" t="n">
-        <v>4.939022697982675e-163</v>
+        <v>1.70166155609836e-186</v>
       </c>
       <c r="CK3" t="n">
-        <v>6.778214529155929e-166</v>
+        <v>2.765877529966644e-189</v>
       </c>
       <c r="CL3" t="n">
-        <v>4.774917216055685e-169</v>
+        <v>2.179923262398447e-191</v>
       </c>
       <c r="CM3" t="n">
-        <v>1.43413373585458e-171</v>
+        <v>2.971493803521223e-194</v>
       </c>
       <c r="CN3" t="n">
-        <v>1.225914648365171e-174</v>
+        <v>2.032813824099344e-197</v>
       </c>
       <c r="CO3" t="n">
-        <v>1.890145219269872e-177</v>
+        <v>4.460350090617057e-200</v>
       </c>
       <c r="CP3" t="n">
-        <v>2.31182098991998e-180</v>
+        <v>9.069435262845212e-202</v>
       </c>
       <c r="CQ3" t="n">
-        <v>5.646705671398009e-183</v>
+        <v>2.075912049122082e-202</v>
       </c>
       <c r="CR3" t="n">
-        <v>5.101670836482347e-185</v>
+        <v>6.411721410531528e-203</v>
       </c>
       <c r="CS3" t="n">
-        <v>1.884876221552207e-187</v>
+        <v>3.385808969215521e-206</v>
       </c>
       <c r="CT3" t="n">
-        <v>4.180278647039086e-190</v>
+        <v>2.065580335729534e-209</v>
       </c>
       <c r="CU3" t="n">
-        <v>9.424519057921695e-193</v>
+        <v>5.430933594612317e-212</v>
       </c>
       <c r="CV3" t="n">
-        <v>1.383322170467666e-195</v>
+        <v>1.291641357218833e-215</v>
       </c>
       <c r="CW3" t="n">
-        <v>1.345119668521655e-198</v>
+        <v>1.237987976879164e-218</v>
       </c>
       <c r="CX3" t="n">
-        <v>4.521368669206971e-202</v>
+        <v>1.369416281474608e-221</v>
       </c>
       <c r="CY3" t="n">
-        <v>3.5531800540029e-205</v>
+        <v>2.940833686185743e-224</v>
       </c>
       <c r="CZ3" t="n">
-        <v>1.289594554821995e-207</v>
+        <v>4.654116248910678e-227</v>
       </c>
       <c r="DA3" t="n">
-        <v>1.039900790106077e-210</v>
+        <v>2.678913647238924e-230</v>
       </c>
       <c r="DB3" t="n">
-        <v>2.530147001790062e-213</v>
+        <v>5.091324953680711e-233</v>
       </c>
       <c r="DC3" t="n">
-        <v>3.408384417468145e-216</v>
+        <v>1.648709665084844e-235</v>
       </c>
       <c r="DD3" t="n">
-        <v>1.701200497943949e-219</v>
+        <v>6.203156590879761e-238</v>
       </c>
       <c r="DE3" t="n">
-        <v>1.24932966666873e-221</v>
+        <v>2.023834418247484e-240</v>
       </c>
       <c r="DF3" t="n">
-        <v>1.207556542009989e-224</v>
+        <v>8.384834960860981e-243</v>
       </c>
       <c r="DG3" t="n">
-        <v>2.559955232229153e-227</v>
+        <v>9.900040973311751e-246</v>
       </c>
       <c r="DH3" t="n">
-        <v>1.426099634350969e-230</v>
+        <v>1.603307264857988e-248</v>
       </c>
       <c r="DI3" t="n">
-        <v>9.477010047172382e-234</v>
+        <v>1.010933488951469e-251</v>
       </c>
       <c r="DJ3" t="n">
-        <v>2.83412232296621e-236</v>
+        <v>3.028848774079391e-255</v>
       </c>
       <c r="DK3" t="n">
-        <v>3.210673891341249e-239</v>
+        <v>3.08370631359843e-258</v>
       </c>
       <c r="DL3" t="n">
-        <v>3.256037517581492e-242</v>
+        <v>5.87038309837235e-261</v>
       </c>
       <c r="DM3" t="n">
-        <v>3.107744568394687e-245</v>
+        <v>9.591965161655266e-265</v>
       </c>
       <c r="DN3" t="n">
-        <v>2.195850694465593e-248</v>
+        <v>9.745790491724164e-268</v>
       </c>
       <c r="DO3" t="n">
-        <v>2.035930002781598e-251</v>
+        <v>4.121145692255298e-271</v>
       </c>
       <c r="DP3" t="n">
-        <v>2.352172562223392e-254</v>
+        <v>3.036267003362949e-274</v>
       </c>
       <c r="DQ3" t="n">
-        <v>2.910767654682732e-257</v>
+        <v>1.772446135072692e-276</v>
       </c>
       <c r="DR3" t="n">
-        <v>7.954766567232817e-260</v>
+        <v>1.679472583374582e-279</v>
       </c>
       <c r="DS3" t="n">
-        <v>6.957780778526225e-263</v>
+        <v>4.013966279681825e-284</v>
       </c>
       <c r="DT3" t="n">
-        <v>2.782687740704523e-265</v>
+        <v>2.016092624994513e-284</v>
       </c>
       <c r="DU3" t="n">
-        <v>1.51622362223081e-268</v>
+        <v>1.336548520551277e-286</v>
       </c>
       <c r="DV3" t="n">
-        <v>1.807987634949266e-271</v>
+        <v>7.384560157818079e-290</v>
       </c>
       <c r="DW3" t="n">
-        <v>2.802134179017095e-274</v>
+        <v>9.89906463557997e-294</v>
       </c>
       <c r="DX3" t="n">
-        <v>2.443605361180025e-277</v>
+        <v>1.634894950735166e-297</v>
       </c>
       <c r="DY3" t="n">
-        <v>9.089088334425414e-281</v>
+        <v>0</v>
       </c>
       <c r="DZ3" t="n">
-        <v>9.334295612432178e-284</v>
+        <v>0</v>
       </c>
       <c r="EA3" t="n">
-        <v>9.826180336094973e-287</v>
+        <v>0</v>
       </c>
       <c r="EB3" t="n">
-        <v>6.000493094402965e-290</v>
+        <v>0</v>
       </c>
       <c r="EC3" t="n">
-        <v>7.07106316874169e-293</v>
+        <v>0</v>
       </c>
       <c r="ED3" t="n">
-        <v>6.778437218129133e-296</v>
+        <v>0</v>
       </c>
       <c r="EE3" t="n">
-        <v>4.865557400667559e-298</v>
+        <v>0</v>
       </c>
       <c r="EF3" t="n">
-        <v>1.346603084280594e-300</v>
+        <v>0</v>
       </c>
       <c r="EG3" t="n">
-        <v>2.004704832119067e-303</v>
+        <v>0</v>
       </c>
       <c r="EH3" t="n">
-        <v>6.519348256947147e-307</v>
+        <v>0</v>
       </c>
       <c r="EI3" t="n">
         <v>0</v>
@@ -17045,76 +17045,76 @@
         <v>0.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3988854863901236</v>
+        <v>0.3603922035622612</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2971523707364307</v>
+        <v>0.5254874019576962</v>
       </c>
       <c r="E4" t="n">
-        <v>0.223667536864964</v>
+        <v>0.7769420315228167</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3165607704925325</v>
+        <v>0.8607159316163546</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5134734097175349</v>
+        <v>0.9402159790981524</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4949728596707051</v>
+        <v>0.9855895819543247</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1870706946332449</v>
+        <v>0.9965743946923332</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06784617356423693</v>
+        <v>0.9964341543005245</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2336835391870474</v>
+        <v>0.9993976503675454</v>
       </c>
       <c r="L4" t="n">
-        <v>0.04850225508655991</v>
+        <v>0.9999125098556306</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4235144842357362</v>
+        <v>0.9999943280171698</v>
       </c>
       <c r="N4" t="n">
-        <v>0.7892382168816392</v>
+        <v>0.9999983314449058</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9635210927636848</v>
+        <v>0.9999997781400123</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9980677240894021</v>
+        <v>0.9999999861647128</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9994231092883384</v>
+        <v>0.9999999989707264</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9999628515776791</v>
+        <v>0.9999999999649953</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9999990528165505</v>
+        <v>0.9999999999982649</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9999987263656666</v>
+        <v>0.999999999999985</v>
       </c>
       <c r="U4" t="n">
-        <v>0.99999988503665</v>
+        <v>0.9999999999999994</v>
       </c>
       <c r="V4" t="n">
-        <v>0.9999999971796002</v>
+        <v>1</v>
       </c>
       <c r="W4" t="n">
-        <v>0.9999999999235786</v>
+        <v>1</v>
       </c>
       <c r="X4" t="n">
-        <v>0.9999999999978956</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.9999999999972726</v>
+        <v>1</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.9999999999999758</v>
+        <v>1</v>
       </c>
       <c r="AA4" t="n">
         <v>1</v>

</xml_diff>